<commit_message>
ABC various changes, fix minimum stock
</commit_message>
<xml_diff>
--- a/comparison_result.xlsx
+++ b/comparison_result.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,7 +480,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>30.344,00</t>
+          <t>998,00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -493,30 +493,30 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>GHIACCIO ALIMENTARE TRITATO 2K</t>
+          <t>6 LEMON ICE LIQUIRIZIA LOVING 480G</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>GHIACCIO ALIMENTARE TRITATO 2K</t>
+          <t>6 LEMON ICE LIQUIRIZIA LOVING 480G</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>30.345,00</t>
+          <t>24.359,00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -525,11 +525,11 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>GHIACCIO ALIMENTARE CUBETTO 2K</t>
+          <t>8 GELATINI RICOPERTI CIOCC.240G</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -537,22 +537,22 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>GHIACCIO ALIMENTARE CUBETTO 2K</t>
+          <t>8 GELATINI RICOPERTI CIOCC.240G</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>24.403,00</t>
+          <t>997,00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -561,19 +561,19 @@
         </is>
       </c>
       <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>6 PRALINATI AMARENA LOVING 360G</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>2</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
+          <t>6 PRALINATI AMARENA LOVING 360G</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -605,7 +605,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -613,18 +613,18 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>997,00</t>
+          <t>24.403,00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -637,30 +637,30 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>6 PRALINATI AMARENA LOVING 360G</t>
+          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>6 PRALINATI AMARENA LOVING 360G</t>
+          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>998,00</t>
+          <t>9.053,00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -669,19 +669,19 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>6 LEMON ICE LIQUIRIZIA LOVING 500G</t>
+          <t>6 MINIBISCOTTI LOVING 325G</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>6 LEMON ICE LIQUIRIZIA LOVING 500G</t>
+          <t>6 MINIBISCOTTI LOVING 325G</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -696,7 +696,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>22.201,00</t>
+          <t>26.900,00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -709,7 +709,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SPAGHETTI ALLA CARBONARA  500G</t>
+          <t>6 BISCOTTI PANNA C/GOCCE CIOC.288G</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -717,7 +717,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>SPAGHETTI ALLA CARBONARA  500G</t>
+          <t>6 BISCOTTI PANNA C/GOCCE CIOC.288G</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -732,7 +732,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>11.129,00</t>
+          <t>1.374,00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -745,30 +745,30 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>MISTO SCOGLIO PESCARE' 300G</t>
+          <t>8 SANDWICH LOVING 400G</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>MISTO SCOGLIO PESCARE' 300G</t>
+          <t>8 SANDWICH LOVING 400G</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1.044,00</t>
+          <t>35.559,00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -777,19 +777,19 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>COZZE SGUSCIATE PESCARE'250G</t>
+          <t>6 CONI CAFFE' 450G</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>COZZE SGUSCIATE PESCARE'250G</t>
+          <t>6 CONI CAFFE' 450G</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -804,7 +804,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>595,00</t>
+          <t>32.499,00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -813,19 +813,19 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>GAMBERETTI SGUSCIATI 330/300G</t>
+          <t>6 CONI PANNA GR 450 LOVING ORO</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>GAMBERETTI SGUSCIATI 330/300G</t>
+          <t>6 CONI PANNA GR 450 LOVING ORO</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -840,7 +840,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>17.205,00</t>
+          <t>11.487,00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -853,35 +853,35 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>FILETTI DI BACCALA' GR 400</t>
+          <t>TARTUFO BIANCO LOVING  2X80G</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>FILETTI DI BACCALA' GR 400</t>
+          <t>TARTUFO BIANCO LOVING  2X80G</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>24.442,00</t>
+          <t>18.294,00</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -889,35 +889,35 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>MEDAGLIONI DI SALMONE 2X80G</t>
+          <t>TORTA GELATO S.HONORE'12/14PORZ 1KG</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>MEDAGLIONI DI SALMONE 2X80G</t>
+          <t>TORTA GELATO S.HONORE'12/14PORZ 1KG</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>25.872,00</t>
+          <t>18.295,00</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -925,35 +925,35 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>GRANFRITTO DI MARE 300G</t>
+          <t>TRANCIO VAR AMARENA 8/10 PORZ. 700G</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>GRANFRITTO DI MARE 300G</t>
+          <t>TRANCIO VAR AMARENA 8/10 PORZ. 700G</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>609,00</t>
+          <t>602,00</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -961,51 +961,51 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>BASTONCINI DI MERLUZZO 900G</t>
+          <t>VASCHETTA VANIGLIA CACAO NOCC.1KG</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>BASTONCINI DI MERLUZZO 900G</t>
+          <t>VASCHETTA VANIGLIA CACAO NOCC.1KG</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>25.438,00</t>
+          <t>18.269,00</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>TRANCIO MARGHERITA 3PZ X 400G</t>
+          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>TRANCIO MARGHERITA 3PZ X 400G</t>
+          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
         </is>
       </c>
       <c r="G16" t="n">
@@ -1020,20 +1020,20 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>35.599,00</t>
+          <t>18.269,00</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>PIZZA PROSCIUTTO/FUNGHI 26X38 570G</t>
+          <t>VASCHETTA ZUPPA INGLESE 1KG</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -1041,27 +1041,27 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>PIZZA PROSCIUTTO/FUNGHI 26X38 570G</t>
+          <t>VASCHETTA ZUPPA INGLESE 1KG</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>29.386,00</t>
+          <t>18.268,00</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -1069,30 +1069,30 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>PIZZA MARGHERITA 26X38 485G</t>
+          <t>VASCHETTA YOGURT FRUTTI BOSCO 500G</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>PIZZA MARGHERITA 26X38 485G</t>
+          <t>VASCHETTA YOGURT FRUTTI BOSCO 500G</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2.359,00</t>
+          <t>1.375,00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1101,11 +1101,11 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>PIZZA MARGHERITA CUCINO IO 3PZ 960G</t>
+          <t>VASCH.PANNA LOVING 500G</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -1113,27 +1113,27 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>PIZZA MARGHERITA CUCINO IO 3PZ 960G</t>
+          <t>VASCH.PANNA LOVING 500G</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>17.607,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>PATATE PREFRITTE 2,5KG</t>
+          <t>VASCHETTA SPAGNOLA LOVING 200G</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>PATATE PREFRITTE 2,5KG</t>
+          <t>VASCHETTA SPAGNOLA LOVING 200G</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -1164,12 +1164,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>603,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>PATATE PREFRITTE STICK 1KG</t>
+          <t>VASCHETTA CAFFE'ARABICA LOVING 200G</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1185,7 +1185,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>PATATE PREFRITTE STICK 1KG</t>
+          <t>VASCHETTA CAFFE'ARABICA LOVING 200G</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1200,20 +1200,20 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1.515,00</t>
+          <t>27.488,00</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>BIETA IN FOGLIA PORZIONATA 1KG</t>
+          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1221,22 +1221,22 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>BIETA IN FOGLIA PORZIONATA 1KG</t>
+          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>606,00</t>
+          <t>602,00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1245,34 +1245,34 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>SPINACI IN FOGLIA PORZIONATI 1KG</t>
+          <t>VASCHETTA FRAGOLA LIMONE PESCA 1KG</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>SPINACI IN FOGLIA PORZIONATI 1KG</t>
+          <t>VASCHETTA FRAGOLA LIMONE PESCA 1KG</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>12.682,00</t>
+          <t>36.839,00</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>CICORIA FOGLIA X FOGLIA 450G</t>
+          <t>VELLUTATA DI ZUCCA E CAROTA 600G</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>CICORIA FOGLIA X FOGLIA 450G</t>
+          <t>VELLUTATA DI ZUCCA E CAROTA 600G</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -1308,7 +1308,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>9.299,00</t>
+          <t>27.610,00</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1321,35 +1321,35 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>VERDURE PER SOFFRITTO 150G</t>
+          <t>PISELLI FINISSIMI 1KG</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>VERDURE PER SOFFRITTO 150G</t>
+          <t>PISELLI FINISSIMI 1KG</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>27.609,00</t>
+          <t>4.550,00</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>VERDURE PER SOFFRITTO 450G</t>
+          <t>PISELLI FINISSIMI BUSTA 450G</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1365,7 +1365,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>VERDURE PER SOFFRITTO 450G</t>
+          <t>PISELLI FINISSIMI BUSTA 450G</t>
         </is>
       </c>
       <c r="G26" t="n">
@@ -1389,7 +1389,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1397,7 +1397,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1416,7 +1416,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>765,00</t>
+          <t>27.609,00</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1425,11 +1425,11 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>FAGIOLINI INTERI FINISSIMI 1KG</t>
+          <t>VERDURE PER SOFFRITTO 450G</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -1437,22 +1437,22 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>FAGIOLINI INTERI FINISSIMI 1KG</t>
+          <t>VERDURE PER SOFFRITTO 450G</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>10.562,00</t>
+          <t>22.587,00</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>ZUCCHINE A CUBETTI 450G</t>
+          <t>BROCCOLI A ROSETTE BONTA'ORTO 600G</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1473,7 +1473,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>ZUCCHINE A CUBETTI 450G</t>
+          <t>BROCCOLI A ROSETTE BONTA'ORTO 600G</t>
         </is>
       </c>
       <c r="G29" t="n">
@@ -1488,7 +1488,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>36.839,00</t>
+          <t>8.399,00</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>VELLUTATA DI ZUCCA E CAROTA 600G</t>
+          <t>ERBETTE DI CAMPO CUBETTI 450G</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1509,7 +1509,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>VELLUTATA DI ZUCCA E CAROTA 600G</t>
+          <t>ERBETTE DI CAMPO CUBETTI 450G</t>
         </is>
       </c>
       <c r="G30" t="n">
@@ -1524,7 +1524,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>22.706,00</t>
+          <t>12.683,00</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1537,7 +1537,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>MINESTRONE LEGGERO BONTA'ORTO 750G</t>
+          <t>BIETA FOGLIA X FOGLIA 450G</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1545,7 +1545,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>MINESTRONE LEGGERO BONTA'ORTO 750G</t>
+          <t>BIETA FOGLIA X FOGLIA 450G</t>
         </is>
       </c>
       <c r="G31" t="n">
@@ -1560,12 +1560,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>36.102,00</t>
+          <t>8.490,00</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1573,71 +1573,71 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>GELATO SOIA FRUTTI ROSSI LOV.250G</t>
+          <t>SPINACI FOGLIA PER FOGLIA 450G</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>GELATO SOIA FRUTTI ROSSI LOV.250G</t>
+          <t>SPINACI FOGLIA PER FOGLIA 450G</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>27.488,00</t>
+          <t>606,00</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
+          <t>SPINACI IN FOGLIA PORZIONATI 1KG</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
+          <t>SPINACI IN FOGLIA PORZIONATI 1KG</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>18.268,00</t>
+          <t>610,00</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1645,7 +1645,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>VASCHETTA AFFOG. AL CACAO 500G</t>
+          <t>CUORI DI CARCIOFO INTERI 450G</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1653,7 +1653,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>VASCHETTA AFFOG. AL CACAO 500G</t>
+          <t>CUORI DI CARCIOFO INTERI 450G</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -1668,12 +1668,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>18.268,00</t>
+          <t>1.515,00</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>VASCHETTA AFFOG. CAFFE' 500G</t>
+          <t>BIETA IN FOGLIA PORZIONATA 1KG</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1689,7 +1689,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>VASCHETTA AFFOG. CAFFE' 500G</t>
+          <t>BIETA IN FOGLIA PORZIONATA 1KG</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -1704,12 +1704,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>18.268,00</t>
+          <t>25.793,00</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1717,43 +1717,43 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>VASCHETTA YOGURT FRUTTI BOSCO 500G</t>
+          <t>PATATE SPICCHI CON BUCCIA 600G</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>VASCHETTA YOGURT FRUTTI BOSCO 500G</t>
+          <t>PATATE SPICCHI CON BUCCIA 600G</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>18.268,00</t>
+          <t>603,00</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>VASCHETTA SPAGNOLA 500G</t>
+          <t>PATATE PREFRITTE STICK 1KG</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -1761,43 +1761,43 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>VASCHETTA SPAGNOLA 500G</t>
+          <t>PATATE PREFRITTE STICK 1KG</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1.375,00</t>
+          <t>18.048,00</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>VASCH.STRACCIATELLA LOVING 500G</t>
+          <t>PIZZA TONNO CIPOLLA CUCINO IO 390G</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>VASCH.STRACCIATELLA LOVING 500G</t>
+          <t>PIZZA TONNO CIPOLLA CUCINO IO 390G</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -1812,7 +1812,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1.375,00</t>
+          <t>23.988,00</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1821,11 +1821,11 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>VASCH.PANNA LOVING 500G</t>
+          <t>MIX DI MINI ARANCINI 300G</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -1833,35 +1833,35 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>VASCH.PANNA LOVING 500G</t>
+          <t>MIX DI MINI ARANCINI 300G</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>18.269,00</t>
+          <t>20.429,00</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
+          <t>FIORI DI ZUCCA IN PASTELLA 300G</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1869,35 +1869,35 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
+          <t>FIORI DI ZUCCA IN PASTELLA 300G</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>18.269,00</t>
+          <t>28.897,00</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>VASCHETTA ZUPPA INGLESE 1KG</t>
+          <t>PANCIOTTELLI PROSC.FORMAGGIO 250G</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1905,11 +1905,11 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>VASCHETTA ZUPPA INGLESE 1KG</t>
+          <t>PANCIOTTELLI PROSC.FORMAGGIO 250G</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
@@ -1920,430 +1920,34 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>602,00</t>
+          <t>9.341,00</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>VASCHETTA VANIGLIA CACAO NOCC.1KG</t>
+          <t>LINGUINE ALLO SCOGLIO  550G</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>VASCHETTA VANIGLIA CACAO NOCC.1KG</t>
+          <t>LINGUINE ALLO SCOGLIO  550G</t>
         </is>
       </c>
       <c r="G42" t="n">
         <v>0</v>
       </c>
       <c r="H42" t="inlineStr">
-        <is>
-          <t>Same</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>18.294,00</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C43" t="n">
-        <v>4</v>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>TORTA GELATO S.HONORE'12/14PORZ 1KG</t>
-        </is>
-      </c>
-      <c r="E43" t="n">
-        <v>6</v>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>TORTA GELATO S.HONORE'12/14PORZ 1KG</t>
-        </is>
-      </c>
-      <c r="G43" t="n">
-        <v>2</v>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>Increase</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>18.295,00</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C44" t="n">
-        <v>1</v>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>TRANCIO GRAN FRUTTA 8/10 PORZ. 700G</t>
-        </is>
-      </c>
-      <c r="E44" t="n">
-        <v>2</v>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>TRANCIO GRAN FRUTTA 8/10 PORZ. 700G</t>
-        </is>
-      </c>
-      <c r="G44" t="n">
-        <v>1</v>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>Increase</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>18.295,00</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="C45" t="n">
-        <v>1</v>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>TRANCIO VAR AMARENA 8/10 PORZ. 700G</t>
-        </is>
-      </c>
-      <c r="E45" t="n">
-        <v>2</v>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>TRANCIO VAR AMARENA 8/10 PORZ. 700G</t>
-        </is>
-      </c>
-      <c r="G45" t="n">
-        <v>1</v>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>Increase</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>9.051,00</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="C46" t="n">
-        <v>2</v>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>DESSERT VANIGLIA CACAO LOVING 320G</t>
-        </is>
-      </c>
-      <c r="E46" t="n">
-        <v>1</v>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>DESSERT VANIGLIA CACAO LOVING 320G</t>
-        </is>
-      </c>
-      <c r="G46" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>Decrease</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>11.487,00</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="C47" t="n">
-        <v>1</v>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>TARTUFO AL CIOCCOLATO LOVING 2X80G</t>
-        </is>
-      </c>
-      <c r="E47" t="n">
-        <v>2</v>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>TARTUFO AL CIOCCOLATO LOVING 2X80G</t>
-        </is>
-      </c>
-      <c r="G47" t="n">
-        <v>1</v>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>Increase</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>11.487,00</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C48" t="n">
-        <v>1</v>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>TARTUFO BIANCO LOVING  2X80G</t>
-        </is>
-      </c>
-      <c r="E48" t="n">
-        <v>2</v>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>TARTUFO BIANCO LOVING  2X80G</t>
-        </is>
-      </c>
-      <c r="G48" t="n">
-        <v>1</v>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>Increase</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>24.358,00</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C49" t="n">
-        <v>1</v>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>TORTA GELATO PANNA CIOCC. 450G LOV</t>
-        </is>
-      </c>
-      <c r="E49" t="n">
-        <v>1</v>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>TORTA GELATO PANNA CIOCC. 450G LOV</t>
-        </is>
-      </c>
-      <c r="G49" t="n">
-        <v>0</v>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>Same</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>26.007,00</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C50" t="n">
-        <v>2</v>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>SOUFFLE' DI CIOCCOLATO 2 X 100G</t>
-        </is>
-      </c>
-      <c r="E50" t="n">
-        <v>1</v>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>SOUFFLE' DI CIOCCOLATO 2 X 100G</t>
-        </is>
-      </c>
-      <c r="G50" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>Decrease</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>32.499,00</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C51" t="n">
-        <v>2</v>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>6 CONI PANNA GR 450 LOVING ORO</t>
-        </is>
-      </c>
-      <c r="E51" t="n">
-        <v>1</v>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>6 CONI PANNA GR 450 LOVING ORO</t>
-        </is>
-      </c>
-      <c r="G51" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>Decrease</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>12.166,00</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C52" t="n">
-        <v>1</v>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>12 MINIMINICONI LOVING 225G</t>
-        </is>
-      </c>
-      <c r="E52" t="n">
-        <v>2</v>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>12 MINIMINICONI LOVING 225G</t>
-        </is>
-      </c>
-      <c r="G52" t="n">
-        <v>1</v>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>Increase</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>9.053,00</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C53" t="n">
-        <v>2</v>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>6 MINIBISCOTTI LOVING 325G</t>
-        </is>
-      </c>
-      <c r="E53" t="n">
-        <v>2</v>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>6 MINIBISCOTTI LOVING 325G</t>
-        </is>
-      </c>
-      <c r="G53" t="n">
-        <v>0</v>
-      </c>
-      <c r="H53" t="inlineStr">
         <is>
           <t>Same</t>
         </is>
@@ -2360,7 +1964,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2393,7 +1997,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>21.820,00</t>
+          <t>15.757,00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -2403,19 +2007,19 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>BAGUETTE CLASSICA COTTA 260G</t>
+          <t>4 MAXISTECCHI LOVING 350G</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2.196,00</t>
+          <t>24.401,00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2430,14 +2034,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>8 MINISTECCHI ASSORT. LOVING 250G</t>
+          <t>4 COPPE AMARENA 350G LOVING</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>24.359,00</t>
+          <t>17.667,00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -2452,36 +2056,36 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>8 GELATINI RICOPERTI CIOCC.240G</t>
+          <t>GELATI DI SOIA ASSORTITI 360G</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>35.560,00</t>
+          <t>32.500,00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>2,00</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4 STECCHI PISTACCHIO CIOC/B.CO 260</t>
+          <t>6 CONI PANNA GR 420 LOVING</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>37.695,00</t>
+          <t>24.402,00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -2496,14 +2100,14 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>GHIACCIOLI ASS. MULTIVIT. 560G</t>
+          <t>6 CONI PANNA/CIOCCOLATO 450G LOVING</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>24.413,00</t>
+          <t>22.645,00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2513,24 +2117,24 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>20 GHIACCIOLI 1200G</t>
+          <t>12 MINI BON BON PANNA/CIOCC. 110G</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>35.510,00</t>
+          <t>9.051,00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2540,14 +2144,14 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>BURGER AGLI SPINACI 2X80 G</t>
+          <t>DESSERT VANIGLIA CACAO LOVING 320G</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>21.708,00</t>
+          <t>9.051,00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2562,14 +2166,14 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>GOCCE DI VERDURA 230G CUCINO IO</t>
+          <t>DESSERT CREMA CAFFE' LOVING 320G</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>25.696,00</t>
+          <t>1.443,00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2584,14 +2188,14 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>BURGER VEGETALE 2 X 75 GR CUCINO IO</t>
+          <t>STRUDEL DI MELE  500G</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>32.367,00</t>
+          <t>35.854,00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2606,41 +2210,41 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>NUGGETS DI POLLO 180G</t>
+          <t>NUTELLA CROISSANT 4X85G</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>26.468,00</t>
+          <t>602,00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>SPEEDY POLLO STICK ORIGINAL 300G</t>
+          <t>VASCHETTA CACAO STRACC.CAFFE' 1KG</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>14.306,00</t>
+          <t>1.375,00</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2650,14 +2254,14 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>GAMBERI ZUCCHINE C/POM.PESCARE'300G</t>
+          <t>VASCH.FRAGOLA/LIMONE LOVING 500G</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>33.193,00</t>
+          <t>27.488,00</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2672,14 +2276,14 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>FILETTI DI SALMONE SELVAGGIO 250G</t>
+          <t>GELATO ALLO YOGURT GRECO B.CO 320G</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>35.203,00</t>
+          <t>27.488,00</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -2694,19 +2298,19 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>TRANCE DI PESCE SPADA 450G</t>
+          <t>GELATO ALLO YOGURT GRECO B.CO 320G</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>11.179,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -2716,19 +2320,19 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>FILETTO DI PANGASIO  800G</t>
+          <t>VASCHETTA LIMONE SICILIA ADS 200G</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>32.476,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -2738,19 +2342,19 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>FILETTO DI MERLUZZO ATLANTICO 800G</t>
+          <t>VASCHETTA TRIPLO CIOCC.ADS 200G</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>12.208,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>9,00</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -2760,14 +2364,14 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>4 PORZIONI DI MERLUZZO PESCARE'400G</t>
+          <t>VASCHETTA PANNA COTTA ADS 200G</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>26.230,00</t>
+          <t>605,00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2782,19 +2386,19 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>ALICI DEL MEDITERRANEO PANATE 200G</t>
+          <t>MINESTRONE 15 VERDURE 1KG</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>31.078,00</t>
+          <t>36.839,00</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2804,14 +2408,14 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>FILETTO DI MERLUZZO CROCCANTE 400G</t>
+          <t>VELLUTATA DI VERDURE  600G</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>27.692,00</t>
+          <t>765,00</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2826,19 +2430,19 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>MIX SALATINI E PIZZETTE 400G</t>
+          <t>FAGIOLINI INTERI FINISSIMI 1KG</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>5.890,00</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2848,14 +2452,14 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI PROSC.FORMAGGIO 250G</t>
+          <t>FAGIOLI BORLOTTI 450G</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>25.619,00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2870,19 +2474,19 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI ALLA PIZZAIOLA 250G</t>
+          <t>FAVE SURGELATE 600G</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>31.404,00</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2892,14 +2496,14 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI FORMAGGIO MOZZAR.250G</t>
+          <t>BIETOLINE COLORATE IN FOGLIA 450G</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>15.758,00</t>
+          <t>1.083,00</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2914,14 +2518,14 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>BOCCONCINI MOZZARELLA PANATI 300G</t>
+          <t>CICORIA IN FOGLIA PORZIONATA 1KG</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>32.821,00</t>
+          <t>26.074,00</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2936,14 +2540,14 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>FRITTELLE ALGHE DI MARE 500G CUCINO</t>
+          <t>MISTO FUNGHI TRIFOLATI 300G</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4.138,00</t>
+          <t>593,00</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2958,14 +2562,14 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>CROCCHETTE DI PATATE  600G</t>
+          <t>MISTO FUNGHI 300G</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>26.942,00</t>
+          <t>35.773,00</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2980,14 +2584,14 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>CALZONE PROSCIUTTO COTTO 250G</t>
+          <t>PATATE A SPICCHI CON ROSMARINO 450G</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>26.186,00</t>
+          <t>18.022,00</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3002,14 +2606,14 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>PIZZA MARGHERITA S/GLUTINE 300G</t>
+          <t>PATATE A SPICCHIO PREFRITTE 1KG</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>35.621,00</t>
+          <t>21.820,00</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3019,19 +2623,19 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>PIZZA SALAMINO/PROVOLONE 26X38 535G</t>
+          <t>BAGUETTE CLASSICA COTTA 260G</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>18.046,00</t>
+          <t>21.822,00</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3046,14 +2650,14 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>PIZZA ALLA DIAVOLA CUCINO IO 315G</t>
+          <t>BAGUETTE 5 CEREALI COTTE 240G</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>26.868,00</t>
+          <t>21.823,00</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3068,14 +2672,14 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>PIZZETTE MARGHERITA 4X80G</t>
+          <t>BAGUETTINO 100% INTEGR. COTTO 130G</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>25.437,00</t>
+          <t>21.824,00</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3090,14 +2694,14 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>PIZZA MARGHERITA 300G</t>
+          <t>DEMI BAGUETTE CLASSICA COTTA 140G</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>15.706,00</t>
+          <t>22.255,00</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3112,7 +2716,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>TORTINO DI PATATE 300G</t>
+          <t>PATATE RUSTICHE PREFRITTE 1K</t>
         </is>
       </c>
     </row>
@@ -3141,7 +2745,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>24.797,00</t>
+          <t>17.607,00</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3156,14 +2760,14 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>PATATE A FETTE GR 600</t>
+          <t>PATATE PREFRITTE 2,5KG</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>35.774,00</t>
+          <t>2.359,00</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3173,19 +2777,19 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>PATATE A BARCHETTA 600G</t>
+          <t>PIZZA MARGHERITA CUCINO IO 3PZ 960G</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>17.518,00</t>
+          <t>26.868,00</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3200,14 +2804,14 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>MISTO BOSCO C/PORCINI GR 1000</t>
+          <t>PIZZETTE MARGHERITA 4X80G</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>20.874,00</t>
+          <t>28.897,00</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3217,24 +2821,24 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>FUNGHI CHAMPIGNON 100%ITALIANI 450G</t>
+          <t>PANCIOTTELLI ALLA PIZZAIOLA 250G</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>21.479,00</t>
+          <t>28.897,00</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -3244,14 +2848,14 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>ASPARAGI PUNTE ASTUCCIO 300G</t>
+          <t>PANCIOTTELLI FORMAGGIO MOZZAR.250G</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>33.967,00</t>
+          <t>31.078,00</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3266,14 +2870,14 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>CARCIOFI A SPICCHI 450G BONTA DEL</t>
+          <t>FILETTO DI MERLUZZO CROCCANTE 400G</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1.083,00</t>
+          <t>24.442,00</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3288,14 +2892,14 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>CICORIA IN FOGLIA PORZIONATA 1KG</t>
+          <t>MEDAGLIONI DI MERLUZZO 2X80G</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>8.490,00</t>
+          <t>27.552,00</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3310,14 +2914,14 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>SPINACI FOGLIA PER FOGLIA 450G</t>
+          <t>FILETTO DI PLATESSA IMPANATA 300G</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>29.360,00</t>
+          <t>12.208,00</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3327,41 +2931,41 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>MIX DI CAVOLI E BROCCOLI 450G</t>
+          <t>4 PORZIONI DI MERLUZZO PESCARE'400G</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>4.550,00</t>
+          <t>32.770,00</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>PISELLI FINISSIMI BUSTA 450G</t>
+          <t>CUORI DI FILETTO DI NASELLO 330G</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>27.610,00</t>
+          <t>17.271,00</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3371,19 +2975,19 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>PISELLI FINISSIMI 1KG</t>
+          <t>FILETTI DI MERLUZZO PESCARE' 600G</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>11.535,00</t>
+          <t>26.520,00</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3398,14 +3002,14 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>ZUPPA DI LEGUMI E CEREALI 450G</t>
+          <t>FILETTO DI SGOMBRO 600G</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>27.488,00</t>
+          <t>24.854,00</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -3420,19 +3024,19 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>GELATO ALLO YOGURT GRECO B.CO 320G</t>
+          <t>FILETTI DI TONNO PINNA GIALLA 225G</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>27.488,00</t>
+          <t>36.479,00</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -3442,19 +3046,19 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO C/NOCCIOLA 320G</t>
+          <t>CODE MAZZANCOLLE TROP.C/GUSC.350G</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>1.375,00</t>
+          <t>22.155,00</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -3464,19 +3068,19 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>VASCH.CREMA/CACAO LOVING 500G</t>
+          <t>VONGOLE C/GUSCIO DEL PACIFICO 500G</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>1.375,00</t>
+          <t>31.679,00</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -3486,41 +3090,41 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>VASCH.FRAGOLA/LIMONE LOVING 500G</t>
+          <t>CODE MAZZANC.SCOTTATE TROPICALI200G</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>602,00</t>
+          <t>1.044,00</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>VASCHETTA CACAO STRACC.CAFFE' 1KG</t>
+          <t>COZZE SGUSCIATE PESCARE'250G</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>602,00</t>
+          <t>12.654,00</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -3530,36 +3134,36 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>VASCHETTA FRAGOLA LIMONE PESCA 1KG</t>
+          <t>GRAN SUGO SCOGLIO C/POMOD.300G</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>35.854,00</t>
+          <t>12.654,00</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>NUTELLA CROISSANT 4X85G</t>
+          <t>GRAN SUGO ALLO SCOGLIO  300G</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>9.051,00</t>
+          <t>10.438,00</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -3574,14 +3178,14 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>DESSERT CREMA CAFFE' LOVING 320G</t>
+          <t>GNOCCHETTI ALLA SORRENTINA 550G</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>32.500,00</t>
+          <t>8.491,00</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -3591,19 +3195,19 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>6 CONI PANNA GR 420 LOVING</t>
+          <t>PISELLI PROSCIUTTO/FORMAGGIO 400G</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>24.402,00</t>
+          <t>35.510,00</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -3618,205 +3222,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>6 CONI PANNA/CIOCCOLATO 450G LOVING</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>35.559,00</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>6 CONI CAFFE' 450G</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>13.554,00</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>6 GRANCONO MIX LOVING 450G</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>30.760,00</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>4 CONI TWIRL PANNA/CIOCC. 280G</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>13.292,00</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>6 MAXISANDWICH LOVING  480G</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>11.190,00</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>6 COPPETTE PANNA/CIOCCOLATO 300G</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>33.310,00</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>4 BISCOTTI YOGURT GRECO 280G</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>26.900,00</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>6 BISCOTTI PANNA C/GOCCE CIOC.288G</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>2.193,00</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>4 COPPA AL CAFFE' LOVING 280G</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>24.401,00</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>4 COPPE AMARENA 350G LOVING</t>
+          <t>BURGER AGLI SPINACI 2X80 G</t>
         </is>
       </c>
     </row>
@@ -3831,7 +3237,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3864,7 +3270,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>605,00</t>
+          <t>14.470,00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -3879,14 +3285,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>MINESTRONE 15 VERDURE 1KG</t>
+          <t>MINESTRONE RICETTA GHIOTTA 750G</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18.022,00</t>
+          <t>12.682,00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3896,19 +3302,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PATATE A SPICCHIO PREFRITTE 1KG</t>
+          <t>CICORIA FOGLIA X FOGLIA 450G</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>25.793,00</t>
+          <t>766,00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3923,14 +3329,14 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>PATATE SPICCHI CON BUCCIA 600G</t>
+          <t>MELANZANE RONDELLE GRIGLIATE 450G</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>22.255,00</t>
+          <t>10.562,00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3945,14 +3351,14 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>PATATE RUSTICHE PREFRITTE 1K</t>
+          <t>ZUCCHINE A CUBETTI 450G</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>8.491,00</t>
+          <t>25.872,00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3967,14 +3373,14 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>PISELLI PROSCIUTTO/FORMAGGIO 400G</t>
+          <t>GRANFRITTO DI MARE 300G</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>610,00</t>
+          <t>36.806,00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3989,14 +3395,14 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CUORI DI CARCIOFO INTERI 450G</t>
+          <t>PERLE DI BACCALA'IN PASTELLA 200G</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>22.587,00</t>
+          <t>26.230,00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -4006,24 +3412,24 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>BROCCOLI A ROSETTE BONTA'ORTO 600G</t>
+          <t>ALICI DEL MEDITERRANEO PANATE 200G</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>18.556,00</t>
+          <t>28.897,00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -4033,36 +3439,36 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>PURE'DI PATATE 600G</t>
+          <t>PANCIOTTELLI AI FUNGHI 250G</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>8.399,00</t>
+          <t>28.897,00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ERBETTE DI CAMPO CUBETTI 450G</t>
+          <t>PANCIOTTELLI SPINACI/MOZZAR.250G</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2.154,00</t>
+          <t>9.336,00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -4077,14 +3483,14 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>FIL. DI PLATESSA PESCARE' 400G</t>
+          <t>RAVIOLI RICOTTA E SPINACI  550G</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>32.045,00</t>
+          <t>1.129,00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -4099,14 +3505,14 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>VONGOLE DEL PACIFICO C/GUSCIO 1K</t>
+          <t>8 MINICONO LOVING 320G</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>30.921,00</t>
+          <t>1.373,00</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -4121,14 +3527,14 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>PAELLA DI MARE 600G</t>
+          <t>8 RICOPERTI LOVING 400G</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>32.717,00</t>
+          <t>2.196,00</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -4138,19 +3544,19 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>FILETTO MERLUZZO ALLA SICILIANA 400</t>
+          <t>8 MINISTECCHI ASSORT. LOVING 250G</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>36.806,00</t>
+          <t>9.052,00</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -4165,14 +3571,14 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>PERLE DI BACCALA'IN PASTELLA 200G</t>
+          <t>6 RICOPERTI FRAGOLA LOVING 300G</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>27.818,00</t>
+          <t>11.190,00</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -4187,14 +3593,14 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>BISTECCHINE DI MARE 300G</t>
+          <t>6 COPPETTE PANNA/CIOCCOLATO 300G</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>24.166,00</t>
+          <t>12.166,00</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -4209,14 +3615,14 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>MIX 5 VERDURE PASTELLATE 300G</t>
+          <t>12 MINIMINICONI LOVING 225G</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>10.438,00</t>
+          <t>13.554,00</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -4231,36 +3637,36 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>GNOCCHETTI ALLA SORRENTINA 550G</t>
+          <t>6 GRANCONO MIX LOVING 450G</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>17.530,00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI SPINACI/MOZZAR.250G</t>
+          <t>6 BARRETTE GELATO PANNA E MOU 250G</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>9.337,00</t>
+          <t>22.646,00</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -4275,19 +3681,19 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>SAUTE' DI MARE ASTUCCIO  500G</t>
+          <t>6 BARRETTE AL COCCO 250G</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>9.339,00</t>
+          <t>24.402,00</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -4297,19 +3703,19 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>TAGLIATELLE AI FUNGHI  550G</t>
+          <t>6 CONI PANNA VAR.AMARENA 450G LOVIN</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>30.760,00</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -4319,19 +3725,19 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>VASCHETTA TRIPLO CIOCC.ADS 200G</t>
+          <t>4 CONI TWIRL PANNA/CIOCC. 280G</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>35.560,00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -4341,29 +3747,29 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>VASCHETTA PISTAC/GIANDUIA ADS 200G</t>
+          <t>4 STECCHI CARAM.SALATO E CIOCC 260G</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>2.193,00</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>9,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>VASCHETTA PANNA COTTA ADS 200G</t>
+          <t>4 COPPA AL CAFFE' LOVING 280G</t>
         </is>
       </c>
     </row>
@@ -4386,6 +3792,50 @@
       <c r="D25" t="inlineStr">
         <is>
           <t>VASCHETTA CARAMELLO SALATO ADS 200G</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>11.487,00</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>TARTUFO AL CIOCCOLATO LOVING 2X80G</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>18.295,00</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>TRANCIO GRAN FRUTTA 8/10 PORZ. 700G</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
New U processor, several changes to the other processors
</commit_message>
<xml_diff>
--- a/comparison_result.xlsx
+++ b/comparison_result.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,7 +480,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>998,00</t>
+          <t>24.413,00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -489,19 +489,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>6 LEMON ICE LIQUIRIZIA LOVING 480G</t>
+          <t>20 GHIACCIOLI 1200G</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>6 LEMON ICE LIQUIRIZIA LOVING 480G</t>
+          <t>20 GHIACCIOLI 1200G</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -516,7 +516,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>24.359,00</t>
+          <t>998,00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -529,30 +529,30 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>8 GELATINI RICOPERTI CIOCC.240G</t>
+          <t>6 LEMON ICE LIQUIRIZIA LOVING 480G</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>8 GELATINI RICOPERTI CIOCC.240G</t>
+          <t>6 LEMON ICE LIQUIRIZIA LOVING 480G</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>997,00</t>
+          <t>25.272,00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -565,7 +565,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>6 PRALINATI AMARENA LOVING 360G</t>
+          <t>10 GHIACCIOLI LOVING 750G</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -573,7 +573,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>6 PRALINATI AMARENA LOVING 360G</t>
+          <t>10 GHIACCIOLI LOVING 750G</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -588,7 +588,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>27.627,00</t>
+          <t>37.695,00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -601,30 +601,30 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>GELATO GRAN RIPIENO MIX 6PZ 360G</t>
+          <t>GHIACCIOLI ASS. MULTIVIT. 560G</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>GELATO GRAN RIPIENO MIX 6PZ 360G</t>
+          <t>GHIACCIOLI ASS. MULTIVIT. 560G</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>24.403,00</t>
+          <t>33.309,00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -633,34 +633,34 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
+          <t>CONI GRANITA LIMONE/ARANCIA 6X105G</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
+          <t>CONI GRANITA LIMONE/ARANCIA 6X105G</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>9.053,00</t>
+          <t>1.373,00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -669,11 +669,11 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>6 MINIBISCOTTI LOVING 325G</t>
+          <t>8 RICOPERTI LOVING 400G</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -681,22 +681,22 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>6 MINIBISCOTTI LOVING 325G</t>
+          <t>8 RICOPERTI LOVING 400G</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>26.900,00</t>
+          <t>27.627,00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -705,34 +705,34 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>6 BISCOTTI PANNA C/GOCCE CIOC.288G</t>
+          <t>GELATO GRAN RIPIENO MIX 6PZ 360G</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>6 BISCOTTI PANNA C/GOCCE CIOC.288G</t>
+          <t>GELATO GRAN RIPIENO MIX 6PZ 360G</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1.374,00</t>
+          <t>24.403,00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -745,7 +745,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>8 SANDWICH LOVING 400G</t>
+          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -753,7 +753,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>8 SANDWICH LOVING 400G</t>
+          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -768,7 +768,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>35.559,00</t>
+          <t>35.560,00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -777,11 +777,11 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>6 CONI CAFFE' 450G</t>
+          <t>4 STECCHI CARAM.SALATO E CIOCC 260G</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -789,22 +789,22 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>6 CONI CAFFE' 450G</t>
+          <t>4 STECCHI CARAM.SALATO E CIOCC 260G</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>32.499,00</t>
+          <t>22.646,00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -813,19 +813,19 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>6 CONI PANNA GR 450 LOVING ORO</t>
+          <t>6 BARRETTE AL COCCO 250G</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>6 CONI PANNA GR 450 LOVING ORO</t>
+          <t>6 BARRETTE AL COCCO 250G</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -840,7 +840,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>11.487,00</t>
+          <t>17.530,00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -853,7 +853,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>TARTUFO BIANCO LOVING  2X80G</t>
+          <t>6 BARRETTE GELATO PANNA E MOU 250G</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -861,7 +861,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>TARTUFO BIANCO LOVING  2X80G</t>
+          <t>6 BARRETTE GELATO PANNA E MOU 250G</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -876,7 +876,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>18.294,00</t>
+          <t>2.196,00</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -889,35 +889,35 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>TORTA GELATO S.HONORE'12/14PORZ 1KG</t>
+          <t>8 MINISTECCHI ASSORT. LOVING 250G</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>TORTA GELATO S.HONORE'12/14PORZ 1KG</t>
+          <t>8 MINISTECCHI ASSORT. LOVING 250G</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>18.295,00</t>
+          <t>13.292,00</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -925,19 +925,19 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>TRANCIO VAR AMARENA 8/10 PORZ. 700G</t>
+          <t>6 MAXISANDWICH LOVING  480G</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>TRANCIO VAR AMARENA 8/10 PORZ. 700G</t>
+          <t>6 MAXISANDWICH LOVING  480G</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -948,12 +948,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>602,00</t>
+          <t>1.374,00</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -961,43 +961,43 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>VASCHETTA VANIGLIA CACAO NOCC.1KG</t>
+          <t>8 SANDWICH LOVING 400G</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>VASCHETTA VANIGLIA CACAO NOCC.1KG</t>
+          <t>8 SANDWICH LOVING 400G</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>18.269,00</t>
+          <t>11.190,00</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
+          <t>6 COPPETTE PANNA/CIOCCOLATO 300G</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -1005,63 +1005,63 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
+          <t>6 COPPETTE PANNA/CIOCCOLATO 300G</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>18.269,00</t>
+          <t>1.129,00</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>8 MINICONO LOVING 320G</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
         <v>2</v>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>VASCHETTA ZUPPA INGLESE 1KG</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>1</v>
-      </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>VASCHETTA ZUPPA INGLESE 1KG</t>
+          <t>8 MINICONO LOVING 320G</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>18.268,00</t>
+          <t>35.947,00</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -1069,35 +1069,35 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>VASCHETTA YOGURT FRUTTI BOSCO 500G</t>
+          <t>CONI PANNA S/GLUTINE 4X75G</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>VASCHETTA YOGURT FRUTTI BOSCO 500G</t>
+          <t>CONI PANNA S/GLUTINE 4X75G</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1.375,00</t>
+          <t>24.402,00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -1105,7 +1105,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>VASCH.PANNA LOVING 500G</t>
+          <t>6 CONI PANNA VAR.AMARENA 450G LOVIN</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -1113,7 +1113,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>VASCH.PANNA LOVING 500G</t>
+          <t>6 CONI PANNA VAR.AMARENA 450G LOVIN</t>
         </is>
       </c>
       <c r="G19" t="n">
@@ -1128,28 +1128,28 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>13.554,00</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>VASCHETTA SPAGNOLA LOVING 200G</t>
+          <t>6 GRANCONO MIX LOVING 450G</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>VASCHETTA SPAGNOLA LOVING 200G</t>
+          <t>6 GRANCONO MIX LOVING 450G</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -1164,12 +1164,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>17.667,00</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>VASCHETTA CAFFE'ARABICA LOVING 200G</t>
+          <t>GELATI DI SOIA ASSORTITI 360G</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1185,7 +1185,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>VASCHETTA CAFFE'ARABICA LOVING 200G</t>
+          <t>GELATI DI SOIA ASSORTITI 360G</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1200,43 +1200,43 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>27.488,00</t>
+          <t>32.500,00</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
+          <t>6 CONI PANNA GR 420 LOVING</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
+          <t>6 CONI PANNA GR 420 LOVING</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>602,00</t>
+          <t>24.358,00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>VASCHETTA FRAGOLA LIMONE PESCA 1KG</t>
+          <t>TORTA GELATO PANNA CIOCC. 450G LOV</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>VASCHETTA FRAGOLA LIMONE PESCA 1KG</t>
+          <t>TORTA GELATO PANNA CIOCC. 450G LOV</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1272,7 +1272,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>36.839,00</t>
+          <t>18.294,00</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1281,47 +1281,47 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>VELLUTATA DI ZUCCA E CAROTA 600G</t>
+          <t>TORTA GELATO S.HONORE'12/14PORZ 1KG</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>VELLUTATA DI ZUCCA E CAROTA 600G</t>
+          <t>TORTA GELATO S.HONORE'12/14PORZ 1KG</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>27.610,00</t>
+          <t>602,00</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>PISELLI FINISSIMI 1KG</t>
+          <t>VASCHETTA CACAO STRACC.CAFFE' 1KG</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -1329,22 +1329,22 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>PISELLI FINISSIMI 1KG</t>
+          <t>VASCHETTA CACAO STRACC.CAFFE' 1KG</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4.550,00</t>
+          <t>602,00</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1357,35 +1357,35 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>PISELLI FINISSIMI BUSTA 450G</t>
+          <t>VASCHETTA VANIGLIA CACAO NOCC.1KG</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>PISELLI FINISSIMI BUSTA 450G</t>
+          <t>VASCHETTA VANIGLIA CACAO NOCC.1KG</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>604,00</t>
+          <t>18.269,00</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -1393,35 +1393,35 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>PISELLI FINI BUSTA 1KG</t>
+          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>PISELLI FINI BUSTA 1KG</t>
+          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>27.609,00</t>
+          <t>18.269,00</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1429,7 +1429,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>VERDURE PER SOFFRITTO 450G</t>
+          <t>VASCHETTA ZUPPA INGLESE 1KG</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -1437,7 +1437,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>VERDURE PER SOFFRITTO 450G</t>
+          <t>VASCHETTA ZUPPA INGLESE 1KG</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -1452,43 +1452,43 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>22.587,00</t>
+          <t>18.268,00</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>BROCCOLI A ROSETTE BONTA'ORTO 600G</t>
+          <t>VASCHETTA YOGURT FRUTTI BOSCO 500G</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>BROCCOLI A ROSETTE BONTA'ORTO 600G</t>
+          <t>VASCHETTA YOGURT FRUTTI BOSCO 500G</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>8.399,00</t>
+          <t>1.375,00</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1501,35 +1501,35 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>ERBETTE DI CAMPO CUBETTI 450G</t>
+          <t>VASCH.PANNA LOVING 500G</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>ERBETTE DI CAMPO CUBETTI 450G</t>
+          <t>VASCH.PANNA LOVING 500G</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>12.683,00</t>
+          <t>18.268,00</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1537,30 +1537,30 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>BIETA FOGLIA X FOGLIA 450G</t>
+          <t>VASCHETTA SPAGNOLA 500G</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>BIETA FOGLIA X FOGLIA 450G</t>
+          <t>VASCHETTA SPAGNOLA 500G</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>8.490,00</t>
+          <t>27.488,00</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1573,19 +1573,19 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>SPINACI FOGLIA PER FOGLIA 450G</t>
+          <t>GELATO ALLO YOGURT GRECO B.CO 320G</t>
         </is>
       </c>
       <c r="E32" t="n">
+        <v>3</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>GELATO ALLO YOGURT GRECO B.CO 320G</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
         <v>2</v>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>SPINACI FOGLIA PER FOGLIA 450G</t>
-        </is>
-      </c>
-      <c r="G32" t="n">
-        <v>1</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
@@ -1596,48 +1596,48 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>606,00</t>
+          <t>27.488,00</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>SPINACI IN FOGLIA PORZIONATI 1KG</t>
+          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>SPINACI IN FOGLIA PORZIONATI 1KG</t>
+          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>610,00</t>
+          <t>27.488,00</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1645,7 +1645,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>CUORI DI CARCIOFO INTERI 450G</t>
+          <t>GELATO YOGURT GRECO C/NOCCIOLA 320G</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1653,7 +1653,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>CUORI DI CARCIOFO INTERI 450G</t>
+          <t>GELATO YOGURT GRECO C/NOCCIOLA 320G</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -1668,12 +1668,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1.515,00</t>
+          <t>27.488,00</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>BIETA IN FOGLIA PORZIONATA 1KG</t>
+          <t>GELATO YOGURT GRECO AL MIELE 320G</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1689,7 +1689,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>BIETA IN FOGLIA PORZIONATA 1KG</t>
+          <t>GELATO YOGURT GRECO AL MIELE 320G</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -1704,12 +1704,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>25.793,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1717,7 +1717,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>PATATE SPICCHI CON BUCCIA 600G</t>
+          <t>VASCHETTA TRIPLO CIOCC.ADS 200G</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1725,7 +1725,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>PATATE SPICCHI CON BUCCIA 600G</t>
+          <t>VASCHETTA TRIPLO CIOCC.ADS 200G</t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -1740,12 +1740,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>603,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>11,00</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1753,30 +1753,30 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>PATATE PREFRITTE STICK 1KG</t>
+          <t>VASCHETTA CARAMELLO SALATO ADS 200G</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>PATATE PREFRITTE STICK 1KG</t>
+          <t>VASCHETTA CARAMELLO SALATO ADS 200G</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>18.048,00</t>
+          <t>2.627,00</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1789,7 +1789,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>PIZZA TONNO CIPOLLA CUCINO IO 390G</t>
+          <t>PREZZEMOLO TRITATO  50G</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1797,7 +1797,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>PIZZA TONNO CIPOLLA CUCINO IO 390G</t>
+          <t>PREZZEMOLO TRITATO  50G</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -1812,7 +1812,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>23.988,00</t>
+          <t>27.609,00</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1825,7 +1825,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>MIX DI MINI ARANCINI 300G</t>
+          <t>VERDURE PER SOFFRITTO 450G</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -1833,7 +1833,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>MIX DI MINI ARANCINI 300G</t>
+          <t>VERDURE PER SOFFRITTO 450G</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -1848,7 +1848,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>20.429,00</t>
+          <t>593,00</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>FIORI DI ZUCCA IN PASTELLA 300G</t>
+          <t>MISTO FUNGHI 300G</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1869,7 +1869,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>FIORI DI ZUCCA IN PASTELLA 300G</t>
+          <t>MISTO FUNGHI 300G</t>
         </is>
       </c>
       <c r="G40" t="n">
@@ -1884,20 +1884,20 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>18.022,00</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI PROSC.FORMAGGIO 250G</t>
+          <t>PATATE A SPICCHIO PREFRITTE 1KG</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1905,22 +1905,22 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI PROSC.FORMAGGIO 250G</t>
+          <t>PATATE A SPICCHIO PREFRITTE 1KG</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>9.341,00</t>
+          <t>603,00</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1933,7 +1933,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>LINGUINE ALLO SCOGLIO  550G</t>
+          <t>PATATE PREFRITTE STICK 1KG</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>LINGUINE ALLO SCOGLIO  550G</t>
+          <t>PATATE PREFRITTE STICK 1KG</t>
         </is>
       </c>
       <c r="G42" t="n">
@@ -1950,6 +1950,762 @@
       <c r="H42" t="inlineStr">
         <is>
           <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>17.607,00</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>PATATE PREFRITTE 2,5KG</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>2</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>PATATE PREFRITTE 2,5KG</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>1</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Increase</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2.359,00</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>PIZZA MARGHERITA CUCINO IO 3PZ 960G</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>1</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>PIZZA MARGHERITA CUCINO IO 3PZ 960G</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>25.437,00</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>PIZZA MARGHERITA 300G</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>1</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>PIZZA MARGHERITA 300G</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>26.868,00</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>PIZZETTE MARGHERITA 4X80G</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>1</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>PIZZETTE MARGHERITA 4X80G</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>24.166,00</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>MIX 5 VERDURE PASTELLATE 300G</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>1</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>MIX 5 VERDURE PASTELLATE 300G</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>12.735,00</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>OLIVE ALL'ASCOLANA PREFRITTE 500G</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>1</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>OLIVE ALL'ASCOLANA PREFRITTE 500G</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>28.897,00</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>PANCIOTTELLI ALLA PIZZAIOLA 250G</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>2</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>PANCIOTTELLI ALLA PIZZAIOLA 250G</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Increase</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>28.897,00</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>PANCIOTTELLI PROSC.FORMAGGIO 250G</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>1</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>PANCIOTTELLI PROSC.FORMAGGIO 250G</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>28.897,00</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>PANCIOTTELLI FORMAGGIO MOZZAR.250G</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>1</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>PANCIOTTELLI FORMAGGIO MOZZAR.250G</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>1.797,00</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>1</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>PINZE GRANCHIO PANATE S/GLUT.250G</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>1</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>PINZE GRANCHIO PANATE S/GLUT.250G</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>20.432,00</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>1</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>BAST.FILETTI MERLUZZO S/GLUTINE 300</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>1</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>BAST.FILETTI MERLUZZO S/GLUTINE 300</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>26.859,00</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>1</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>MINI TOAST PROSCIUT/MOZZAR. 180G</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>1</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>MINI TOAST PROSCIUT/MOZZAR. 180G</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>35.681,00</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>1</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>ANELLI CIUFFI CALAMARO PATAG. 400G</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>1</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>ANELLI CIUFFI CALAMARO PATAG. 400G</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>22.155,00</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>VONGOLE C/GUSCIO DEL PACIFICO 500G</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>1</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>VONGOLE C/GUSCIO DEL PACIFICO 500G</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>14.306,00</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>1</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>GAMBERI ZUCCHINE C/POM.PESCARE'300G</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>1</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>GAMBERI ZUCCHINE C/POM.PESCARE'300G</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>12.654,00</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>1</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>GRAN SUGO ALLO SCOGLIO  300G</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>1</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>GRAN SUGO ALLO SCOGLIO  300G</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>12.654,00</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>1</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>GRAN SUGO AI FRUTTI DI MARE  300G</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>1</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>GRAN SUGO AI FRUTTI DI MARE  300G</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>12.654,00</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>1</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>GRAN SUGO AI GAMBERI 250G</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>1</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>GRAN SUGO AI GAMBERI 250G</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>35.510,00</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>BURGER AGLI SPINACI 2X80 G</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>1</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>BURGER AGLI SPINACI 2X80 G</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>35.559,00</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>1</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>6 CONI CAFFE' 450G</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>2</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>6 CONI CAFFE' 450G</t>
+        </is>
+      </c>
+      <c r="G62" t="n">
+        <v>1</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Increase</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>9.053,00</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>1</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>6 MINIBISCOTTI LOVING 325G</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>2</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>6 MINIBISCOTTI LOVING 325G</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
+        <v>1</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>Increase</t>
         </is>
       </c>
     </row>
@@ -1964,7 +2720,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1997,7 +2753,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>15.757,00</t>
+          <t>11.189,00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -2007,19 +2763,19 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4 MAXISTECCHI LOVING 350G</t>
+          <t>6 STECCHI RICOPERTI CIOCC.300G</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>24.401,00</t>
+          <t>15.757,00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2034,14 +2790,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>4 COPPE AMARENA 350G LOVING</t>
+          <t>4 MAXISTECCHI LOVING 350G</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>17.667,00</t>
+          <t>30.345,00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -2051,19 +2807,19 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>GELATI DI SOIA ASSORTITI 360G</t>
+          <t>GHIACCIO ALIMENTARE CUBETTO 2K</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>32.500,00</t>
+          <t>24.401,00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -2078,7 +2834,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>6 CONI PANNA GR 420 LOVING</t>
+          <t>4 COPPE AMARENA 350G LOVING</t>
         </is>
       </c>
     </row>
@@ -2095,7 +2851,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2107,7 +2863,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>22.645,00</t>
+          <t>32.499,00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2117,12 +2873,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>12 MINI BON BON PANNA/CIOCC. 110G</t>
+          <t>6 CONI PANNA GR 450 LOVING ORO</t>
         </is>
       </c>
     </row>
@@ -2151,7 +2907,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>9.051,00</t>
+          <t>22.076,00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2166,19 +2922,19 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>DESSERT CREMA CAFFE' LOVING 320G</t>
+          <t>MISTO FRUTTI DI BOSCO 300G</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1.443,00</t>
+          <t>1.375,00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -2188,19 +2944,19 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>STRUDEL DI MELE  500G</t>
+          <t>VASCH.CREMA/CACAO LOVING 500G</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>35.854,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -2210,41 +2966,41 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>NUTELLA CROISSANT 4X85G</t>
+          <t>VASCHETTA LIMONE SICILIA ADS 200G</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>602,00</t>
+          <t>605,00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>VASCHETTA CACAO STRACC.CAFFE' 1KG</t>
+          <t>MINESTRONE 15 VERDURE 1KG</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1.375,00</t>
+          <t>31.628,00</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2254,14 +3010,14 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>VASCH.FRAGOLA/LIMONE LOVING 500G</t>
+          <t>ROSETTE DI BROCCOLO ROMANESCO 600G</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>27.488,00</t>
+          <t>22.587,00</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2276,14 +3032,14 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>GELATO ALLO YOGURT GRECO B.CO 320G</t>
+          <t>BROCCOLI A ROSETTE BONTA'ORTO 600G</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>27.488,00</t>
+          <t>8.399,00</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -2293,24 +3049,24 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>GELATO ALLO YOGURT GRECO B.CO 320G</t>
+          <t>ERBETTE DI CAMPO CUBETTI 450G</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>12.683,00</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -2320,19 +3076,19 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>VASCHETTA LIMONE SICILIA ADS 200G</t>
+          <t>BIETA FOGLIA X FOGLIA 450G</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>1.083,00</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -2342,19 +3098,19 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>VASCHETTA TRIPLO CIOCC.ADS 200G</t>
+          <t>CICORIA IN FOGLIA PORZIONATA 1KG</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>17.518,00</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>9,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -2364,14 +3120,14 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>VASCHETTA PANNA COTTA ADS 200G</t>
+          <t>MISTO BOSCO C/PORCINI GR 1000</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>605,00</t>
+          <t>24.797,00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2386,19 +3142,19 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>MINESTRONE 15 VERDURE 1KG</t>
+          <t>PATATE A FETTE GR 600</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>36.839,00</t>
+          <t>35.621,00</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2408,14 +3164,14 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>VELLUTATA DI VERDURE  600G</t>
+          <t>PIZZA SALAMINO/PROVOLONE 26X38 535G</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>765,00</t>
+          <t>29.386,00</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2430,14 +3186,14 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>FAGIOLINI INTERI FINISSIMI 1KG</t>
+          <t>PIZZA MARGHERITA 26X38 485G</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>5.890,00</t>
+          <t>26.186,00</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2452,14 +3208,14 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>FAGIOLI BORLOTTI 450G</t>
+          <t>PIZZA MARGHERITA S/GLUTINE 300G</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>25.619,00</t>
+          <t>37.651,00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2474,19 +3230,19 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>FAVE SURGELATE 600G</t>
+          <t>FOCACCIA FARCITA PROSC/FORM.330G</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>31.404,00</t>
+          <t>18.380,00</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2496,14 +3252,14 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>BIETOLINE COLORATE IN FOGLIA 450G</t>
+          <t>PIZZA VERD.GRIGLIATE TAGLIERE 235G</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1.083,00</t>
+          <t>9.376,00</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2518,14 +3274,14 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>CICORIA IN FOGLIA PORZIONATA 1KG</t>
+          <t>CROCCHETTE PATATE ALLA ROMANA 500G</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>26.074,00</t>
+          <t>4.138,00</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2540,14 +3296,14 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>MISTO FUNGHI TRIFOLATI 300G</t>
+          <t>CROCCHETTE DI PATATE  600G</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>593,00</t>
+          <t>1.500,00</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2562,14 +3318,14 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>MISTO FUNGHI 300G</t>
+          <t>SUPPLI'DI RISO AL RAGU'500G</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>35.773,00</t>
+          <t>13.597,00</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2584,19 +3340,19 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>PATATE A SPICCHI CON ROSMARINO 450G</t>
+          <t>MISTO OLIVE/CROCC/SUPPLI/ARANC 500G</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>18.022,00</t>
+          <t>28.897,00</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2606,14 +3362,14 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>PATATE A SPICCHIO PREFRITTE 1KG</t>
+          <t>PANCIOTTELLI AI FUNGHI 250G</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>21.820,00</t>
+          <t>27.692,00</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2623,19 +3379,19 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>BAGUETTE CLASSICA COTTA 260G</t>
+          <t>MIX SALATINI E PIZZETTE 400G</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>21.822,00</t>
+          <t>24.880,00</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2650,14 +3406,14 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>BAGUETTE 5 CEREALI COTTE 240G</t>
+          <t>MERLUZZETTI PANATI 100G</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>21.823,00</t>
+          <t>27.552,00</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2672,14 +3428,14 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>BAGUETTINO 100% INTEGR. COTTO 130G</t>
+          <t>FILETTO DI PLATESSA IMPANATA 300G</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>21.824,00</t>
+          <t>32.770,00</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2694,14 +3450,14 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>DEMI BAGUETTE CLASSICA COTTA 140G</t>
+          <t>CUORI DI FILETTO DI NASELLO 330G</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>22.255,00</t>
+          <t>11.179,00</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2716,14 +3472,14 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>PATATE RUSTICHE PREFRITTE 1K</t>
+          <t>FILETTO DI PANGASIO  800G</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>18.424,00</t>
+          <t>33.193,00</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2738,14 +3494,14 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>PATATE STICK DA FORNO 1KG</t>
+          <t>FILETTI DI SALMONE SELVAGGIO 250G</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>17.607,00</t>
+          <t>17.367,00</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2760,14 +3516,14 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>PATATE PREFRITTE 2,5KG</t>
+          <t>CALAMARI INTERI PULITI 400G</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2.359,00</t>
+          <t>32.045,00</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2777,19 +3533,19 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>PIZZA MARGHERITA CUCINO IO 3PZ 960G</t>
+          <t>VONGOLE DEL PACIFICO C/GUSCIO 1K</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>26.868,00</t>
+          <t>36.837,00</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2804,14 +3560,14 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>PIZZETTE MARGHERITA 4X80G</t>
+          <t>COTOLETTE DI POLLO C/SPINACI 2X110</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>35.597,00</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2821,24 +3577,24 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI ALLA PIZZAIOLA 250G</t>
+          <t>10 BASTONCINI DI VERDURE 300G</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>35.269,00</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2848,14 +3604,14 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI FORMAGGIO MOZZAR.250G</t>
+          <t>BURGER VEGAN AI CECI 2X75 VERDE AMO</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>31.078,00</t>
+          <t>21.820,00</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2865,19 +3621,19 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>FILETTO DI MERLUZZO CROCCANTE 400G</t>
+          <t>BAGUETTE CLASSICA COTTA 260G</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>24.442,00</t>
+          <t>12.654,00</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2892,19 +3648,19 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>MEDAGLIONI DI MERLUZZO 2X80G</t>
+          <t>GRAN SUGO ALLE COZZE  350G</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>27.552,00</t>
+          <t>12.654,00</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2914,14 +3670,14 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>FILETTO DI PLATESSA IMPANATA 300G</t>
+          <t>GRAN SUGO SCOGLIO C/POMOD.300G</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>12.208,00</t>
+          <t>27.657,00</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2931,298 +3687,12 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>4 PORZIONI DI MERLUZZO PESCARE'400G</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>32.770,00</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>CUORI DI FILETTO DI NASELLO 330G</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>17.271,00</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>FILETTI DI MERLUZZO PESCARE' 600G</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>26.520,00</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>FILETTO DI SGOMBRO 600G</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>24.854,00</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>FILETTI DI TONNO PINNA GIALLA 225G</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>36.479,00</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>CODE MAZZANCOLLE TROP.C/GUSC.350G</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>22.155,00</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>VONGOLE C/GUSCIO DEL PACIFICO 500G</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>31.679,00</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>CODE MAZZANC.SCOTTATE TROPICALI200G</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>1.044,00</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>COZZE SGUSCIATE PESCARE'250G</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>12.654,00</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>6,00</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>GRAN SUGO SCOGLIO C/POMOD.300G</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>12.654,00</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>3,00</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>GRAN SUGO ALLO SCOGLIO  300G</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>10.438,00</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>GNOCCHETTI ALLA SORRENTINA 550G</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>8.491,00</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>PISELLI PROSCIUTTO/FORMAGGIO 400G</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>35.510,00</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>BURGER AGLI SPINACI 2X80 G</t>
+          <t>STECCO FRUIT  GR 390</t>
         </is>
       </c>
     </row>
@@ -3237,7 +3707,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3270,7 +3740,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>14.470,00</t>
+          <t>25.793,00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -3285,14 +3755,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>MINESTRONE RICETTA GHIOTTA 750G</t>
+          <t>PATATE SPICCHI CON BUCCIA 600G</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>12.682,00</t>
+          <t>22.255,00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3307,14 +3777,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CICORIA FOGLIA X FOGLIA 450G</t>
+          <t>PATATE RUSTICHE PREFRITTE 1K</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>766,00</t>
+          <t>604,00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3329,14 +3799,14 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>MELANZANE RONDELLE GRIGLIATE 450G</t>
+          <t>PISELLI FINI BUSTA 1KG</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>10.562,00</t>
+          <t>8.491,00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3351,14 +3821,14 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ZUCCHINE A CUBETTI 450G</t>
+          <t>PISELLI PROSCIUTTO/FORMAGGIO 400G</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>25.872,00</t>
+          <t>15.706,00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3373,14 +3843,14 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>GRANFRITTO DI MARE 300G</t>
+          <t>TORTINO DI PATATE 300G</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>36.806,00</t>
+          <t>21.708,00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3395,14 +3865,14 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>PERLE DI BACCALA'IN PASTELLA 200G</t>
+          <t>GOCCE DI VERDURA 230G CUCINO IO</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>26.230,00</t>
+          <t>606,00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -3412,24 +3882,24 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ALICI DEL MEDITERRANEO PANATE 200G</t>
+          <t>SPINACI IN FOGLIA PORZIONATI 1KG</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>10.246,00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -3439,19 +3909,19 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI AI FUNGHI 250G</t>
+          <t>SPINACI FORMAGGIO/MOZZARELLA 450G</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>765,00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -3461,14 +3931,14 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI SPINACI/MOZZAR.250G</t>
+          <t>FAGIOLINI INTERI FINISSIMI 1KG</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>9.336,00</t>
+          <t>10.562,00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -3483,14 +3953,14 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>RAVIOLI RICOTTA E SPINACI  550G</t>
+          <t>ZUCCHINE A CUBETTI 450G</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1.129,00</t>
+          <t>25.748,00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -3505,14 +3975,14 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>8 MINICONO LOVING 320G</t>
+          <t>GAMBERI ARGENTINA INTERI 800G</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1.373,00</t>
+          <t>35.203,00</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -3527,14 +3997,14 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>8 RICOPERTI LOVING 400G</t>
+          <t>TRANCE DI PESCE SPADA 450G</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2.196,00</t>
+          <t>24.854,00</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -3544,19 +4014,19 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>8 MINISTECCHI ASSORT. LOVING 250G</t>
+          <t>FILETTI DI TONNO PINNA GIALLA 225G</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>9.052,00</t>
+          <t>26.364,00</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -3571,14 +4041,14 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>6 RICOPERTI FRAGOLA LOVING 300G</t>
+          <t>FISH &amp; CHIPS PASTELLATO 400G</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>11.190,00</t>
+          <t>31.078,00</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -3593,14 +4063,14 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>6 COPPETTE PANNA/CIOCCOLATO 300G</t>
+          <t>FILETTO DI MERLUZZO CROCCANTE 400G</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>12.166,00</t>
+          <t>32.966,00</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -3615,14 +4085,14 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>12 MINIMINICONI LOVING 225G</t>
+          <t>POLPETTE MERLUZZO MEDITERRANEA 500G</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>13.554,00</t>
+          <t>36.806,00</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -3637,14 +4107,14 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>6 GRANCONO MIX LOVING 450G</t>
+          <t>PERLE DI BACCALA'IN PASTELLA 200G</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>17.530,00</t>
+          <t>35.598,00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -3654,19 +4124,19 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>6 BARRETTE GELATO PANNA E MOU 250G</t>
+          <t>6 BASTONCINI DI SALMONE 150G</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>22.646,00</t>
+          <t>609,00</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3681,19 +4151,19 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>6 BARRETTE AL COCCO 250G</t>
+          <t>BASTONCINI DI MERLUZZO 900G</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>24.402,00</t>
+          <t>18.380,00</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -3703,19 +4173,19 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>6 CONI PANNA VAR.AMARENA 450G LOVIN</t>
+          <t>PIZZA FUNGHI BOSCO AL TAGLIERE 215G</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>30.760,00</t>
+          <t>18.380,00</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -3725,14 +4195,14 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>4 CONI TWIRL PANNA/CIOCC. 280G</t>
+          <t>PIZZA MARGHERITA AL TAGLIERE 220G</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>35.560,00</t>
+          <t>25.438,00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -3747,41 +4217,41 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>4 STECCHI CARAM.SALATO E CIOCC 260G</t>
+          <t>TRANCIO MARGHERITA 3PZ X 400G</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2.193,00</t>
+          <t>26.942,00</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>4 COPPA AL CAFFE' LOVING 280G</t>
+          <t>CALZONE POMODORO MOZZARELLA  250G</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>23.968,00</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>11,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -3791,51 +4261,293 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>VASCHETTA CARAMELLO SALATO ADS 200G</t>
+          <t>HAMBURGER BOVINO 10X75</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>11.487,00</t>
+          <t>30.344,00</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
           <t>2,00</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>TARTUFO AL CIOCCOLATO LOVING 2X80G</t>
+          <t>GHIACCIO ALIMENTARE TRITATO 2K</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>12.165,00</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>6 FRUTTA GELATA LOVING  360G</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>26.900,00</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>6 BISCOTTI PANNA C/GOCCE CIOC.288G</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>30.760,00</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>4 CONI TWIRL PANNA/CIOCC. 280G</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>32.200,00</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>GHIACCIOLI THE AL LIMONE 6X70G</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>35.560,00</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>4 STECCHI PISTACCHIO CIOC/B.CO 260</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>1.375,00</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>VASCH.STRACCIATELLA LOVING 500G</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>12.167,00</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>VASCHETTA PISTAC/GIANDUIA ADS 200G</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>12.167,00</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>9,00</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>VASCHETTA PANNA COTTA ADS 200G</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>18.268,00</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>6,00</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>VASCHETTA AFFOG. AL CACAO 500G</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
           <t>18.295,00</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>TRANCIO GRAN FRUTTA 8/10 PORZ. 700G</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>18.295,00</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>2,00</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>TRANCIO GRAN FRUTTA 8/10 PORZ. 700G</t>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>TRANCIO VAR AMARENA 8/10 PORZ. 700G</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>10.796,00</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>HAMBURGER VEGET.MELANZANE 100G</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Deepened the tuning of the processors
</commit_message>
<xml_diff>
--- a/comparison_result.xlsx
+++ b/comparison_result.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,7 +480,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>24.413,00</t>
+          <t>37.695,00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -493,30 +493,30 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>20 GHIACCIOLI 1200G</t>
+          <t>GHIACCIOLI ASS. MULTIVIT. 560G</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>20 GHIACCIOLI 1200G</t>
+          <t>GHIACCIOLI ASS. MULTIVIT. 560G</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>998,00</t>
+          <t>33.309,00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -525,34 +525,34 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>6 LEMON ICE LIQUIRIZIA LOVING 480G</t>
+          <t>CONI GRANITA LIMONE/ARANCIA 6X105G</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>6 LEMON ICE LIQUIRIZIA LOVING 480G</t>
+          <t>CONI GRANITA LIMONE/ARANCIA 6X105G</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>25.272,00</t>
+          <t>24.413,00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -565,30 +565,30 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>10 GHIACCIOLI LOVING 750G</t>
+          <t>20 GHIACCIOLI 1200G</t>
         </is>
       </c>
       <c r="E4" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>20 GHIACCIOLI 1200G</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
         <v>2</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>10 GHIACCIOLI LOVING 750G</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>-1</v>
-      </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>37.695,00</t>
+          <t>25.272,00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -601,7 +601,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>GHIACCIOLI ASS. MULTIVIT. 560G</t>
+          <t>10 GHIACCIOLI LOVING 750G</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -609,7 +609,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>GHIACCIOLI ASS. MULTIVIT. 560G</t>
+          <t>10 GHIACCIOLI LOVING 750G</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -624,7 +624,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>33.309,00</t>
+          <t>998,00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -637,30 +637,30 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>CONI GRANITA LIMONE/ARANCIA 6X105G</t>
+          <t>6 LEMON ICE LIQUIRIZIA LOVING 480G</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>CONI GRANITA LIMONE/ARANCIA 6X105G</t>
+          <t>6 LEMON ICE LIQUIRIZIA LOVING 480G</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1.373,00</t>
+          <t>27.627,00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -669,23 +669,23 @@
         </is>
       </c>
       <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>GELATO GRAN RIPIENO MIX 6PZ 360G</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
         <v>3</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>8 RICOPERTI LOVING 400G</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>2</v>
-      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>8 RICOPERTI LOVING 400G</t>
+          <t>GELATO GRAN RIPIENO MIX 6PZ 360G</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -696,7 +696,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>27.627,00</t>
+          <t>24.403,00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -705,34 +705,34 @@
         </is>
       </c>
       <c r="C8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
         <v>2</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>GELATO GRAN RIPIENO MIX 6PZ 360G</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>3</v>
-      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>GELATO GRAN RIPIENO MIX 6PZ 360G</t>
+          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>24.403,00</t>
+          <t>15.757,00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -741,34 +741,34 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
+          <t>4 MAXISTECCHI LOVING 350G</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
+          <t>4 MAXISTECCHI LOVING 350G</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>35.560,00</t>
+          <t>997,00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -781,30 +781,30 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>4 STECCHI CARAM.SALATO E CIOCC 260G</t>
+          <t>6 PRALINATI AMARENA LOVING 360G</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>4 STECCHI CARAM.SALATO E CIOCC 260G</t>
+          <t>6 PRALINATI AMARENA LOVING 360G</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>22.646,00</t>
+          <t>35.560,00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -817,30 +817,30 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>6 BARRETTE AL COCCO 250G</t>
+          <t>4 STECCHI CARAM.SALATO E CIOCC 260G</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>6 BARRETTE AL COCCO 250G</t>
+          <t>4 STECCHI CARAM.SALATO E CIOCC 260G</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>17.530,00</t>
+          <t>1.373,00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -853,30 +853,30 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>6 BARRETTE GELATO PANNA E MOU 250G</t>
+          <t>8 RICOPERTI LOVING 400G</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>6 BARRETTE GELATO PANNA E MOU 250G</t>
+          <t>8 RICOPERTI LOVING 400G</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2.196,00</t>
+          <t>30.344,00</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -889,7 +889,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>8 MINISTECCHI ASSORT. LOVING 250G</t>
+          <t>GHIACCIO ALIMENTARE TRITATO 2K</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -897,7 +897,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>8 MINISTECCHI ASSORT. LOVING 250G</t>
+          <t>GHIACCIO ALIMENTARE TRITATO 2K</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -912,7 +912,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>13.292,00</t>
+          <t>2.196,00</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -925,30 +925,30 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>6 MAXISANDWICH LOVING  480G</t>
+          <t>8 MINISTECCHI ASSORT. LOVING 250G</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>6 MAXISANDWICH LOVING  480G</t>
+          <t>8 MINISTECCHI ASSORT. LOVING 250G</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1.374,00</t>
+          <t>17.530,00</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>8 SANDWICH LOVING 400G</t>
+          <t>6 BARRETTE GELATO PANNA E MOU 250G</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -969,7 +969,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>8 SANDWICH LOVING 400G</t>
+          <t>6 BARRETTE GELATO PANNA E MOU 250G</t>
         </is>
       </c>
       <c r="G15" t="n">
@@ -984,7 +984,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>11.190,00</t>
+          <t>9.053,00</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -993,34 +993,34 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>6 COPPETTE PANNA/CIOCCOLATO 300G</t>
+          <t>6 MINIBISCOTTI LOVING 325G</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>6 COPPETTE PANNA/CIOCCOLATO 300G</t>
+          <t>6 MINIBISCOTTI LOVING 325G</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1.129,00</t>
+          <t>2.193,00</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1029,11 +1029,11 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>8 MINICONO LOVING 320G</t>
+          <t>4 COPPA AL CAFFE' LOVING 280G</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -1041,22 +1041,22 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>8 MINICONO LOVING 320G</t>
+          <t>4 COPPA AL CAFFE' LOVING 280G</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>35.947,00</t>
+          <t>17.772,00</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1069,7 +1069,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>CONI PANNA S/GLUTINE 4X75G</t>
+          <t>8 BISCOTTI TONDI VAN/CAC LOVIN.280G</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -1077,7 +1077,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>CONI PANNA S/GLUTINE 4X75G</t>
+          <t>8 BISCOTTI TONDI VAN/CAC LOVIN.280G</t>
         </is>
       </c>
       <c r="G18" t="n">
@@ -1092,28 +1092,28 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>24.402,00</t>
+          <t>13.292,00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>6 CONI PANNA VAR.AMARENA 450G LOVIN</t>
+          <t>6 MAXISANDWICH LOVING  480G</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>6 CONI PANNA VAR.AMARENA 450G LOVIN</t>
+          <t>6 MAXISANDWICH LOVING  480G</t>
         </is>
       </c>
       <c r="G19" t="n">
@@ -1128,7 +1128,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>13.554,00</t>
+          <t>1.374,00</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1137,19 +1137,19 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>6 GRANCONO MIX LOVING 450G</t>
+          <t>8 SANDWICH LOVING 400G</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>6 GRANCONO MIX LOVING 450G</t>
+          <t>8 SANDWICH LOVING 400G</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -1164,7 +1164,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>17.667,00</t>
+          <t>1.129,00</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1177,30 +1177,30 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>GELATI DI SOIA ASSORTITI 360G</t>
+          <t>8 MINICONO LOVING 320G</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>GELATI DI SOIA ASSORTITI 360G</t>
+          <t>8 MINICONO LOVING 320G</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>32.500,00</t>
+          <t>12.166,00</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1209,34 +1209,34 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>6 CONI PANNA GR 420 LOVING</t>
+          <t>12 MINIMINICONI LOVING 225G</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>6 CONI PANNA GR 420 LOVING</t>
+          <t>12 MINIMINICONI LOVING 225G</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>24.358,00</t>
+          <t>17.667,00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>TORTA GELATO PANNA CIOCC. 450G LOV</t>
+          <t>GELATI DI SOIA ASSORTITI 360G</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>TORTA GELATO PANNA CIOCC. 450G LOV</t>
+          <t>GELATI DI SOIA ASSORTITI 360G</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1272,7 +1272,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>18.294,00</t>
+          <t>13.554,00</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1281,39 +1281,39 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>TORTA GELATO S.HONORE'12/14PORZ 1KG</t>
+          <t>6 GRANCONO MIX LOVING 450G</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>TORTA GELATO S.HONORE'12/14PORZ 1KG</t>
+          <t>6 GRANCONO MIX LOVING 450G</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>602,00</t>
+          <t>24.402,00</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>VASCHETTA CACAO STRACC.CAFFE' 1KG</t>
+          <t>6 CONI PANNA/CIOCCOLATO 450G LOVING</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -1329,7 +1329,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>VASCHETTA CACAO STRACC.CAFFE' 1KG</t>
+          <t>6 CONI PANNA/CIOCCOLATO 450G LOVING</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -1344,7 +1344,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>602,00</t>
+          <t>24.402,00</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1353,75 +1353,75 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>VASCHETTA VANIGLIA CACAO NOCC.1KG</t>
+          <t>6 CONI PANNA VAR.AMARENA 450G LOVIN</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>VASCHETTA VANIGLIA CACAO NOCC.1KG</t>
+          <t>6 CONI PANNA VAR.AMARENA 450G LOVIN</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>18.269,00</t>
+          <t>32.500,00</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
+          <t>6 CONI PANNA GR 420 LOVING</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
+          <t>6 CONI PANNA GR 420 LOVING</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>18.269,00</t>
+          <t>11.487,00</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1429,7 +1429,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>VASCHETTA ZUPPA INGLESE 1KG</t>
+          <t>TARTUFO BIANCO LOVING  2X80G</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -1437,7 +1437,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>VASCHETTA ZUPPA INGLESE 1KG</t>
+          <t>TARTUFO BIANCO LOVING  2X80G</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -1452,43 +1452,43 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>18.268,00</t>
+          <t>22.645,00</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>VASCHETTA YOGURT FRUTTI BOSCO 500G</t>
+          <t>12 MINI BON BON PANNA/CIOCC. 110G</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>VASCHETTA YOGURT FRUTTI BOSCO 500G</t>
+          <t>12 MINI BON BON PANNA/CIOCC. 110G</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1.375,00</t>
+          <t>32.052,00</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1501,107 +1501,107 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>VASCH.PANNA LOVING 500G</t>
+          <t>CORNETTO CLASSICO VUOTO 4PZ 280G</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>VASCH.PANNA LOVING 500G</t>
+          <t>CORNETTO CLASSICO VUOTO 4PZ 280G</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>18.268,00</t>
+          <t>18.294,00</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>VASCHETTA SPAGNOLA 500G</t>
+          <t>TORTA GELATO S.HONORE'12/14PORZ 1KG</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>VASCHETTA SPAGNOLA 500G</t>
+          <t>TORTA GELATO S.HONORE'12/14PORZ 1KG</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>27.488,00</t>
+          <t>18.295,00</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>GELATO ALLO YOGURT GRECO B.CO 320G</t>
+          <t>TRANCIO VAR AMARENA 8/10 PORZ. 700G</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>GELATO ALLO YOGURT GRECO B.CO 320G</t>
+          <t>TRANCIO VAR AMARENA 8/10 PORZ. 700G</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>27.488,00</t>
+          <t>602,00</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1609,35 +1609,35 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
+          <t>VASCHETTA FRAGOLA LIMONE PESCA 1KG</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
+          <t>VASCHETTA FRAGOLA LIMONE PESCA 1KG</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>27.488,00</t>
+          <t>18.269,00</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1645,7 +1645,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO C/NOCCIOLA 320G</t>
+          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1653,7 +1653,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO C/NOCCIOLA 320G</t>
+          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -1668,12 +1668,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>27.488,00</t>
+          <t>1.375,00</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO AL MIELE 320G</t>
+          <t>VASCH.PANNA LOVING 500G</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1689,7 +1689,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO AL MIELE 320G</t>
+          <t>VASCH.PANNA LOVING 500G</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -1704,7 +1704,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>1.375,00</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1717,7 +1717,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>VASCHETTA TRIPLO CIOCC.ADS 200G</t>
+          <t>VASCH.STRACCIATELLA LOVING 500G</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1725,7 +1725,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>VASCHETTA TRIPLO CIOCC.ADS 200G</t>
+          <t>VASCH.STRACCIATELLA LOVING 500G</t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -1740,12 +1740,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>18.268,00</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>11,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1753,35 +1753,35 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>VASCHETTA CARAMELLO SALATO ADS 200G</t>
+          <t>VASCHETTA AFFOG. AL CACAO 500G</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>VASCHETTA CARAMELLO SALATO ADS 200G</t>
+          <t>VASCHETTA AFFOG. AL CACAO 500G</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2.627,00</t>
+          <t>18.268,00</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1789,35 +1789,35 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>PREZZEMOLO TRITATO  50G</t>
+          <t>VASCHETTA SPAGNOLA 500G</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>PREZZEMOLO TRITATO  50G</t>
+          <t>VASCHETTA SPAGNOLA 500G</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>27.609,00</t>
+          <t>18.268,00</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1825,7 +1825,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>VERDURE PER SOFFRITTO 450G</t>
+          <t>VASCHETTA AFFOG. CAFFE' 500G</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -1833,7 +1833,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>VERDURE PER SOFFRITTO 450G</t>
+          <t>VASCHETTA AFFOG. CAFFE' 500G</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -1848,12 +1848,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>593,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>MISTO FUNGHI 300G</t>
+          <t>VASCHETTA SPAGNOLA LOVING 200G</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1869,7 +1869,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>MISTO FUNGHI 300G</t>
+          <t>VASCHETTA SPAGNOLA LOVING 200G</t>
         </is>
       </c>
       <c r="G40" t="n">
@@ -1884,20 +1884,20 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>18.022,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>PATATE A SPICCHIO PREFRITTE 1KG</t>
+          <t>VASCHETTA CASSATA LOVING 200G</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1905,35 +1905,35 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>PATATE A SPICCHIO PREFRITTE 1KG</t>
+          <t>VASCHETTA CASSATA LOVING 200G</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>603,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>PATATE PREFRITTE STICK 1KG</t>
+          <t>VASCHETTA CAFFE'ARABICA LOVING 200G</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -1941,27 +1941,27 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>PATATE PREFRITTE STICK 1KG</t>
+          <t>VASCHETTA CAFFE'ARABICA LOVING 200G</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>17.607,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1969,43 +1969,43 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>PATATE PREFRITTE 2,5KG</t>
+          <t>VASCHETTA TRIPLO CIOCC.ADS 200G</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>PATATE PREFRITTE 2,5KG</t>
+          <t>VASCHETTA TRIPLO CIOCC.ADS 200G</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2.359,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>PIZZA MARGHERITA CUCINO IO 3PZ 960G</t>
+          <t>VASCHETTA LIMONE SICILIA ADS 200G</t>
         </is>
       </c>
       <c r="E44" t="n">
@@ -2013,27 +2013,27 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>PIZZA MARGHERITA CUCINO IO 3PZ 960G</t>
+          <t>VASCHETTA LIMONE SICILIA ADS 200G</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>25.437,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>9,00</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -2041,7 +2041,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>PIZZA MARGHERITA 300G</t>
+          <t>VASCHETTA PANNA COTTA ADS 200G</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -2049,7 +2049,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>PIZZA MARGHERITA 300G</t>
+          <t>VASCHETTA PANNA COTTA ADS 200G</t>
         </is>
       </c>
       <c r="G45" t="n">
@@ -2064,48 +2064,48 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>26.868,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>11,00</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>PIZZETTE MARGHERITA 4X80G</t>
+          <t>VASCHETTA CARAMELLO SALATO ADS 200G</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>PIZZETTE MARGHERITA 4X80G</t>
+          <t>VASCHETTA CARAMELLO SALATO ADS 200G</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>24.166,00</t>
+          <t>27.488,00</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -2113,35 +2113,35 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>MIX 5 VERDURE PASTELLATE 300G</t>
+          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>MIX 5 VERDURE PASTELLATE 300G</t>
+          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>12.735,00</t>
+          <t>27.488,00</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -2149,7 +2149,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>OLIVE ALL'ASCOLANA PREFRITTE 500G</t>
+          <t>GELATO YOGURT GRECO C/NOCCIOLA 320G</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -2157,7 +2157,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>OLIVE ALL'ASCOLANA PREFRITTE 500G</t>
+          <t>GELATO YOGURT GRECO C/NOCCIOLA 320G</t>
         </is>
       </c>
       <c r="G48" t="n">
@@ -2172,7 +2172,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>605,00</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2185,35 +2185,35 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI ALLA PIZZAIOLA 250G</t>
+          <t>MINESTRONE 15 VERDURE 1KG</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI ALLA PIZZAIOLA 250G</t>
+          <t>MINESTRONE 15 VERDURE 1KG</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>604,00</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI PROSC.FORMAGGIO 250G</t>
+          <t>PISELLI FINI BUSTA 1KG</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI PROSC.FORMAGGIO 250G</t>
+          <t>PISELLI FINI BUSTA 1KG</t>
         </is>
       </c>
       <c r="G50" t="n">
@@ -2244,12 +2244,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>22.587,00</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -2257,7 +2257,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI FORMAGGIO MOZZAR.250G</t>
+          <t>BROCCOLI A ROSETTE BONTA'ORTO 600G</t>
         </is>
       </c>
       <c r="E51" t="n">
@@ -2265,7 +2265,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI FORMAGGIO MOZZAR.250G</t>
+          <t>BROCCOLI A ROSETTE BONTA'ORTO 600G</t>
         </is>
       </c>
       <c r="G51" t="n">
@@ -2280,7 +2280,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>1.797,00</t>
+          <t>27.609,00</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>PINZE GRANCHIO PANATE S/GLUT.250G</t>
+          <t>VERDURE PER SOFFRITTO 450G</t>
         </is>
       </c>
       <c r="E52" t="n">
@@ -2301,7 +2301,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>PINZE GRANCHIO PANATE S/GLUT.250G</t>
+          <t>VERDURE PER SOFFRITTO 450G</t>
         </is>
       </c>
       <c r="G52" t="n">
@@ -2316,7 +2316,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>20.432,00</t>
+          <t>606,00</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2325,34 +2325,34 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>BAST.FILETTI MERLUZZO S/GLUTINE 300</t>
+          <t>SPINACI IN FOGLIA PORZIONATI 1KG</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>BAST.FILETTI MERLUZZO S/GLUTINE 300</t>
+          <t>SPINACI IN FOGLIA PORZIONATI 1KG</t>
         </is>
       </c>
       <c r="G53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>26.859,00</t>
+          <t>8.490,00</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2365,7 +2365,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>MINI TOAST PROSCIUT/MOZZAR. 180G</t>
+          <t>SPINACI FOGLIA PER FOGLIA 450G</t>
         </is>
       </c>
       <c r="E54" t="n">
@@ -2373,7 +2373,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>MINI TOAST PROSCIUT/MOZZAR. 180G</t>
+          <t>SPINACI FOGLIA PER FOGLIA 450G</t>
         </is>
       </c>
       <c r="G54" t="n">
@@ -2388,7 +2388,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>35.681,00</t>
+          <t>1.515,00</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>ANELLI CIUFFI CALAMARO PATAG. 400G</t>
+          <t>BIETA IN FOGLIA PORZIONATA 1KG</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -2409,7 +2409,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>ANELLI CIUFFI CALAMARO PATAG. 400G</t>
+          <t>BIETA IN FOGLIA PORZIONATA 1KG</t>
         </is>
       </c>
       <c r="G55" t="n">
@@ -2424,7 +2424,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>22.155,00</t>
+          <t>22.255,00</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>VONGOLE C/GUSCIO DEL PACIFICO 500G</t>
+          <t>PATATE RUSTICHE PREFRITTE 1K</t>
         </is>
       </c>
       <c r="E56" t="n">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>VONGOLE C/GUSCIO DEL PACIFICO 500G</t>
+          <t>PATATE RUSTICHE PREFRITTE 1K</t>
         </is>
       </c>
       <c r="G56" t="n">
@@ -2460,7 +2460,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>14.306,00</t>
+          <t>593,00</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2473,7 +2473,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>GAMBERI ZUCCHINE C/POM.PESCARE'300G</t>
+          <t>MISTO FUNGHI 300G</t>
         </is>
       </c>
       <c r="E57" t="n">
@@ -2481,7 +2481,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>GAMBERI ZUCCHINE C/POM.PESCARE'300G</t>
+          <t>MISTO FUNGHI 300G</t>
         </is>
       </c>
       <c r="G57" t="n">
@@ -2496,12 +2496,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>12.654,00</t>
+          <t>18.022,00</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -2509,7 +2509,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>GRAN SUGO ALLO SCOGLIO  300G</t>
+          <t>PATATE A SPICCHIO PREFRITTE 1KG</t>
         </is>
       </c>
       <c r="E58" t="n">
@@ -2517,7 +2517,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>GRAN SUGO ALLO SCOGLIO  300G</t>
+          <t>PATATE A SPICCHIO PREFRITTE 1KG</t>
         </is>
       </c>
       <c r="G58" t="n">
@@ -2532,12 +2532,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>12.654,00</t>
+          <t>603,00</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -2545,43 +2545,43 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>GRAN SUGO AI FRUTTI DI MARE  300G</t>
+          <t>PATATE PREFRITTE STICK 1KG</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>GRAN SUGO AI FRUTTI DI MARE  300G</t>
+          <t>PATATE PREFRITTE STICK 1KG</t>
         </is>
       </c>
       <c r="G59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>12.654,00</t>
+          <t>18.424,00</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>GRAN SUGO AI GAMBERI 250G</t>
+          <t>PATATE STICK DA FORNO 1KG</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -2589,22 +2589,22 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>GRAN SUGO AI GAMBERI 250G</t>
+          <t>PATATE STICK DA FORNO 1KG</t>
         </is>
       </c>
       <c r="G60" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>35.510,00</t>
+          <t>25.820,00</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2617,7 +2617,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>BURGER AGLI SPINACI 2X80 G</t>
+          <t>SFOGLINO RICOTTA E SPINACI 300G</t>
         </is>
       </c>
       <c r="E61" t="n">
@@ -2625,7 +2625,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>BURGER AGLI SPINACI 2X80 G</t>
+          <t>SFOGLINO RICOTTA E SPINACI 300G</t>
         </is>
       </c>
       <c r="G61" t="n">
@@ -2640,7 +2640,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>35.559,00</t>
+          <t>35.621,00</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2653,30 +2653,30 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>6 CONI CAFFE' 450G</t>
+          <t>PIZZA SALAMINO/PROVOLONE 26X38 535G</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>6 CONI CAFFE' 450G</t>
+          <t>PIZZA SALAMINO/PROVOLONE 26X38 535G</t>
         </is>
       </c>
       <c r="G62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>9.053,00</t>
+          <t>13.597,00</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2689,23 +2689,671 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>6 MINIBISCOTTI LOVING 325G</t>
+          <t>MISTO OLIVE/CROCC/SUPPLI/ARANC 500G</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>6 MINIBISCOTTI LOVING 325G</t>
+          <t>MISTO OLIVE/CROCC/SUPPLI/ARANC 500G</t>
         </is>
       </c>
       <c r="G63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>28.897,00</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>1</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>PANCIOTTELLI PROSC.FORMAGGIO 250G</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>1</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>PANCIOTTELLI PROSC.FORMAGGIO 250G</t>
+        </is>
+      </c>
+      <c r="G64" t="n">
+        <v>0</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>31.079,00</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>1</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>18 BASTONCINI FILETTO MERLUZZO 450G</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>18 BASTONCINI FILETTO MERLUZZO 450G</t>
+        </is>
+      </c>
+      <c r="G65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>609,00</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>1</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>BASTONCINI DI MERLUZZO 900G</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>1</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>BASTONCINI DI MERLUZZO 900G</t>
+        </is>
+      </c>
+      <c r="G66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>31.529,00</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>1</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>GRANFRITTO MISTO   500G</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>GRANFRITTO MISTO   500G</t>
+        </is>
+      </c>
+      <c r="G67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>17.271,00</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>1</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>FILETTI DI MERLUZZO PESCARE' 600G</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>FILETTI DI MERLUZZO PESCARE' 600G</t>
+        </is>
+      </c>
+      <c r="G68" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>11.179,00</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>1</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>FILETTO DI PANGASIO  800G</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>1</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>FILETTO DI PANGASIO  800G</t>
+        </is>
+      </c>
+      <c r="G69" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>595,00</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>3</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>GAMBERETTI SGUSCIATI 330/300G</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>GAMBERETTI SGUSCIATI 330/300G</t>
+        </is>
+      </c>
+      <c r="G70" t="n">
+        <v>-2</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Decrease</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>22.155,00</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>1</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>VONGOLE C/GUSCIO DEL PACIFICO 500G</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>1</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>VONGOLE C/GUSCIO DEL PACIFICO 500G</t>
+        </is>
+      </c>
+      <c r="G71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>14.306,00</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>1</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>GAMBERI ZUCCHINE C/POM.PESCARE'300G</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>1</v>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>GAMBERI ZUCCHINE C/POM.PESCARE'300G</t>
+        </is>
+      </c>
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>12.654,00</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>6,00</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>1</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>GRAN SUGO SCOGLIO C/POMOD.300G</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>1</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>GRAN SUGO SCOGLIO C/POMOD.300G</t>
+        </is>
+      </c>
+      <c r="G73" t="n">
+        <v>0</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>12.654,00</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>1</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>GRAN SUGO AI FRUTTI DI MARE  300G</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>1</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>GRAN SUGO AI FRUTTI DI MARE  300G</t>
+        </is>
+      </c>
+      <c r="G74" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>12.654,00</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>1</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>GRAN SUGO ALLO SCOGLIO  300G</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>1</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>GRAN SUGO ALLO SCOGLIO  300G</t>
+        </is>
+      </c>
+      <c r="G75" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>12.654,00</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>4,00</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>1</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>GRAN SUGO ALLE VONGOLE CUCINO  350G</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>1</v>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>GRAN SUGO ALLE VONGOLE CUCINO  350G</t>
+        </is>
+      </c>
+      <c r="G76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>23.968,00</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>1</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>HAMBURGER BOVINO 10X75</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>1</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>HAMBURGER BOVINO 10X75</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
+        <v>0</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>35.597,00</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>1</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>10 BASTONCINI DI VERDURE 300G</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>1</v>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>10 BASTONCINI DI VERDURE 300G</t>
+        </is>
+      </c>
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>8.491,00</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>1</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>PISELLI PROSCIUTTO/FORMAGGIO 400G</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>1</v>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>PISELLI PROSCIUTTO/FORMAGGIO 400G</t>
+        </is>
+      </c>
+      <c r="G79" t="n">
+        <v>0</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>10.796,00</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>1</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>HAMBURGER VEGET.MELANZANE 100G</t>
+        </is>
+      </c>
+      <c r="E80" t="n">
+        <v>1</v>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>HAMBURGER VEGET.MELANZANE 100G</t>
+        </is>
+      </c>
+      <c r="G80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>10.796,00</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>1</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>HAMBURGER VEGET.CARCIOFI 100G</t>
+        </is>
+      </c>
+      <c r="E81" t="n">
+        <v>1</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>HAMBURGER VEGET.CARCIOFI 100G</t>
+        </is>
+      </c>
+      <c r="G81" t="n">
+        <v>0</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Same</t>
         </is>
       </c>
     </row>
@@ -2720,7 +3368,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2753,7 +3401,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>11.189,00</t>
+          <t>21.820,00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -2763,19 +3411,19 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>6 STECCHI RICOPERTI CIOCC.300G</t>
+          <t>BAGUETTE CLASSICA COTTA 260G</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>15.757,00</t>
+          <t>21.823,00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2790,14 +3438,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>4 MAXISTECCHI LOVING 350G</t>
+          <t>BAGUETTINO 100% INTEGR. COTTO 130G</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>30.345,00</t>
+          <t>24.359,00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -2807,19 +3455,19 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>GHIACCIO ALIMENTARE CUBETTO 2K</t>
+          <t>8 GELATINI RICOPERTI CIOCC.240G</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>24.401,00</t>
+          <t>30.345,00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -2829,19 +3477,19 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4 COPPE AMARENA 350G LOVING</t>
+          <t>GHIACCIO ALIMENTARE CUBETTO 2K</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>24.402,00</t>
+          <t>30.760,00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -2851,19 +3499,19 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>6 CONI PANNA/CIOCCOLATO 450G LOVING</t>
+          <t>4 CONI TWIRL PANNA/CIOCC. 280G</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>32.499,00</t>
+          <t>35.559,00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2873,24 +3521,24 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>6 CONI PANNA GR 450 LOVING ORO</t>
+          <t>6 CONI CAFFE' 450G</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>9.051,00</t>
+          <t>32.499,00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2900,80 +3548,80 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>DESSERT VANIGLIA CACAO LOVING 320G</t>
+          <t>6 CONI PANNA GR 450 LOVING ORO</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>22.076,00</t>
+          <t>11.487,00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>MISTO FRUTTI DI BOSCO 300G</t>
+          <t>TARTUFO AL CIOCCOLATO LOVING 2X80G</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1.375,00</t>
+          <t>24.358,00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>VASCH.CREMA/CACAO LOVING 500G</t>
+          <t>TORTA GELATO PANNA CIOCC. 450G LOV</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>9.051,00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>VASCHETTA LIMONE SICILIA ADS 200G</t>
+          <t>DESSERT VANIGLIA CACAO LOVING 320G</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>605,00</t>
+          <t>9.051,00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2988,14 +3636,14 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>MINESTRONE 15 VERDURE 1KG</t>
+          <t>DESSERT CREMA CAFFE' LOVING 320G</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>31.628,00</t>
+          <t>18.295,00</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -3005,24 +3653,24 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ROSETTE DI BROCCOLO ROMANESCO 600G</t>
+          <t>TRANCIO GRAN FRUTTA 8/10 PORZ. 700G</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>22.587,00</t>
+          <t>18.269,00</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -3032,58 +3680,58 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>BROCCOLI A ROSETTE BONTA'ORTO 600G</t>
+          <t>VASCHETTA NOCCIOLATO 1KG</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>8.399,00</t>
+          <t>18.269,00</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>ERBETTE DI CAMPO CUBETTI 450G</t>
+          <t>VASCHETTA ZUPPA INGLESE 1KG</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>12.683,00</t>
+          <t>1.375,00</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>BIETA FOGLIA X FOGLIA 450G</t>
+          <t>VASCH.CREMA/CACAO LOVING 500G</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1.083,00</t>
+          <t>18.268,00</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -3098,14 +3746,14 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>CICORIA IN FOGLIA PORZIONATA 1KG</t>
+          <t>VASCHETTA TIRAMISU' 500G</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>17.518,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -3115,19 +3763,19 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>MISTO BOSCO C/PORCINI GR 1000</t>
+          <t>VASCHETTA STRACCIATELLA LOVING 200G</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>24.797,00</t>
+          <t>36.103,00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -3142,14 +3790,14 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>PATATE A FETTE GR 600</t>
+          <t>SORBETTO AL LIMONE LOVING 250G</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>35.621,00</t>
+          <t>766,00</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3164,14 +3812,14 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>PIZZA SALAMINO/PROVOLONE 26X38 535G</t>
+          <t>MELANZANE RONDELLE GRIGLIATE 450G</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>29.386,00</t>
+          <t>27.610,00</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -3186,14 +3834,14 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>PIZZA MARGHERITA 26X38 485G</t>
+          <t>PISELLI FINISSIMI 1KG</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>26.186,00</t>
+          <t>9.298,00</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -3208,14 +3856,14 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>PIZZA MARGHERITA S/GLUTINE 300G</t>
+          <t>CIPOLLA TRITATA 150G</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>37.651,00</t>
+          <t>8.399,00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -3225,24 +3873,24 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>FOCACCIA FARCITA PROSC/FORM.330G</t>
+          <t>ERBETTE DI CAMPO CUBETTI 450G</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>18.380,00</t>
+          <t>12.683,00</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -3252,14 +3900,14 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>PIZZA VERD.GRIGLIATE TAGLIERE 235G</t>
+          <t>BIETA FOGLIA X FOGLIA 450G</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>9.376,00</t>
+          <t>1.287,00</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3274,14 +3922,14 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>CROCCHETTE PATATE ALLA ROMANA 500G</t>
+          <t>FUNGHI PORCINI CUBETTATI 300G</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4.138,00</t>
+          <t>35.774,00</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3296,14 +3944,14 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>CROCCHETTE DI PATATE  600G</t>
+          <t>PATATE A BARCHETTA 600G</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1.500,00</t>
+          <t>15.706,00</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3318,14 +3966,14 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>SUPPLI'DI RISO AL RAGU'500G</t>
+          <t>TORTINO DI PATATE 300G</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>13.597,00</t>
+          <t>2.359,00</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -3340,19 +3988,19 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>MISTO OLIVE/CROCC/SUPPLI/ARANC 500G</t>
+          <t>PIZZA MARGHERITA CUCINO IO 3PZ 960G</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>18.047,00</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -3362,14 +4010,14 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI AI FUNGHI 250G</t>
+          <t>PIZZA 4 FORMAGGI CUCINO IO 350G</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>27.692,00</t>
+          <t>18.210,00</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3384,14 +4032,14 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>MIX SALATINI E PIZZETTE 400G</t>
+          <t>PIZZA IMPERIALE VERACE 490G</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>24.880,00</t>
+          <t>18.048,00</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3406,19 +4054,19 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>MERLUZZETTI PANATI 100G</t>
+          <t>PIZZA TONNO CIPOLLA CUCINO IO 390G</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>27.552,00</t>
+          <t>26.361,00</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -3428,14 +4076,14 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>FILETTO DI PLATESSA IMPANATA 300G</t>
+          <t>PIZZAROLLO SPINACI E RICOTTA 180GR</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>32.770,00</t>
+          <t>18.046,00</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3450,19 +4098,19 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>CUORI DI FILETTO DI NASELLO 330G</t>
+          <t>PIZZA ALLA DIAVOLA CUCINO IO 315G</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>11.179,00</t>
+          <t>18.380,00</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -3472,14 +4120,14 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>FILETTO DI PANGASIO  800G</t>
+          <t>PIZZA CON PATATE  AL TAGLIERE 200G</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>33.193,00</t>
+          <t>26.231,00</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3494,14 +4142,14 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>FILETTI DI SALMONE SELVAGGIO 250G</t>
+          <t>PANZEROTTINI POMODORO/MOZZ.250G</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>17.367,00</t>
+          <t>26.860,00</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3516,14 +4164,14 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>CALAMARI INTERI PULITI 400G</t>
+          <t>MINI HOTDOGS IN PASTA PIZZA 220G</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>32.045,00</t>
+          <t>20.428,00</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3538,14 +4186,14 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>VONGOLE DEL PACIFICO C/GUSCIO 1K</t>
+          <t>FILETTI BACCALA' IN PASTELLA 300G</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>36.837,00</t>
+          <t>15.758,00</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3560,14 +4208,14 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>COTOLETTE DI POLLO C/SPINACI 2X110</t>
+          <t>BOCCONCINI MOZZARELLA PANATI 300G</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>35.597,00</t>
+          <t>32.528,00</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3582,14 +4230,14 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>10 BASTONCINI DI VERDURE 300G</t>
+          <t>MOZZARELLA IN CARROZZA 4X50G</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>35.269,00</t>
+          <t>12.735,00</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3604,36 +4252,36 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>BURGER VEGAN AI CECI 2X75 VERDE AMO</t>
+          <t>OLIVE ALL'ASCOLANA PREFRITTE 500G</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>21.820,00</t>
+          <t>28.897,00</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>BAGUETTE CLASSICA COTTA 260G</t>
+          <t>PANCIOTTELLI SPINACI/MOZZAR.250G</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>12.654,00</t>
+          <t>24.442,00</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3648,19 +4296,19 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>GRAN SUGO ALLE COZZE  350G</t>
+          <t>MEDAGLIONI DI MERLUZZO 2X80G</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>12.654,00</t>
+          <t>24.442,00</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -3670,14 +4318,14 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>GRAN SUGO SCOGLIO C/POMOD.300G</t>
+          <t>MEDAGLIONI DI SALMONE 2X80G</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>27.657,00</t>
+          <t>27.552,00</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3692,7 +4340,293 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>STECCO FRUIT  GR 390</t>
+          <t>FILETTO DI PLATESSA IMPANATA 300G</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>32.770,00</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>CUORI DI FILETTO DI NASELLO 330G</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>17.205,00</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>FILETTI DI BACCALA' GR 400</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>26.520,00</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>FILETTO DI SGOMBRO 600G</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>591,00</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>MERLUZZO DECAPITATO P.V. PESCARE'</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>24.854,00</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>FILETTI DI TONNO PINNA GIALLA 225G</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>1.084,00</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>SEPPIE PULITE 400G</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>23.661,00</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>ANELLI TOTANO ATLANICI  400G</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>592,00</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>MISTO DEL PESCATORE PESCARE' 300G</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>10.438,00</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>GNOCCHETTI ALLA SORRENTINA 550G</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>22.200,00</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>BUCATINI ALL'AMATRICIANA 500G</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>32.966,00</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>POLPETTE MERLUZZO MEDITERRANEA 500G</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>34.018,00</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>COTOLETTE DI POLLO 2X90 G</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>35.269,00</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>BURGER VEGAN AI CECI 2X75 VERDE AMO</t>
         </is>
       </c>
     </row>
@@ -3740,7 +4674,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>25.793,00</t>
+          <t>36.839,00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -3755,14 +4689,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>PATATE SPICCHI CON BUCCIA 600G</t>
+          <t>VELLUTATA DI ZUCCA E CAROTA 600G</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>22.255,00</t>
+          <t>17.607,00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3777,14 +4711,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PATATE RUSTICHE PREFRITTE 1K</t>
+          <t>PATATE PREFRITTE 2,5KG</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>604,00</t>
+          <t>8.396,00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3799,14 +4733,14 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>PISELLI FINI BUSTA 1KG</t>
+          <t>PEPERONATA 450G</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>8.491,00</t>
+          <t>610,00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3821,14 +4755,14 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>PISELLI PROSCIUTTO/FORMAGGIO 400G</t>
+          <t>CUORI DI CARCIOFO INTERI 450G</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>15.706,00</t>
+          <t>765,00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3843,14 +4777,14 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>TORTINO DI PATATE 300G</t>
+          <t>FAGIOLINI INTERI FINISSIMI 1KG</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>21.708,00</t>
+          <t>2.630,00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3865,14 +4799,14 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>GOCCE DI VERDURA 230G CUCINO IO</t>
+          <t>BASILICO TRITATO  50G</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>606,00</t>
+          <t>1.505,00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -3882,19 +4816,19 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SPINACI IN FOGLIA PORZIONATI 1KG</t>
+          <t>PESCE X SPAGHETTATA PESCARE'300G</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>10.246,00</t>
+          <t>18.595,00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -3909,14 +4843,14 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>SPINACI FORMAGGIO/MOZZARELLA 450G</t>
+          <t>ZUPPA DI PESCE PESCARE 800G</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>765,00</t>
+          <t>27.383,00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -3931,14 +4865,14 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>FAGIOLINI INTERI FINISSIMI 1KG</t>
+          <t>POLPO PULITO 500G</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10.562,00</t>
+          <t>31.679,00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -3953,14 +4887,14 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ZUCCHINE A CUBETTI 450G</t>
+          <t>CODE MAZZANC.SCOTTATE TROPICALI200G</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>25.748,00</t>
+          <t>35.681,00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -3975,14 +4909,14 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>GAMBERI ARGENTINA INTERI 800G</t>
+          <t>ANELLI CIUFFI CALAMARO PATAG. 400G</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>35.203,00</t>
+          <t>25.871,00</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -3997,14 +4931,14 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>TRANCE DI PESCE SPADA 450G</t>
+          <t>BOCCONCINI DI MARE  200G</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>24.854,00</t>
+          <t>30.865,00</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -4019,14 +4953,14 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>FILETTI DI TONNO PINNA GIALLA 225G</t>
+          <t>FILETTO MERLUZZO ALLA GRIGLIA 250G</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>26.364,00</t>
+          <t>31.078,00</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -4041,14 +4975,14 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>FISH &amp; CHIPS PASTELLATO 400G</t>
+          <t>FILETTO DI MERLUZZO CROCCANTE 400G</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>31.078,00</t>
+          <t>31.522,00</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -4063,14 +4997,14 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>FILETTO DI MERLUZZO CROCCANTE 400G</t>
+          <t>BACCALA' CON PATATE 350G</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>32.966,00</t>
+          <t>28.021,00</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -4085,14 +5019,14 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>POLPETTE MERLUZZO MEDITERRANEA 500G</t>
+          <t>PANZEROTTO ALLA PUGLIESE 250G</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>36.806,00</t>
+          <t>32.305,00</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -4107,19 +5041,19 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>PERLE DI BACCALA'IN PASTELLA 200G</t>
+          <t>PANCAKES 450G</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>35.598,00</t>
+          <t>18.380,00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -4129,14 +5063,14 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>6 BASTONCINI DI SALMONE 150G</t>
+          <t>PIZZA MARGHERITA AL TAGLIERE 220G</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>609,00</t>
+          <t>26.868,00</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -4151,19 +5085,19 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>BASTONCINI DI MERLUZZO 900G</t>
+          <t>PIZZETTE MARGHERITA 4X80G</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>18.380,00</t>
+          <t>25.820,00</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -4173,19 +5107,19 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>PIZZA FUNGHI BOSCO AL TAGLIERE 215G</t>
+          <t>SFOGLINO CARCIOFI E RICOTTA 300G</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>18.380,00</t>
+          <t>28.897,00</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -4195,14 +5129,14 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>PIZZA MARGHERITA AL TAGLIERE 220G</t>
+          <t>PANCIOTTELLI FORMAGGIO MOZZAR.250G</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>25.438,00</t>
+          <t>9.337,00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -4217,19 +5151,19 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>TRANCIO MARGHERITA 3PZ X 400G</t>
+          <t>SAUTE' DI MARE ASTUCCIO  500G</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>26.942,00</t>
+          <t>9.338,00</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -4239,14 +5173,14 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>CALZONE POMODORO MOZZARELLA  250G</t>
+          <t>SPAGHETTI ALLE VONGOLE 550G</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>23.968,00</t>
+          <t>12.654,00</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -4261,36 +5195,36 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>HAMBURGER BOVINO 10X75</t>
+          <t>GRAN SUGO ALLE COZZE  350G</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>30.344,00</t>
+          <t>12.654,00</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>GHIACCIO ALIMENTARE TRITATO 2K</t>
+          <t>GRAN SUGO AI GAMBERI 250G</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>12.165,00</t>
+          <t>9.052,00</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -4305,14 +5239,14 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>6 FRUTTA GELATA LOVING  360G</t>
+          <t>6 RICOPERTI FRAGOLA LOVING 300G</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>26.900,00</t>
+          <t>11.190,00</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -4327,14 +5261,14 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>6 BISCOTTI PANNA C/GOCCE CIOC.288G</t>
+          <t>6 COPPETTE PANNA/CIOCCOLATO 300G</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>30.760,00</t>
+          <t>22.646,00</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -4349,14 +5283,14 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>4 CONI TWIRL PANNA/CIOCC. 280G</t>
+          <t>6 BARRETTE AL COCCO 250G</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>32.200,00</t>
+          <t>30.728,00</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -4371,36 +5305,36 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>GHIACCIOLI THE AL LIMONE 6X70G</t>
+          <t>4 STECCHI MIX YOGURT GRECO 280G</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>35.560,00</t>
+          <t>32.200,00</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>4 STECCHI PISTACCHIO CIOC/B.CO 260</t>
+          <t>GHIACCIOLI THE AL LIMONE 6X70G</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1.375,00</t>
+          <t>32.200,00</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -4415,19 +5349,19 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>VASCH.STRACCIATELLA LOVING 500G</t>
+          <t>GHIACCIOLI THE ALLA PESCA 6X70G</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>33.310,00</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -4437,19 +5371,19 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>VASCHETTA PISTAC/GIANDUIA ADS 200G</t>
+          <t>4 BISCOTTI YOGURT GRECO 280G</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>27.488,00</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>9,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -4459,19 +5393,19 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>VASCHETTA PANNA COTTA ADS 200G</t>
+          <t>GELATO YOGURT GRECO AL MIELE 320G</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>18.268,00</t>
+          <t>32.300,00</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -4481,19 +5415,19 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>VASCHETTA AFFOG. AL CACAO 500G</t>
+          <t>GELATO PROTEIN GO FIT ARAGHIDI 300</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>18.295,00</t>
+          <t>32.300,00</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -4503,41 +5437,41 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>TRANCIO GRAN FRUTTA 8/10 PORZ. 700G</t>
+          <t>GELATO PROTEIN GO FIT VANIGLIA 300</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>18.295,00</t>
+          <t>1.797,00</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>TRANCIO VAR AMARENA 8/10 PORZ. 700G</t>
+          <t>PINZE GRANCHIO PANATE S/GLUT.250G</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>10.796,00</t>
+          <t>20.432,00</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -4547,7 +5481,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>HAMBURGER VEGET.MELANZANE 100G</t>
+          <t>BAST.FILETTI MERLUZZO S/GLUTINE 300</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
various fixed, new oscillation, C remake
</commit_message>
<xml_diff>
--- a/comparison_result.xlsx
+++ b/comparison_result.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,7 +480,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>37.695,00</t>
+          <t>998,00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -489,19 +489,19 @@
         </is>
       </c>
       <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>6 LEMON ICE LIQUIRIZIA LOVING 480G</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>2</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>GHIACCIOLI ASS. MULTIVIT. 560G</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>GHIACCIOLI ASS. MULTIVIT. 560G</t>
+          <t>6 LEMON ICE LIQUIRIZIA LOVING 480G</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -516,7 +516,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>33.309,00</t>
+          <t>25.272,00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -529,30 +529,30 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CONI GRANITA LIMONE/ARANCIA 6X105G</t>
+          <t>10 GHIACCIOLI LOVING 750G</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>CONI GRANITA LIMONE/ARANCIA 6X105G</t>
+          <t>10 GHIACCIOLI LOVING 750G</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>24.413,00</t>
+          <t>30.728,00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -561,23 +561,23 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>20 GHIACCIOLI 1200G</t>
+          <t>4 STECCHI MIX YOGURT GRECO 280G</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>20 GHIACCIOLI 1200G</t>
+          <t>4 STECCHI MIX YOGURT GRECO 280G</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -588,28 +588,28 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>25.272,00</t>
+          <t>35.560,00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>10 GHIACCIOLI LOVING 750G</t>
+          <t>4 STECCHI PISTACCHIO CIOC/B.CO 260</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>10 GHIACCIOLI LOVING 750G</t>
+          <t>4 STECCHI PISTACCHIO CIOC/B.CO 260</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -624,7 +624,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>998,00</t>
+          <t>24.403,00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -633,11 +633,11 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>6 LEMON ICE LIQUIRIZIA LOVING 480G</t>
+          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -645,22 +645,22 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>6 LEMON ICE LIQUIRIZIA LOVING 480G</t>
+          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>27.627,00</t>
+          <t>11.189,00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -669,34 +669,34 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>GELATO GRAN RIPIENO MIX 6PZ 360G</t>
+          <t>6 STECCHI RICOPERTI CIOCC.300G</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>GELATO GRAN RIPIENO MIX 6PZ 360G</t>
+          <t>6 STECCHI RICOPERTI CIOCC.300G</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>24.403,00</t>
+          <t>997,00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -709,30 +709,30 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
+          <t>6 PRALINATI AMARENA LOVING 360G</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
+          <t>6 PRALINATI AMARENA LOVING 360G</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>15.757,00</t>
+          <t>27.627,00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -741,34 +741,34 @@
         </is>
       </c>
       <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>GELATO GRAN RIPIENO MIX 6PZ 360G</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
         <v>2</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>4 MAXISTECCHI LOVING 350G</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>4 MAXISTECCHI LOVING 350G</t>
+          <t>GELATO GRAN RIPIENO MIX 6PZ 360G</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>997,00</t>
+          <t>9.052,00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -777,11 +777,11 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>6 PRALINATI AMARENA LOVING 360G</t>
+          <t>6 RICOPERTI FRAGOLA LOVING 300G</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -789,22 +789,22 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>6 PRALINATI AMARENA LOVING 360G</t>
+          <t>6 RICOPERTI FRAGOLA LOVING 300G</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>35.560,00</t>
+          <t>27.657,00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -817,30 +817,30 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>4 STECCHI CARAM.SALATO E CIOCC 260G</t>
+          <t>STECCO FRUIT  GR 390</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>4 STECCHI CARAM.SALATO E CIOCC 260G</t>
+          <t>STECCO FRUIT  GR 390</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1.373,00</t>
+          <t>30.345,00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -849,11 +849,11 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>8 RICOPERTI LOVING 400G</t>
+          <t>GHIACCIO ALIMENTARE CUBETTO 2K</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -861,22 +861,22 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>8 RICOPERTI LOVING 400G</t>
+          <t>GHIACCIO ALIMENTARE CUBETTO 2K</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>30.344,00</t>
+          <t>22.646,00</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -889,7 +889,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>GHIACCIO ALIMENTARE TRITATO 2K</t>
+          <t>6 BARRETTE AL COCCO 250G</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -897,7 +897,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>GHIACCIO ALIMENTARE TRITATO 2K</t>
+          <t>6 BARRETTE AL COCCO 250G</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -912,7 +912,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2.196,00</t>
+          <t>17.530,00</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -925,30 +925,30 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>8 MINISTECCHI ASSORT. LOVING 250G</t>
+          <t>6 BARRETTE GELATO PANNA E MOU 250G</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>8 MINISTECCHI ASSORT. LOVING 250G</t>
+          <t>6 BARRETTE GELATO PANNA E MOU 250G</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>17.530,00</t>
+          <t>2.196,00</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>6 BARRETTE GELATO PANNA E MOU 250G</t>
+          <t>8 MINISTECCHI ASSORT. LOVING 250G</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -969,7 +969,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>6 BARRETTE GELATO PANNA E MOU 250G</t>
+          <t>8 MINISTECCHI ASSORT. LOVING 250G</t>
         </is>
       </c>
       <c r="G15" t="n">
@@ -984,7 +984,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>9.053,00</t>
+          <t>30.344,00</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -993,34 +993,34 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>6 MINIBISCOTTI LOVING 325G</t>
+          <t>GHIACCIO ALIMENTARE TRITATO 2K</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>6 MINIBISCOTTI LOVING 325G</t>
+          <t>GHIACCIO ALIMENTARE TRITATO 2K</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2.193,00</t>
+          <t>9.053,00</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1029,27 +1029,27 @@
         </is>
       </c>
       <c r="C17" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>6 MINIBISCOTTI LOVING 325G</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
         <v>3</v>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>4 COPPA AL CAFFE' LOVING 280G</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>2</v>
-      </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>4 COPPA AL CAFFE' LOVING 280G</t>
+          <t>6 MINIBISCOTTI LOVING 325G</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
@@ -1092,7 +1092,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>13.292,00</t>
+          <t>33.310,00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1101,19 +1101,19 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>6 MAXISANDWICH LOVING  480G</t>
+          <t>4 BISCOTTI YOGURT GRECO 280G</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>6 MAXISANDWICH LOVING  480G</t>
+          <t>4 BISCOTTI YOGURT GRECO 280G</t>
         </is>
       </c>
       <c r="G19" t="n">
@@ -1128,7 +1128,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1.374,00</t>
+          <t>11.190,00</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1137,19 +1137,19 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>8 SANDWICH LOVING 400G</t>
+          <t>6 COPPETTE PANNA/CIOCCOLATO 300G</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>8 SANDWICH LOVING 400G</t>
+          <t>6 COPPETTE PANNA/CIOCCOLATO 300G</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -1164,7 +1164,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1.129,00</t>
+          <t>1.374,00</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1173,34 +1173,34 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>8 MINICONO LOVING 320G</t>
+          <t>8 SANDWICH LOVING 400G</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>8 MINICONO LOVING 320G</t>
+          <t>8 SANDWICH LOVING 400G</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>12.166,00</t>
+          <t>13.292,00</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1209,19 +1209,19 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>12 MINIMINICONI LOVING 225G</t>
+          <t>6 MAXISANDWICH LOVING  480G</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>12 MINIMINICONI LOVING 225G</t>
+          <t>6 MAXISANDWICH LOVING  480G</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -1236,7 +1236,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>17.667,00</t>
+          <t>30.760,00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>GELATI DI SOIA ASSORTITI 360G</t>
+          <t>4 CONI TWIRL PANNA/CIOCC. 280G</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>GELATI DI SOIA ASSORTITI 360G</t>
+          <t>4 CONI TWIRL PANNA/CIOCC. 280G</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1313,15 +1313,15 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>6 CONI PANNA/CIOCCOLATO 450G LOVING</t>
+          <t>6 CONI PANNA VAR.AMARENA 450G LOVIN</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -1329,15 +1329,15 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>6 CONI PANNA/CIOCCOLATO 450G LOVING</t>
+          <t>6 CONI PANNA VAR.AMARENA 450G LOVIN</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
@@ -1349,23 +1349,23 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>6 CONI PANNA VAR.AMARENA 450G LOVIN</t>
+          <t>6 CONI PANNA/CIOCCOLATO 450G LOVING</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>6 CONI PANNA VAR.AMARENA 450G LOVIN</t>
+          <t>6 CONI PANNA/CIOCCOLATO 450G LOVING</t>
         </is>
       </c>
       <c r="G26" t="n">
@@ -1389,23 +1389,23 @@
         </is>
       </c>
       <c r="C27" t="n">
+        <v>6</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>6 CONI PANNA GR 420 LOVING</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
         <v>5</v>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>6 CONI PANNA GR 420 LOVING</t>
         </is>
       </c>
-      <c r="E27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>6 CONI PANNA GR 420 LOVING</t>
-        </is>
-      </c>
       <c r="G27" t="n">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -1425,7 +1425,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1441,23 +1441,23 @@
         </is>
       </c>
       <c r="G28" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>22.645,00</t>
+          <t>9.051,00</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12 MINI BON BON PANNA/CIOCC. 110G</t>
+          <t>DESSERT VANIGLIA CACAO LOVING 320G</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1473,7 +1473,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>12 MINI BON BON PANNA/CIOCC. 110G</t>
+          <t>DESSERT VANIGLIA CACAO LOVING 320G</t>
         </is>
       </c>
       <c r="G29" t="n">
@@ -1488,7 +1488,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>32.052,00</t>
+          <t>18.294,00</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1497,11 +1497,11 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>CORNETTO CLASSICO VUOTO 4PZ 280G</t>
+          <t>TORTA GELATO S.HONORE'12/14PORZ 1KG</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1509,22 +1509,22 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>CORNETTO CLASSICO VUOTO 4PZ 280G</t>
+          <t>TORTA GELATO S.HONORE'12/14PORZ 1KG</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>18.294,00</t>
+          <t>18.295,00</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1537,23 +1537,23 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>TORTA GELATO S.HONORE'12/14PORZ 1KG</t>
+          <t>TRANCIO GRAN FRUTTA 8/10 PORZ. 700G</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>TORTA GELATO S.HONORE'12/14PORZ 1KG</t>
+          <t>TRANCIO GRAN FRUTTA 8/10 PORZ. 700G</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
@@ -1569,27 +1569,27 @@
         </is>
       </c>
       <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>TRANCIO VAR AMARENA 8/10 PORZ. 700G</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
         <v>3</v>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>TRANCIO VAR AMARENA 8/10 PORZ. 700G</t>
         </is>
       </c>
-      <c r="E32" t="n">
+      <c r="G32" t="n">
         <v>2</v>
       </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>TRANCIO VAR AMARENA 8/10 PORZ. 700G</t>
-        </is>
-      </c>
-      <c r="G32" t="n">
-        <v>-1</v>
-      </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
@@ -1632,12 +1632,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>18.269,00</t>
+          <t>602,00</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1645,7 +1645,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
+          <t>VASCHETTA VANIGLIA CACAO NOCC.1KG</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1653,7 +1653,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
+          <t>VASCHETTA VANIGLIA CACAO NOCC.1KG</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -1668,20 +1668,20 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1.375,00</t>
+          <t>18.269,00</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>VASCH.PANNA LOVING 500G</t>
+          <t>VASCHETTA ZUPPA INGLESE 1KG</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1689,22 +1689,22 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>VASCH.PANNA LOVING 500G</t>
+          <t>VASCHETTA ZUPPA INGLESE 1KG</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1.375,00</t>
+          <t>18.269,00</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1717,7 +1717,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>VASCH.STRACCIATELLA LOVING 500G</t>
+          <t>VASCHETTA NOCCIOLATO 1KG</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1725,7 +1725,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>VASCH.STRACCIATELLA LOVING 500G</t>
+          <t>VASCHETTA NOCCIOLATO 1KG</t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -1745,23 +1745,23 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>VASCHETTA AFFOG. AL CACAO 500G</t>
+          <t>VASCHETTA TIRAMISU' 500G</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>VASCHETTA AFFOG. AL CACAO 500G</t>
+          <t>VASCHETTA TIRAMISU' 500G</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -1781,15 +1781,15 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>VASCHETTA SPAGNOLA 500G</t>
+          <t>VASCHETTA YOGURT FRUTTI BOSCO 500G</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1797,15 +1797,15 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>VASCHETTA SPAGNOLA 500G</t>
+          <t>VASCHETTA YOGURT FRUTTI BOSCO 500G</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
@@ -1817,38 +1817,38 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>VASCHETTA AFFOG. CAFFE' 500G</t>
+          <t>VASCHETTA SPAGNOLA 500G</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>VASCHETTA AFFOG. CAFFE' 500G</t>
+          <t>VASCHETTA SPAGNOLA 500G</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>18.268,00</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>VASCHETTA SPAGNOLA LOVING 200G</t>
+          <t>VASCHETTA AFFOG. CAFFE' 500G</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1869,7 +1869,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>VASCHETTA SPAGNOLA LOVING 200G</t>
+          <t>VASCHETTA AFFOG. CAFFE' 500G</t>
         </is>
       </c>
       <c r="G40" t="n">
@@ -1884,20 +1884,20 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>18.268,00</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>VASCHETTA CASSATA LOVING 200G</t>
+          <t>VASCHETTA AFFOG. AL CACAO 500G</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1905,35 +1905,35 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>VASCHETTA CASSATA LOVING 200G</t>
+          <t>VASCHETTA AFFOG. AL CACAO 500G</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>27.488,00</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>VASCHETTA CAFFE'ARABICA LOVING 200G</t>
+          <t>GELATO ALLO YOGURT GRECO B.CO 320G</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -1941,15 +1941,15 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>VASCHETTA CAFFE'ARABICA LOVING 200G</t>
+          <t>GELATO ALLO YOGURT GRECO B.CO 320G</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
@@ -1961,7 +1961,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1969,7 +1969,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>VASCHETTA TRIPLO CIOCC.ADS 200G</t>
+          <t>VASCHETTA PISTAC/GIANDUIA ADS 200G</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -1977,7 +1977,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>VASCHETTA TRIPLO CIOCC.ADS 200G</t>
+          <t>VASCHETTA PISTAC/GIANDUIA ADS 200G</t>
         </is>
       </c>
       <c r="G43" t="n">
@@ -1997,15 +1997,15 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>VASCHETTA LIMONE SICILIA ADS 200G</t>
+          <t>VASCHETTA STRACCIATELLA LOVING 200G</t>
         </is>
       </c>
       <c r="E44" t="n">
@@ -2013,99 +2013,99 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>VASCHETTA LIMONE SICILIA ADS 200G</t>
+          <t>VASCHETTA STRACCIATELLA LOVING 200G</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>27.488,00</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>9,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>VASCHETTA PANNA COTTA ADS 200G</t>
+          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>VASCHETTA PANNA COTTA ADS 200G</t>
+          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>27.488,00</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>11,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C46" t="n">
+        <v>2</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>GELATO YOGURT GRECO AL MIELE 320G</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
         <v>3</v>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>VASCHETTA CARAMELLO SALATO ADS 200G</t>
-        </is>
-      </c>
-      <c r="E46" t="n">
-        <v>2</v>
-      </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>VASCHETTA CARAMELLO SALATO ADS 200G</t>
+          <t>GELATO YOGURT GRECO AL MIELE 320G</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>27.488,00</t>
+          <t>36.103,00</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -2113,35 +2113,35 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
+          <t>SORBETTO AL LIMONE LOVING 250G</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
+          <t>SORBETTO AL LIMONE LOVING 250G</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>27.488,00</t>
+          <t>1.341,00</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -2149,7 +2149,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO C/NOCCIOLA 320G</t>
+          <t>MIX DI VERDURE GRIGLIATE 450G</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -2157,7 +2157,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO C/NOCCIOLA 320G</t>
+          <t>MIX DI VERDURE GRIGLIATE 450G</t>
         </is>
       </c>
       <c r="G48" t="n">
@@ -2172,7 +2172,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>605,00</t>
+          <t>27.610,00</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2181,11 +2181,11 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>MINESTRONE 15 VERDURE 1KG</t>
+          <t>PISELLI FINISSIMI 1KG</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -2193,22 +2193,22 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>MINESTRONE 15 VERDURE 1KG</t>
+          <t>PISELLI FINISSIMI 1KG</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>604,00</t>
+          <t>765,00</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>PISELLI FINI BUSTA 1KG</t>
+          <t>FAGIOLINI INTERI FINISSIMI 1KG</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>PISELLI FINI BUSTA 1KG</t>
+          <t>FAGIOLINI INTERI FINISSIMI 1KG</t>
         </is>
       </c>
       <c r="G50" t="n">
@@ -2244,20 +2244,20 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>22.587,00</t>
+          <t>4.550,00</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>BROCCOLI A ROSETTE BONTA'ORTO 600G</t>
+          <t>PISELLI FINISSIMI BUSTA 450G</t>
         </is>
       </c>
       <c r="E51" t="n">
@@ -2265,22 +2265,22 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>BROCCOLI A ROSETTE BONTA'ORTO 600G</t>
+          <t>PISELLI FINISSIMI BUSTA 450G</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>27.609,00</t>
+          <t>604,00</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>VERDURE PER SOFFRITTO 450G</t>
+          <t>PISELLI FINI BUSTA 1KG</t>
         </is>
       </c>
       <c r="E52" t="n">
@@ -2301,7 +2301,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>VERDURE PER SOFFRITTO 450G</t>
+          <t>PISELLI FINI BUSTA 1KG</t>
         </is>
       </c>
       <c r="G52" t="n">
@@ -2316,7 +2316,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>606,00</t>
+          <t>27.609,00</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2325,34 +2325,34 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>SPINACI IN FOGLIA PORZIONATI 1KG</t>
+          <t>VERDURE PER SOFFRITTO 450G</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>SPINACI IN FOGLIA PORZIONATI 1KG</t>
+          <t>VERDURE PER SOFFRITTO 450G</t>
         </is>
       </c>
       <c r="G53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>8.490,00</t>
+          <t>606,00</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2361,19 +2361,19 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>SPINACI FOGLIA PER FOGLIA 450G</t>
+          <t>SPINACI IN FOGLIA PORZIONATI 1KG</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>SPINACI FOGLIA PER FOGLIA 450G</t>
+          <t>SPINACI IN FOGLIA PORZIONATI 1KG</t>
         </is>
       </c>
       <c r="G54" t="n">
@@ -2388,7 +2388,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>1.515,00</t>
+          <t>593,00</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>BIETA IN FOGLIA PORZIONATA 1KG</t>
+          <t>MISTO FUNGHI 300G</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -2409,7 +2409,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>BIETA IN FOGLIA PORZIONATA 1KG</t>
+          <t>MISTO FUNGHI 300G</t>
         </is>
       </c>
       <c r="G55" t="n">
@@ -2424,7 +2424,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>22.255,00</t>
+          <t>25.793,00</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>PATATE RUSTICHE PREFRITTE 1K</t>
+          <t>PATATE SPICCHI CON BUCCIA 600G</t>
         </is>
       </c>
       <c r="E56" t="n">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>PATATE RUSTICHE PREFRITTE 1K</t>
+          <t>PATATE SPICCHI CON BUCCIA 600G</t>
         </is>
       </c>
       <c r="G56" t="n">
@@ -2460,7 +2460,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>593,00</t>
+          <t>24.797,00</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2473,7 +2473,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>MISTO FUNGHI 300G</t>
+          <t>PATATE A FETTE GR 600</t>
         </is>
       </c>
       <c r="E57" t="n">
@@ -2481,7 +2481,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>MISTO FUNGHI 300G</t>
+          <t>PATATE A FETTE GR 600</t>
         </is>
       </c>
       <c r="G57" t="n">
@@ -2496,7 +2496,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>18.022,00</t>
+          <t>603,00</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2509,7 +2509,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>PATATE A SPICCHIO PREFRITTE 1KG</t>
+          <t>PATATE PREFRITTE STICK 1KG</t>
         </is>
       </c>
       <c r="E58" t="n">
@@ -2517,7 +2517,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>PATATE A SPICCHIO PREFRITTE 1KG</t>
+          <t>PATATE PREFRITTE STICK 1KG</t>
         </is>
       </c>
       <c r="G58" t="n">
@@ -2532,7 +2532,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>603,00</t>
+          <t>17.607,00</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2545,30 +2545,30 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>PATATE PREFRITTE STICK 1KG</t>
+          <t>PATATE PREFRITTE 2,5KG</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>PATATE PREFRITTE STICK 1KG</t>
+          <t>PATATE PREFRITTE 2,5KG</t>
         </is>
       </c>
       <c r="G59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>18.424,00</t>
+          <t>18.556,00</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2577,11 +2577,11 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>PATATE STICK DA FORNO 1KG</t>
+          <t>PURE'DI PATATE 600G</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -2589,22 +2589,22 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>PATATE STICK DA FORNO 1KG</t>
+          <t>PURE'DI PATATE 600G</t>
         </is>
       </c>
       <c r="G60" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>25.820,00</t>
+          <t>2.359,00</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2613,11 +2613,11 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>SFOGLINO RICOTTA E SPINACI 300G</t>
+          <t>PIZZA MARGHERITA CUCINO IO 3PZ 960G</t>
         </is>
       </c>
       <c r="E61" t="n">
@@ -2625,22 +2625,22 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>SFOGLINO RICOTTA E SPINACI 300G</t>
+          <t>PIZZA MARGHERITA CUCINO IO 3PZ 960G</t>
         </is>
       </c>
       <c r="G61" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>35.621,00</t>
+          <t>29.386,00</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2653,7 +2653,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>PIZZA SALAMINO/PROVOLONE 26X38 535G</t>
+          <t>PIZZA MARGHERITA 26X38 485G</t>
         </is>
       </c>
       <c r="E62" t="n">
@@ -2661,7 +2661,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>PIZZA SALAMINO/PROVOLONE 26X38 535G</t>
+          <t>PIZZA MARGHERITA 26X38 485G</t>
         </is>
       </c>
       <c r="G62" t="n">
@@ -2676,7 +2676,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>13.597,00</t>
+          <t>35.599,00</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2689,7 +2689,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>MISTO OLIVE/CROCC/SUPPLI/ARANC 500G</t>
+          <t>PIZZA PROSCIUTTO/FUNGHI 26X38 570G</t>
         </is>
       </c>
       <c r="E63" t="n">
@@ -2697,7 +2697,7 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>MISTO OLIVE/CROCC/SUPPLI/ARANC 500G</t>
+          <t>PIZZA PROSCIUTTO/FUNGHI 26X38 570G</t>
         </is>
       </c>
       <c r="G63" t="n">
@@ -2712,12 +2712,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>25.438,00</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -2725,7 +2725,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI PROSC.FORMAGGIO 250G</t>
+          <t>TRANCIO MARGHERITA 3PZ X 400G</t>
         </is>
       </c>
       <c r="E64" t="n">
@@ -2733,7 +2733,7 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI PROSC.FORMAGGIO 250G</t>
+          <t>TRANCIO MARGHERITA 3PZ X 400G</t>
         </is>
       </c>
       <c r="G64" t="n">
@@ -2748,12 +2748,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>31.079,00</t>
+          <t>18.380,00</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -2761,7 +2761,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>18 BASTONCINI FILETTO MERLUZZO 450G</t>
+          <t>PIZZA MARGHERITA AL TAGLIERE 220G</t>
         </is>
       </c>
       <c r="E65" t="n">
@@ -2769,7 +2769,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>18 BASTONCINI FILETTO MERLUZZO 450G</t>
+          <t>PIZZA MARGHERITA AL TAGLIERE 220G</t>
         </is>
       </c>
       <c r="G65" t="n">
@@ -2784,7 +2784,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>609,00</t>
+          <t>26.858,00</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2797,7 +2797,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>BASTONCINI DI MERLUZZO 900G</t>
+          <t>BOCCONCINI SCAMORZINE PANATE 200G</t>
         </is>
       </c>
       <c r="E66" t="n">
@@ -2805,7 +2805,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>BASTONCINI DI MERLUZZO 900G</t>
+          <t>BOCCONCINI SCAMORZINE PANATE 200G</t>
         </is>
       </c>
       <c r="G66" t="n">
@@ -2820,12 +2820,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>31.529,00</t>
+          <t>28.897,00</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>GRANFRITTO MISTO   500G</t>
+          <t>PANCIOTTELLI PROSC.FORMAGGIO 250G</t>
         </is>
       </c>
       <c r="E67" t="n">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>GRANFRITTO MISTO   500G</t>
+          <t>PANCIOTTELLI PROSC.FORMAGGIO 250G</t>
         </is>
       </c>
       <c r="G67" t="n">
@@ -2856,7 +2856,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>17.271,00</t>
+          <t>27.692,00</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2869,7 +2869,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>FILETTI DI MERLUZZO PESCARE' 600G</t>
+          <t>MIX SALATINI E PIZZETTE 400G</t>
         </is>
       </c>
       <c r="E68" t="n">
@@ -2877,7 +2877,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>FILETTI DI MERLUZZO PESCARE' 600G</t>
+          <t>MIX SALATINI E PIZZETTE 400G</t>
         </is>
       </c>
       <c r="G68" t="n">
@@ -2892,7 +2892,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>11.179,00</t>
+          <t>26.859,00</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2905,7 +2905,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>FILETTO DI PANGASIO  800G</t>
+          <t>MINI TOAST PROSCIUT/MOZZAR. 180G</t>
         </is>
       </c>
       <c r="E69" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>FILETTO DI PANGASIO  800G</t>
+          <t>MINI TOAST PROSCIUT/MOZZAR. 180G</t>
         </is>
       </c>
       <c r="G69" t="n">
@@ -2928,7 +2928,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>595,00</t>
+          <t>609,00</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2937,11 +2937,11 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>GAMBERETTI SGUSCIATI 330/300G</t>
+          <t>BASTONCINI DI MERLUZZO 900G</t>
         </is>
       </c>
       <c r="E70" t="n">
@@ -2949,22 +2949,22 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>GAMBERETTI SGUSCIATI 330/300G</t>
+          <t>BASTONCINI DI MERLUZZO 900G</t>
         </is>
       </c>
       <c r="G70" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>22.155,00</t>
+          <t>27.552,00</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>VONGOLE C/GUSCIO DEL PACIFICO 500G</t>
+          <t>FILETTO DI PLATESSA IMPANATA 300G</t>
         </is>
       </c>
       <c r="E71" t="n">
@@ -2985,7 +2985,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>VONGOLE C/GUSCIO DEL PACIFICO 500G</t>
+          <t>FILETTO DI PLATESSA IMPANATA 300G</t>
         </is>
       </c>
       <c r="G71" t="n">
@@ -3000,7 +3000,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>14.306,00</t>
+          <t>17.367,00</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -3013,7 +3013,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>GAMBERI ZUCCHINE C/POM.PESCARE'300G</t>
+          <t>CALAMARI INTERI PULITI 400G</t>
         </is>
       </c>
       <c r="E72" t="n">
@@ -3021,7 +3021,7 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>GAMBERI ZUCCHINE C/POM.PESCARE'300G</t>
+          <t>CALAMARI INTERI PULITI 400G</t>
         </is>
       </c>
       <c r="G72" t="n">
@@ -3036,12 +3036,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>12.654,00</t>
+          <t>595,00</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>GRAN SUGO SCOGLIO C/POMOD.300G</t>
+          <t>GAMBERETTI SGUSCIATI 330/300G</t>
         </is>
       </c>
       <c r="E73" t="n">
@@ -3057,7 +3057,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>GRAN SUGO SCOGLIO C/POMOD.300G</t>
+          <t>GAMBERETTI SGUSCIATI 330/300G</t>
         </is>
       </c>
       <c r="G73" t="n">
@@ -3072,20 +3072,20 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>12.654,00</t>
+          <t>1.084,00</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>GRAN SUGO AI FRUTTI DI MARE  300G</t>
+          <t>SEPPIE PULITE 400G</t>
         </is>
       </c>
       <c r="E74" t="n">
@@ -3093,27 +3093,27 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>GRAN SUGO AI FRUTTI DI MARE  300G</t>
+          <t>SEPPIE PULITE 400G</t>
         </is>
       </c>
       <c r="G74" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>12.654,00</t>
+          <t>32.045,00</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>GRAN SUGO ALLO SCOGLIO  300G</t>
+          <t>VONGOLE DEL PACIFICO C/GUSCIO 1K</t>
         </is>
       </c>
       <c r="E75" t="n">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>GRAN SUGO ALLO SCOGLIO  300G</t>
+          <t>VONGOLE DEL PACIFICO C/GUSCIO 1K</t>
         </is>
       </c>
       <c r="G75" t="n">
@@ -3144,12 +3144,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>12.654,00</t>
+          <t>22.155,00</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -3157,7 +3157,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>GRAN SUGO ALLE VONGOLE CUCINO  350G</t>
+          <t>VONGOLE C/GUSCIO DEL PACIFICO 500G</t>
         </is>
       </c>
       <c r="E76" t="n">
@@ -3165,7 +3165,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>GRAN SUGO ALLE VONGOLE CUCINO  350G</t>
+          <t>VONGOLE C/GUSCIO DEL PACIFICO 500G</t>
         </is>
       </c>
       <c r="G76" t="n">
@@ -3180,7 +3180,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>23.968,00</t>
+          <t>14.306,00</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -3193,7 +3193,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>HAMBURGER BOVINO 10X75</t>
+          <t>GAMBERI ZUCCHINE C/POM.PESCARE'300G</t>
         </is>
       </c>
       <c r="E77" t="n">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>HAMBURGER BOVINO 10X75</t>
+          <t>GAMBERI ZUCCHINE C/POM.PESCARE'300G</t>
         </is>
       </c>
       <c r="G77" t="n">
@@ -3216,7 +3216,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>35.597,00</t>
+          <t>1.505,00</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -3229,7 +3229,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>10 BASTONCINI DI VERDURE 300G</t>
+          <t>PESCE X SPAGHETTATA PESCARE'300G</t>
         </is>
       </c>
       <c r="E78" t="n">
@@ -3237,7 +3237,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>10 BASTONCINI DI VERDURE 300G</t>
+          <t>PESCE X SPAGHETTATA PESCARE'300G</t>
         </is>
       </c>
       <c r="G78" t="n">
@@ -3252,12 +3252,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>8.491,00</t>
+          <t>12.654,00</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -3265,7 +3265,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>PISELLI PROSCIUTTO/FORMAGGIO 400G</t>
+          <t>GRAN SUGO AI FRUTTI DI MARE  300G</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>PISELLI PROSCIUTTO/FORMAGGIO 400G</t>
+          <t>GRAN SUGO AI FRUTTI DI MARE  300G</t>
         </is>
       </c>
       <c r="G79" t="n">
@@ -3288,12 +3288,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>10.796,00</t>
+          <t>12.654,00</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -3301,7 +3301,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>HAMBURGER VEGET.MELANZANE 100G</t>
+          <t>GRAN SUGO AI GAMBERI 250G</t>
         </is>
       </c>
       <c r="E80" t="n">
@@ -3309,7 +3309,7 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>HAMBURGER VEGET.MELANZANE 100G</t>
+          <t>GRAN SUGO AI GAMBERI 250G</t>
         </is>
       </c>
       <c r="G80" t="n">
@@ -3324,7 +3324,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>10.796,00</t>
+          <t>26.390,00</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -3337,7 +3337,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>HAMBURGER VEGET.CARCIOFI 100G</t>
+          <t>LASAGNA ALLA BOLOGNESE GR 600</t>
         </is>
       </c>
       <c r="E81" t="n">
@@ -3345,13 +3345,85 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>HAMBURGER VEGET.CARCIOFI 100G</t>
+          <t>LASAGNA ALLA BOLOGNESE GR 600</t>
         </is>
       </c>
       <c r="G81" t="n">
         <v>0</v>
       </c>
       <c r="H81" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>35.269,00</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>1</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>BURGER VEGAN AI CECI 2X75 VERDE AMO</t>
+        </is>
+      </c>
+      <c r="E82" t="n">
+        <v>1</v>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>BURGER VEGAN AI CECI 2X75 VERDE AMO</t>
+        </is>
+      </c>
+      <c r="G82" t="n">
+        <v>0</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>10.246,00</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>1</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>SPINACI FORMAGGIO/MOZZARELLA 450G</t>
+        </is>
+      </c>
+      <c r="E83" t="n">
+        <v>1</v>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>SPINACI FORMAGGIO/MOZZARELLA 450G</t>
+        </is>
+      </c>
+      <c r="G83" t="n">
+        <v>0</v>
+      </c>
+      <c r="H83" t="inlineStr">
         <is>
           <t>Same</t>
         </is>
@@ -3368,7 +3440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3411,7 +3483,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -3445,7 +3517,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>24.359,00</t>
+          <t>24.413,00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3455,19 +3527,19 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>8 GELATINI RICOPERTI CIOCC.240G</t>
+          <t>20 GHIACCIOLI 1200G</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>30.345,00</t>
+          <t>35.560,00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3482,14 +3554,14 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>GHIACCIO ALIMENTARE CUBETTO 2K</t>
+          <t>4 STECCHI CARAM.SALATO E CIOCC 260G</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>30.760,00</t>
+          <t>24.359,00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3499,19 +3571,19 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4 CONI TWIRL PANNA/CIOCC. 280G</t>
+          <t>8 GELATINI RICOPERTI CIOCC.240G</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>35.559,00</t>
+          <t>2.193,00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3521,19 +3593,19 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>6 CONI CAFFE' 450G</t>
+          <t>4 COPPA AL CAFFE' LOVING 280G</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>32.499,00</t>
+          <t>24.401,00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -3548,36 +3620,36 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>6 CONI PANNA GR 450 LOVING ORO</t>
+          <t>4 COPPE AMARENA 350G LOVING</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>11.487,00</t>
+          <t>35.947,00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>TARTUFO AL CIOCCOLATO LOVING 2X80G</t>
+          <t>CONI PANNA S/GLUTINE 4X75G</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>24.358,00</t>
+          <t>35.559,00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -3587,90 +3659,90 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>TORTA GELATO PANNA CIOCC. 450G LOV</t>
+          <t>6 CONI CAFFE' 450G</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>9.051,00</t>
+          <t>24.358,00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>2,00</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>DESSERT VANIGLIA CACAO LOVING 320G</t>
+          <t>TORTA GELATO PANNA CIOCC. 450G LOV</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>9.051,00</t>
+          <t>11.487,00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>DESSERT CREMA CAFFE' LOVING 320G</t>
+          <t>TARTUFO AL CIOCCOLATO LOVING 2X80G</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>18.295,00</t>
+          <t>36.771,00</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>TRANCIO GRAN FRUTTA 8/10 PORZ. 700G</t>
+          <t>BABA'MIGNON RHUM 180G</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>18.269,00</t>
+          <t>9.051,00</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -3680,19 +3752,19 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>VASCHETTA NOCCIOLATO 1KG</t>
+          <t>DESSERT CREMA CAFFE' LOVING 320G</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>18.269,00</t>
+          <t>602,00</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -3702,7 +3774,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>VASCHETTA ZUPPA INGLESE 1KG</t>
+          <t>VASCHETTA CACAO STRACC.CAFFE' 1KG</t>
         </is>
       </c>
     </row>
@@ -3714,29 +3786,29 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>VASCH.CREMA/CACAO LOVING 500G</t>
+          <t>VASCH.PANNA LOVING 500G</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>18.268,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -3746,7 +3818,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>VASCHETTA TIRAMISU' 500G</t>
+          <t>VASCHETTA SPAGNOLA LOVING 200G</t>
         </is>
       </c>
     </row>
@@ -3758,29 +3830,29 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>VASCHETTA STRACCIATELLA LOVING 200G</t>
+          <t>VASCHETTA CASSATA LOVING 200G</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>36.103,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -3790,19 +3862,19 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>SORBETTO AL LIMONE LOVING 250G</t>
+          <t>VASCHETTA TRIPLO CIOCC.ADS 200G</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>766,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -3812,19 +3884,19 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>MELANZANE RONDELLE GRIGLIATE 450G</t>
+          <t>VASCHETTA LIMONE SICILIA ADS 200G</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>27.610,00</t>
+          <t>32.300,00</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -3834,14 +3906,14 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>PISELLI FINISSIMI 1KG</t>
+          <t>GELATO PROTEIN GO FIT VANIGLIA 300</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>9.298,00</t>
+          <t>33.965,00</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -3856,14 +3928,14 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>CIPOLLA TRITATA 150G</t>
+          <t>ZUCCA GIALLA IN CUBETTI 450G</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>8.399,00</t>
+          <t>2.627,00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -3873,19 +3945,19 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>ERBETTE DI CAMPO CUBETTI 450G</t>
+          <t>PREZZEMOLO TRITATO  50G</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>12.683,00</t>
+          <t>8.399,00</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -3895,19 +3967,19 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>BIETA FOGLIA X FOGLIA 450G</t>
+          <t>ERBETTE DI CAMPO CUBETTI 450G</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1.287,00</t>
+          <t>12.683,00</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3922,14 +3994,14 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>FUNGHI PORCINI CUBETTATI 300G</t>
+          <t>BIETA FOGLIA X FOGLIA 450G</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>35.774,00</t>
+          <t>1.083,00</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3944,14 +4016,14 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>PATATE A BARCHETTA 600G</t>
+          <t>CICORIA IN FOGLIA PORZIONATA 1KG</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>15.706,00</t>
+          <t>18.424,00</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3966,14 +4038,14 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>TORTINO DI PATATE 300G</t>
+          <t>PATATE STICK DA FORNO 1KG</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2.359,00</t>
+          <t>26.868,00</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -3988,14 +4060,14 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>PIZZA MARGHERITA CUCINO IO 3PZ 960G</t>
+          <t>PIZZETTE MARGHERITA 4X80G</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>18.047,00</t>
+          <t>1.500,00</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -4010,14 +4082,14 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>PIZZA 4 FORMAGGI CUCINO IO 350G</t>
+          <t>SUPPLI'DI RISO AL RAGU'500G</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>18.210,00</t>
+          <t>13.597,00</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -4032,14 +4104,14 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>PIZZA IMPERIALE VERACE 490G</t>
+          <t>MISTO OLIVE/CROCC/SUPPLI/ARANC 500G</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>18.048,00</t>
+          <t>31.079,00</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -4054,36 +4126,36 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>PIZZA TONNO CIPOLLA CUCINO IO 390G</t>
+          <t>18 BASTONCINI FILETTO MERLUZZO 450G</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>26.361,00</t>
+          <t>32.770,00</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
           <t>2,00</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>PIZZAROLLO SPINACI E RICOTTA 180GR</t>
+          <t>CUORI DI FILETTO DI NASELLO 330G</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>18.046,00</t>
+          <t>17.205,00</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -4098,19 +4170,19 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>PIZZA ALLA DIAVOLA CUCINO IO 315G</t>
+          <t>FILETTI DI BACCALA' GR 400</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>18.380,00</t>
+          <t>591,00</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -4120,14 +4192,14 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>PIZZA CON PATATE  AL TAGLIERE 200G</t>
+          <t>MERLUZZO DECAPITATO P.V. PESCARE'</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>26.231,00</t>
+          <t>36.474,00</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4142,14 +4214,14 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>PANZEROTTINI POMODORO/MOZZ.250G</t>
+          <t>CODE GAMBERI ARGENTINI SGUS.240G</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>26.860,00</t>
+          <t>1.044,00</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -4164,14 +4236,14 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>MINI HOTDOGS IN PASTA PIZZA 220G</t>
+          <t>COZZE SGUSCIATE PESCARE'250G</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>20.428,00</t>
+          <t>10.438,00</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4186,14 +4258,14 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>FILETTI BACCALA' IN PASTELLA 300G</t>
+          <t>GNOCCHETTI ALLA SORRENTINA 550G</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>15.758,00</t>
+          <t>34.018,00</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4208,14 +4280,14 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>BOCCONCINI MOZZARELLA PANATI 300G</t>
+          <t>COTOLETTE DI POLLO 2X90 G</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>32.528,00</t>
+          <t>36.486,00</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -4230,14 +4302,14 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>MOZZARELLA IN CARROZZA 4X50G</t>
+          <t>RAVIOLI DI CARNE AL VAPORE 150G</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>12.735,00</t>
+          <t>27.445,00</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4252,19 +4324,19 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>OLIVE ALL'ASCOLANA PREFRITTE 500G</t>
+          <t>INVOLTINO PRIMAVERA 180G</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>35.597,00</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -4274,359 +4346,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI SPINACI/MOZZAR.250G</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>24.442,00</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>MEDAGLIONI DI MERLUZZO 2X80G</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>24.442,00</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>MEDAGLIONI DI SALMONE 2X80G</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>27.552,00</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>FILETTO DI PLATESSA IMPANATA 300G</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>32.770,00</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>CUORI DI FILETTO DI NASELLO 330G</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>17.205,00</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>FILETTI DI BACCALA' GR 400</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>26.520,00</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>FILETTO DI SGOMBRO 600G</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>591,00</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>MERLUZZO DECAPITATO P.V. PESCARE'</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>24.854,00</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>FILETTI DI TONNO PINNA GIALLA 225G</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>1.084,00</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>SEPPIE PULITE 400G</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>23.661,00</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>ANELLI TOTANO ATLANICI  400G</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>592,00</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>MISTO DEL PESCATORE PESCARE' 300G</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>10.438,00</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>GNOCCHETTI ALLA SORRENTINA 550G</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>22.200,00</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>BUCATINI ALL'AMATRICIANA 500G</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>32.966,00</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>POLPETTE MERLUZZO MEDITERRANEA 500G</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>34.018,00</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>COTOLETTE DI POLLO 2X90 G</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>35.269,00</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>BURGER VEGAN AI CECI 2X75 VERDE AMO</t>
+          <t>10 BASTONCINI DI VERDURE 300G</t>
         </is>
       </c>
     </row>
@@ -4641,7 +4361,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4674,7 +4394,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>36.839,00</t>
+          <t>22.706,00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -4689,14 +4409,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>VELLUTATA DI ZUCCA E CAROTA 600G</t>
+          <t>MINESTRONE LEGGERO BONTA'ORTO 750G</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>17.607,00</t>
+          <t>36.839,00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -4711,14 +4431,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PATATE PREFRITTE 2,5KG</t>
+          <t>VELLUTATA DI ZUCCA E CAROTA 600G</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>8.396,00</t>
+          <t>18.022,00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -4733,14 +4453,14 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>PEPERONATA 450G</t>
+          <t>PATATE A SPICCHIO PREFRITTE 1KG</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>610,00</t>
+          <t>25.619,00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -4755,14 +4475,14 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CUORI DI CARCIOFO INTERI 450G</t>
+          <t>FAVE SURGELATE 600G</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>765,00</t>
+          <t>29.360,00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -4777,14 +4497,14 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>FAGIOLINI INTERI FINISSIMI 1KG</t>
+          <t>MIX DI CAVOLI E BROCCOLI 450G</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2.630,00</t>
+          <t>31.628,00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -4799,14 +4519,14 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>BASILICO TRITATO  50G</t>
+          <t>ROSETTE DI BROCCOLO ROMANESCO 600G</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1.505,00</t>
+          <t>1.515,00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -4821,14 +4541,14 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>PESCE X SPAGHETTATA PESCARE'300G</t>
+          <t>BIETA IN FOGLIA PORZIONATA 1KG</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>18.595,00</t>
+          <t>8.396,00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -4843,14 +4563,14 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ZUPPA DI PESCE PESCARE 800G</t>
+          <t>PEPERONATA 450G</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>27.383,00</t>
+          <t>22.587,00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -4865,14 +4585,14 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>POLPO PULITO 500G</t>
+          <t>BROCCOLI A ROSETTE BONTA'ORTO 600G</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>31.679,00</t>
+          <t>33.967,00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -4887,14 +4607,14 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>CODE MAZZANC.SCOTTATE TROPICALI200G</t>
+          <t>CARCIOFI A SPICCHI 450G BONTA DEL</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>35.681,00</t>
+          <t>18.261,00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -4909,14 +4629,14 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ANELLI CIUFFI CALAMARO PATAG. 400G</t>
+          <t>CONTORNO CAVOLO NERO TOSCANA 450G</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>25.871,00</t>
+          <t>11.129,00</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -4931,14 +4651,14 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>BOCCONCINI DI MARE  200G</t>
+          <t>MISTO SCOGLIO PESCARE' 300G</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>30.865,00</t>
+          <t>18.595,00</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -4953,14 +4673,14 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>FILETTO MERLUZZO ALLA GRIGLIA 250G</t>
+          <t>ZUPPA DI PESCE PESCARE 800G</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>31.078,00</t>
+          <t>27.383,00</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -4975,14 +4695,14 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>FILETTO DI MERLUZZO CROCCANTE 400G</t>
+          <t>POLPO PULITO 500G</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>31.522,00</t>
+          <t>28.364,00</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -4997,14 +4717,14 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>BACCALA' CON PATATE 350G</t>
+          <t>GRAN SELEZIONE FRUTTI DI MARE 600G</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>28.021,00</t>
+          <t>32.476,00</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -5019,14 +4739,14 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>PANZEROTTO ALLA PUGLIESE 250G</t>
+          <t>FILETTO DI MERLUZZO ATLANTICO 800G</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>32.305,00</t>
+          <t>25.871,00</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -5041,19 +4761,19 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>PANCAKES 450G</t>
+          <t>BOCCONCINI DI MARE  200G</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>18.380,00</t>
+          <t>1.494,00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -5063,14 +4783,14 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>PIZZA MARGHERITA AL TAGLIERE 220G</t>
+          <t>CAPRICCI DI MARE  S/GLUT. 400G</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>26.868,00</t>
+          <t>9.376,00</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -5085,19 +4805,19 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>PIZZETTE MARGHERITA 4X80G</t>
+          <t>CROCCHETTE PATATE ALLA ROMANA 500G</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>25.820,00</t>
+          <t>26.468,00</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -5107,19 +4827,19 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>SFOGLINO CARCIOFI E RICOTTA 300G</t>
+          <t>SPEEDY POLLO STICK ORIGINAL 300G</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>12.735,00</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -5129,14 +4849,14 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI FORMAGGIO MOZZAR.250G</t>
+          <t>OLIVE ALL'ASCOLANA PREFRITTE 500G</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>9.337,00</t>
+          <t>18.048,00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -5151,19 +4871,19 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>SAUTE' DI MARE ASTUCCIO  500G</t>
+          <t>PIZZA TONNO CIPOLLA CUCINO IO 390G</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>9.338,00</t>
+          <t>18.380,00</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -5173,19 +4893,19 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>SPAGHETTI ALLE VONGOLE 550G</t>
+          <t>PIZZA VERD.GRIGLIATE TAGLIERE 235G</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>12.654,00</t>
+          <t>18.380,00</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -5195,19 +4915,19 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>GRAN SUGO ALLE COZZE  350G</t>
+          <t>PIZZA INTEGRALE MARGH.TAGLIERE 220G</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>12.654,00</t>
+          <t>25.437,00</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -5217,19 +4937,19 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>GRAN SUGO AI GAMBERI 250G</t>
+          <t>PIZZA MARGHERITA 300G</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>9.052,00</t>
+          <t>28.897,00</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -5239,19 +4959,19 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>6 RICOPERTI FRAGOLA LOVING 300G</t>
+          <t>PANCIOTTELLI SPINACI/MOZZAR.250G</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>11.190,00</t>
+          <t>28.897,00</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -5261,14 +4981,14 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>6 COPPETTE PANNA/CIOCCOLATO 300G</t>
+          <t>PANCIOTTELLI FORMAGGIO MOZZAR.250G</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>22.646,00</t>
+          <t>35.854,00</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -5283,14 +5003,14 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>6 BARRETTE AL COCCO 250G</t>
+          <t>NUTELLA CROISSANT 4X85G</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>30.728,00</t>
+          <t>9.339,00</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -5305,41 +5025,41 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>4 STECCHI MIX YOGURT GRECO 280G</t>
+          <t>TAGLIATELLE AI FUNGHI  550G</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>32.200,00</t>
+          <t>12.654,00</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>GHIACCIOLI THE AL LIMONE 6X70G</t>
+          <t>GRAN SUGO ALLO SCOGLIO  300G</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>32.200,00</t>
+          <t>12.654,00</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -5349,14 +5069,14 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>GHIACCIOLI THE ALLA PESCA 6X70G</t>
+          <t>GRAN SUGO ALLE VONGOLE CUCINO  350G</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>33.310,00</t>
+          <t>1.443,00</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -5371,19 +5091,19 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>4 BISCOTTI YOGURT GRECO 280G</t>
+          <t>STRUDEL DI MELE  500G</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>27.488,00</t>
+          <t>1.129,00</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -5393,14 +5113,14 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO AL MIELE 320G</t>
+          <t>8 MINICONO LOVING 320G</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>32.300,00</t>
+          <t>1.373,00</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -5415,19 +5135,19 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>GELATO PROTEIN GO FIT ARAGHIDI 300</t>
+          <t>8 RICOPERTI LOVING 400G</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>32.300,00</t>
+          <t>26.900,00</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -5437,14 +5157,14 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>GELATO PROTEIN GO FIT VANIGLIA 300</t>
+          <t>6 BISCOTTI PANNA C/GOCCE CIOC.288G</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1.797,00</t>
+          <t>32.200,00</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -5459,19 +5179,19 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>PINZE GRANCHIO PANATE S/GLUT.250G</t>
+          <t>GHIACCIOLI THE AL LIMONE 6X70G</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20.432,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>9,00</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -5481,7 +5201,73 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>BAST.FILETTI MERLUZZO S/GLUTINE 300</t>
+          <t>VASCHETTA PANNA COTTA ADS 200G</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>27.488,00</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>GELATO YOGURT GRECO C/NOCCIOLA 320G</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>18.269,00</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>35.510,00</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>BURGER AGLI SPINACI 2X80 G</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
small post order fixes
</commit_message>
<xml_diff>
--- a/comparison_result.xlsx
+++ b/comparison_result.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -505,11 +505,11 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -541,23 +541,23 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>35.560,00</t>
+          <t>998,00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -565,7 +565,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4 STECCHI PISTACCHIO CIOC/B.CO 260</t>
+          <t>6 LEMON ICE LIQUIRIZIA LOVING 480G</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -573,7 +573,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>4 STECCHI PISTACCHIO CIOC/B.CO 260</t>
+          <t>6 LEMON ICE LIQUIRIZIA LOVING 480G</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -588,28 +588,28 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>24.403,00</t>
+          <t>35.560,00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
+          <t>4 STECCHI PISTACCHIO CIOC/B.CO 260</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
+          <t>4 STECCHI PISTACCHIO CIOC/B.CO 260</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -624,7 +624,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>15.757,00</t>
+          <t>35.560,00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -633,11 +633,11 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4 MAXISTECCHI LOVING 350G</t>
+          <t>4 STECCHI CARAM.SALATO E CIOCC 260G</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -645,22 +645,22 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>4 MAXISTECCHI LOVING 350G</t>
+          <t>4 STECCHI CARAM.SALATO E CIOCC 260G</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2.196,00</t>
+          <t>24.403,00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -669,11 +669,11 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>8 MINISTECCHI ASSORT. LOVING 250G</t>
+          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -681,22 +681,22 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>8 MINISTECCHI ASSORT. LOVING 250G</t>
+          <t>4 MAXISTECCHI MANDORLATI 320G LOVIN</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Increase</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>17.772,00</t>
+          <t>15.757,00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -705,11 +705,11 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>8 BISCOTTI TONDI VAN/CAC LOVIN.280G</t>
+          <t>4 MAXISTECCHI LOVING 350G</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -717,22 +717,22 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>8 BISCOTTI TONDI VAN/CAC LOVIN.280G</t>
+          <t>4 MAXISTECCHI LOVING 350G</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>24.402,00</t>
+          <t>27.627,00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -741,11 +741,11 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>6 CONI PANNA/CIOCCOLATO 450G LOVING</t>
+          <t>GELATO GRAN RIPIENO MIX 6PZ 360G</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -753,22 +753,22 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>6 CONI PANNA/CIOCCOLATO 450G LOVING</t>
+          <t>GELATO GRAN RIPIENO MIX 6PZ 360G</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>32.500,00</t>
+          <t>997,00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -777,19 +777,19 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>6 CONI PANNA GR 420 LOVING</t>
+          <t>6 PRALINATI AMARENA LOVING 360G</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>6 CONI PANNA GR 420 LOVING</t>
+          <t>6 PRALINATI AMARENA LOVING 360G</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -804,56 +804,56 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>18.269,00</t>
+          <t>30.345,00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
+          <t>GHIACCIO ALIMENTARE CUBETTO 2K</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
+          <t>GHIACCIO ALIMENTARE CUBETTO 2K</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>32.300,00</t>
+          <t>30.344,00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>GELATO PROTEIN GO FIT VANIGLIA 300</t>
+          <t>GHIACCIO ALIMENTARE TRITATO 2K</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -861,27 +861,27 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>GELATO PROTEIN GO FIT VANIGLIA 300</t>
+          <t>GHIACCIO ALIMENTARE TRITATO 2K</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>37.780,00</t>
+          <t>22.646,00</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -889,7 +889,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>GELATO NOCCIOLA S/LATTOSIO 250G</t>
+          <t>6 BARRETTE AL COCCO 250G</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -897,7 +897,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>GELATO NOCCIOLA S/LATTOSIO 250G</t>
+          <t>6 BARRETTE AL COCCO 250G</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -912,7 +912,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>37.780,00</t>
+          <t>17.530,00</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -925,66 +925,66 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>GELATO CIOCCOLATO S/LATTOSIO 250G</t>
+          <t>6 BARRETTE GELATO PANNA E MOU 250G</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>GELATO CIOCCOLATO S/LATTOSIO 250G</t>
+          <t>6 BARRETTE GELATO PANNA E MOU 250G</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>37.780,00</t>
+          <t>2.196,00</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>8 MINISTECCHI ASSORT. LOVING 250G</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
         <v>2</v>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>GELATO FIORDILATTE S/LATTOSIO 250G</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>1</v>
-      </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>GELATO FIORDILATTE S/LATTOSIO 250G</t>
+          <t>8 MINISTECCHI ASSORT. LOVING 250G</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>14.470,00</t>
+          <t>26.900,00</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -993,11 +993,11 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>MINESTRONE RICETTA GHIOTTA 750G</t>
+          <t>6 BISCOTTI PANNA C/GOCCE CIOC.288G</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -1005,22 +1005,22 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>MINESTRONE RICETTA GHIOTTA 750G</t>
+          <t>6 BISCOTTI PANNA C/GOCCE CIOC.288G</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>765,00</t>
+          <t>9.053,00</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1029,11 +1029,11 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>FAGIOLINI INTERI FINISSIMI 1KG</t>
+          <t>6 MINIBISCOTTI LOVING 325G</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -1041,22 +1041,22 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>FAGIOLINI INTERI FINISSIMI 1KG</t>
+          <t>6 MINIBISCOTTI LOVING 325G</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>13.249,00</t>
+          <t>2.193,00</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1065,11 +1065,11 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>TRIS DI VERDURE  600G</t>
+          <t>4 COPPA AL CAFFE' LOVING 280G</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -1077,22 +1077,22 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>TRIS DI VERDURE  600G</t>
+          <t>4 COPPA AL CAFFE' LOVING 280G</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>604,00</t>
+          <t>17.772,00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1105,30 +1105,30 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>PISELLI FINI BUSTA 1KG</t>
+          <t>8 BISCOTTI TONDI VAN/CAC LOVIN.280G</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>PISELLI FINI BUSTA 1KG</t>
+          <t>8 BISCOTTI TONDI VAN/CAC LOVIN.280G</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>9.299,00</t>
+          <t>33.310,00</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>VERDURE PER SOFFRITTO 150G</t>
+          <t>4 BISCOTTI YOGURT GRECO 280G</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>VERDURE PER SOFFRITTO 150G</t>
+          <t>4 BISCOTTI YOGURT GRECO 280G</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -1164,7 +1164,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>606,00</t>
+          <t>1.374,00</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1177,30 +1177,30 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>SPINACI IN FOGLIA PORZIONATI 1KG</t>
+          <t>8 SANDWICH LOVING 400G</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>SPINACI IN FOGLIA PORZIONATI 1KG</t>
+          <t>8 SANDWICH LOVING 400G</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>21.479,00</t>
+          <t>13.292,00</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1209,11 +1209,11 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ASPARAGI PUNTE ASTUCCIO 300G</t>
+          <t>6 MAXISANDWICH LOVING  480G</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1221,22 +1221,22 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>ASPARAGI PUNTE ASTUCCIO 300G</t>
+          <t>6 MAXISANDWICH LOVING  480G</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>593,00</t>
+          <t>30.760,00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>MISTO FUNGHI 300G</t>
+          <t>4 CONI TWIRL PANNA/CIOCC. 280G</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>MISTO FUNGHI 300G</t>
+          <t>4 CONI TWIRL PANNA/CIOCC. 280G</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1272,7 +1272,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>18.022,00</t>
+          <t>12.166,00</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>PATATE A SPICCHIO PREFRITTE 1KG</t>
+          <t>12 MINIMINICONI LOVING 225G</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>PATATE A SPICCHIO PREFRITTE 1KG</t>
+          <t>12 MINIMINICONI LOVING 225G</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -1308,7 +1308,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>25.793,00</t>
+          <t>35.559,00</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1317,34 +1317,34 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>PATATE SPICCHI CON BUCCIA 600G</t>
+          <t>6 CONI CAFFE' 450G</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>PATATE SPICCHI CON BUCCIA 600G</t>
+          <t>6 CONI CAFFE' 450G</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>603,00</t>
+          <t>24.402,00</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1353,11 +1353,11 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>PATATE PREFRITTE STICK 1KG</t>
+          <t>6 CONI PANNA/CIOCCOLATO 450G LOVING</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1365,22 +1365,22 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>PATATE PREFRITTE STICK 1KG</t>
+          <t>6 CONI PANNA/CIOCCOLATO 450G LOVING</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>17.607,00</t>
+          <t>32.500,00</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1389,34 +1389,34 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>PATATE PREFRITTE 2,5KG</t>
+          <t>6 CONI PANNA GR 420 LOVING</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>PATATE PREFRITTE 2,5KG</t>
+          <t>6 CONI PANNA GR 420 LOVING</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2.359,00</t>
+          <t>32.499,00</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1425,19 +1425,19 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>PIZZA MARGHERITA CUCINO IO 3PZ 960G</t>
+          <t>6 CONI PANNA GR 450 LOVING ORO</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>PIZZA MARGHERITA CUCINO IO 3PZ 960G</t>
+          <t>6 CONI PANNA GR 450 LOVING ORO</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -1452,20 +1452,20 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>18.048,00</t>
+          <t>9.051,00</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>PIZZA TONNO CIPOLLA CUCINO IO 390G</t>
+          <t>DESSERT VANIGLIA CACAO LOVING 320G</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1473,22 +1473,22 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>PIZZA TONNO CIPOLLA CUCINO IO 390G</t>
+          <t>DESSERT VANIGLIA CACAO LOVING 320G</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>35.621,00</t>
+          <t>18.294,00</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1497,11 +1497,11 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>PIZZA SALAMINO/PROVOLONE 26X38 535G</t>
+          <t>TORTA GELATO S.HONORE'12/14PORZ 1KG</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1509,22 +1509,22 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>PIZZA SALAMINO/PROVOLONE 26X38 535G</t>
+          <t>TORTA GELATO S.HONORE'12/14PORZ 1KG</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>26.860,00</t>
+          <t>18.295,00</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1533,11 +1533,11 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>MINI HOTDOGS IN PASTA PIZZA 220G</t>
+          <t>TRANCIO GRAN FRUTTA 8/10 PORZ. 700G</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1545,71 +1545,71 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>MINI HOTDOGS IN PASTA PIZZA 220G</t>
+          <t>TRANCIO GRAN FRUTTA 8/10 PORZ. 700G</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>-7</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1.500,00</t>
+          <t>18.295,00</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>SUPPLI'DI RISO AL RAGU'500G</t>
+          <t>TRANCIO VAR AMARENA 8/10 PORZ. 700G</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>SUPPLI'DI RISO AL RAGU'500G</t>
+          <t>TRANCIO VAR AMARENA 8/10 PORZ. 700G</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>32.821,00</t>
+          <t>18.269,00</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>FRITTELLE ALGHE DI MARE 500G CUCINO</t>
+          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1617,22 +1617,22 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>FRITTELLE ALGHE DI MARE 500G CUCINO</t>
+          <t>VASCHETTA STRACC. VAR. AMAMERA 1KG</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>13.597,00</t>
+          <t>602,00</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1645,7 +1645,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>MISTO OLIVE/CROCC/SUPPLI/ARANC 500G</t>
+          <t>VASCHETTA FRAGOLA LIMONE PESCA 1KG</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1653,7 +1653,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>MISTO OLIVE/CROCC/SUPPLI/ARANC 500G</t>
+          <t>VASCHETTA FRAGOLA LIMONE PESCA 1KG</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -1668,20 +1668,20 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>12.735,00</t>
+          <t>602,00</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>OLIVE ALL'ASCOLANA PREFRITTE 500G</t>
+          <t>VASCHETTA VANIGLIA CACAO NOCC.1KG</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1689,27 +1689,27 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>OLIVE ALL'ASCOLANA PREFRITTE 500G</t>
+          <t>VASCHETTA VANIGLIA CACAO NOCC.1KG</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Decrease</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>26.859,00</t>
+          <t>18.269,00</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1717,35 +1717,35 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>MINI TOAST PROSCIUT/MOZZAR. 180G</t>
+          <t>VASCHETTA NOCCIOLATO 1KG</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>MINI TOAST PROSCIUT/MOZZAR. 180G</t>
+          <t>VASCHETTA NOCCIOLATO 1KG</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>27.692,00</t>
+          <t>18.268,00</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1753,35 +1753,35 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>MIX SALATINI E PIZZETTE 400G</t>
+          <t>VASCHETTA SPAGNOLA 500G</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>MIX SALATINI E PIZZETTE 400G</t>
+          <t>VASCHETTA SPAGNOLA 500G</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Decrease</t>
+          <t>Same</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>18.268,00</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1789,30 +1789,30 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI SPINACI/MOZZAR.250G</t>
+          <t>VASCHETTA YOGURT FRUTTI BOSCO 500G</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI SPINACI/MOZZAR.250G</t>
+          <t>VASCHETTA YOGURT FRUTTI BOSCO 500G</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>26.364,00</t>
+          <t>1.375,00</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1825,7 +1825,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>FISH &amp; CHIPS PASTELLATO 400G</t>
+          <t>VASCH.PANNA LOVING 500G</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -1833,7 +1833,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>FISH &amp; CHIPS PASTELLATO 400G</t>
+          <t>VASCH.PANNA LOVING 500G</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -1848,12 +1848,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>25.872,00</t>
+          <t>1.375,00</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>GRANFRITTO DI MARE 300G</t>
+          <t>VASCH.STRACCIATELLA LOVING 500G</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1869,7 +1869,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>GRANFRITTO DI MARE 300G</t>
+          <t>VASCH.STRACCIATELLA LOVING 500G</t>
         </is>
       </c>
       <c r="G40" t="n">
@@ -1884,7 +1884,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>26.230,00</t>
+          <t>18.268,00</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1897,35 +1897,35 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>ALICI DEL MEDITERRANEO PANATE 200G</t>
+          <t>VASCHETTA TIRAMISU' 500G</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>ALICI DEL MEDITERRANEO PANATE 200G</t>
+          <t>VASCHETTA TIRAMISU' 500G</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>17.205,00</t>
+          <t>18.268,00</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1933,7 +1933,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>FILETTI DI BACCALA' GR 400</t>
+          <t>VASCHETTA AFFOG. AL CACAO 500G</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>FILETTI DI BACCALA' GR 400</t>
+          <t>VASCHETTA AFFOG. AL CACAO 500G</t>
         </is>
       </c>
       <c r="G42" t="n">
@@ -1956,7 +1956,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>595,00</t>
+          <t>27.488,00</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1969,35 +1969,35 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>GAMBERETTI SGUSCIATI 330/300G</t>
+          <t>GELATO ALLO YOGURT GRECO B.CO 320G</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>GAMBERETTI SGUSCIATI 330/300G</t>
+          <t>GELATO ALLO YOGURT GRECO B.CO 320G</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Same</t>
+          <t>Increase</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1.044,00</t>
+          <t>27.488,00</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -2005,7 +2005,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>COZZE SGUSCIATE PESCARE'250G</t>
+          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
         </is>
       </c>
       <c r="E44" t="n">
@@ -2013,7 +2013,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>COZZE SGUSCIATE PESCARE'250G</t>
+          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
         </is>
       </c>
       <c r="G44" t="n">
@@ -2028,12 +2028,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>12.654,00</t>
+          <t>27.488,00</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -2041,7 +2041,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>GRAN SUGO SCOGLIO C/POMOD.300G</t>
+          <t>GELATO YOGURT GRECO C/NOCCIOLA 320G</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -2049,7 +2049,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>GRAN SUGO SCOGLIO C/POMOD.300G</t>
+          <t>GELATO YOGURT GRECO C/NOCCIOLA 320G</t>
         </is>
       </c>
       <c r="G45" t="n">
@@ -2064,7 +2064,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>12.654,00</t>
+          <t>27.488,00</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2077,7 +2077,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>GRAN SUGO ALLO SCOGLIO  300G</t>
+          <t>GELATO YOGURT GRECO AL MIELE 320G</t>
         </is>
       </c>
       <c r="E46" t="n">
@@ -2085,7 +2085,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>GRAN SUGO ALLO SCOGLIO  300G</t>
+          <t>GELATO YOGURT GRECO AL MIELE 320G</t>
         </is>
       </c>
       <c r="G46" t="n">
@@ -2100,12 +2100,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>22.202,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -2113,7 +2113,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>PENNETTE SALMONE E GAMBERI 600G</t>
+          <t>VASCHETTA SPAGNOLA LOVING 200G</t>
         </is>
       </c>
       <c r="E47" t="n">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>PENNETTE SALMONE E GAMBERI 600G</t>
+          <t>VASCHETTA SPAGNOLA LOVING 200G</t>
         </is>
       </c>
       <c r="G47" t="n">
@@ -2136,12 +2136,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>36.486,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -2149,7 +2149,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>RAVIOLI DI CARNE AL VAPORE 150G</t>
+          <t>VASCHETTA CASSATA LOVING 200G</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -2157,7 +2157,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>RAVIOLI DI CARNE AL VAPORE 150G</t>
+          <t>VASCHETTA CASSATA LOVING 200G</t>
         </is>
       </c>
       <c r="G48" t="n">
@@ -2172,12 +2172,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>9.341,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -2185,7 +2185,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>LINGUINE ALLO SCOGLIO  550G</t>
+          <t>VASCHETTA PISTAC/GIANDUIA ADS 200G</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -2193,7 +2193,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>LINGUINE ALLO SCOGLIO  550G</t>
+          <t>VASCHETTA PISTAC/GIANDUIA ADS 200G</t>
         </is>
       </c>
       <c r="G49" t="n">
@@ -2208,12 +2208,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>30.343,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>SPEEDY ALETTE CROCCANTI 360G</t>
+          <t>VASCHETTA TRIPLO CIOCC.ADS 200G</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>SPEEDY ALETTE CROCCANTI 360G</t>
+          <t>VASCHETTA TRIPLO CIOCC.ADS 200G</t>
         </is>
       </c>
       <c r="G50" t="n">
@@ -2244,7 +2244,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>35.597,00</t>
+          <t>766,00</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2257,7 +2257,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>10 BASTONCINI DI VERDURE 300G</t>
+          <t>MELANZANE RONDELLE GRIGLIATE 450G</t>
         </is>
       </c>
       <c r="E51" t="n">
@@ -2265,13 +2265,1093 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>10 BASTONCINI DI VERDURE 300G</t>
+          <t>MELANZANE RONDELLE GRIGLIATE 450G</t>
         </is>
       </c>
       <c r="G51" t="n">
         <v>0</v>
       </c>
       <c r="H51" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>1.341,00</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>1</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>MIX DI VERDURE GRIGLIATE 450G</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>1</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>MIX DI VERDURE GRIGLIATE 450G</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>22.587,00</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>1</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>BROCCOLI A ROSETTE BONTA'ORTO 600G</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>1</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>BROCCOLI A ROSETTE BONTA'ORTO 600G</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>604,00</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>2</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>PISELLI FINI BUSTA 1KG</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>1</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>PISELLI FINI BUSTA 1KG</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Decrease</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>606,00</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>6</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>SPINACI IN FOGLIA PORZIONATI 1KG</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>3</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>SPINACI IN FOGLIA PORZIONATI 1KG</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>-3</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Decrease</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>17.518,00</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>MISTO BOSCO C/PORCINI GR 1000</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>1</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>MISTO BOSCO C/PORCINI GR 1000</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>22.255,00</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>1</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>PATATE RUSTICHE PREFRITTE 1K</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>1</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>PATATE RUSTICHE PREFRITTE 1K</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>18.022,00</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>1</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>PATATE A SPICCHIO PREFRITTE 1KG</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>1</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>PATATE A SPICCHIO PREFRITTE 1KG</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>603,00</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>1</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>PATATE PREFRITTE STICK 1KG</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>2</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>PATATE PREFRITTE STICK 1KG</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>1</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Increase</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2.359,00</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>1</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>PIZZA MARGHERITA CUCINO IO 3PZ 960G</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>1</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>PIZZA MARGHERITA CUCINO IO 3PZ 960G</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>29.386,00</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>PIZZA MARGHERITA 26X38 485G</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>1</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>PIZZA MARGHERITA 26X38 485G</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>35.599,00</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>1</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>PIZZA PROSCIUTTO/FUNGHI 26X38 570G</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>1</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>PIZZA PROSCIUTTO/FUNGHI 26X38 570G</t>
+        </is>
+      </c>
+      <c r="G62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>20.429,00</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>1</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>FIORI DI ZUCCA IN PASTELLA 300G</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>1</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>FIORI DI ZUCCA IN PASTELLA 300G</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>12.735,00</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>1</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>OLIVE ALL'ASCOLANA PREFRITTE 500G</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>1</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>OLIVE ALL'ASCOLANA PREFRITTE 500G</t>
+        </is>
+      </c>
+      <c r="G64" t="n">
+        <v>0</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>1.797,00</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>1</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>PINZE GRANCHIO PANATE S/GLUT.250G</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>PINZE GRANCHIO PANATE S/GLUT.250G</t>
+        </is>
+      </c>
+      <c r="G65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>28.897,00</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>1</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>PANCIOTTELLI PROSC.FORMAGGIO 250G</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>1</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>PANCIOTTELLI PROSC.FORMAGGIO 250G</t>
+        </is>
+      </c>
+      <c r="G66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>31.079,00</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>1</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>18 BASTONCINI FILETTO MERLUZZO 450G</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>18 BASTONCINI FILETTO MERLUZZO 450G</t>
+        </is>
+      </c>
+      <c r="G67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>31.078,00</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>1</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>FILETTO DI MERLUZZO CROCCANTE 400G</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>FILETTO DI MERLUZZO CROCCANTE 400G</t>
+        </is>
+      </c>
+      <c r="G68" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>12.208,00</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>1</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>4 PORZIONI DI MERLUZZO PESCARE'400G</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>1</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>4 PORZIONI DI MERLUZZO PESCARE'400G</t>
+        </is>
+      </c>
+      <c r="G69" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>1.494,00</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>1</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>CAPRICCI DI MARE  S/GLUT. 400G</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>CAPRICCI DI MARE  S/GLUT. 400G</t>
+        </is>
+      </c>
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>33.120,00</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>1</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>NUGGETS DI MERLUZZO GRATINATI 225G</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>1</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>NUGGETS DI MERLUZZO GRATINATI 225G</t>
+        </is>
+      </c>
+      <c r="G71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>33.224,00</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>1</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>ARROSTICINI DI TOTANO PANATI 280G</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>1</v>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>ARROSTICINI DI TOTANO PANATI 280G</t>
+        </is>
+      </c>
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>26.090,00</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>1</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>FILETTI DI ORATA PESCARE' 400G</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>1</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>FILETTI DI ORATA PESCARE' 400G</t>
+        </is>
+      </c>
+      <c r="G73" t="n">
+        <v>0</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>12.654,00</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>6,00</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>1</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>GRAN SUGO SCOGLIO C/POMOD.300G</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>2</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>GRAN SUGO SCOGLIO C/POMOD.300G</t>
+        </is>
+      </c>
+      <c r="G74" t="n">
+        <v>1</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Increase</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>12.654,00</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>1</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>GRAN SUGO ALLO SCOGLIO  300G</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>3</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>GRAN SUGO ALLO SCOGLIO  300G</t>
+        </is>
+      </c>
+      <c r="G75" t="n">
+        <v>2</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Increase</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>9.341,00</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>1</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>LINGUINE ALLO SCOGLIO  550G</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>1</v>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>LINGUINE ALLO SCOGLIO  550G</t>
+        </is>
+      </c>
+      <c r="G76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>10.438,00</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>1</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>GNOCCHETTI ALLA SORRENTINA 550G</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>1</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>GNOCCHETTI ALLA SORRENTINA 550G</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
+        <v>0</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>9.338,00</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>1</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>SPAGHETTI ALLE VONGOLE 550G</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>1</v>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>SPAGHETTI ALLE VONGOLE 550G</t>
+        </is>
+      </c>
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>9.339,00</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>1</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>TAGLIATELLE AI FUNGHI  550G</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>1</v>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>TAGLIATELLE AI FUNGHI  550G</t>
+        </is>
+      </c>
+      <c r="G79" t="n">
+        <v>0</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>10.246,00</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>1</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>SPINACI FORMAGGIO/MOZZARELLA 450G</t>
+        </is>
+      </c>
+      <c r="E80" t="n">
+        <v>1</v>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>SPINACI FORMAGGIO/MOZZARELLA 450G</t>
+        </is>
+      </c>
+      <c r="G80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Same</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>25.748,00</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>1</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>GAMBERI ARGENTINA INTERI 800G</t>
+        </is>
+      </c>
+      <c r="E81" t="n">
+        <v>1</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>GAMBERI ARGENTINA INTERI 800G</t>
+        </is>
+      </c>
+      <c r="G81" t="n">
+        <v>0</v>
+      </c>
+      <c r="H81" t="inlineStr">
         <is>
           <t>Same</t>
         </is>
@@ -2288,7 +3368,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2331,7 +3411,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2343,7 +3423,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>21.822,00</t>
+          <t>21.824,00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2358,19 +3438,19 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>BAGUETTE 5 CEREALI COTTE 240G</t>
+          <t>DEMI BAGUETTE CLASSICA COTTA 140G</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>32.200,00</t>
+          <t>26.590,00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2380,7 +3460,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>GHIACCIOLI THE ALLA PESCA 6X70G</t>
+          <t>RUSTICHETTA SEMOLA RIMAC. 0,150</t>
         </is>
       </c>
     </row>
@@ -2397,7 +3477,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2419,7 +3499,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2431,7 +3511,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>998,00</t>
+          <t>24.359,00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2441,19 +3521,19 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>6 LEMON ICE LIQUIRIZIA LOVING 480G</t>
+          <t>8 GELATINI RICOPERTI CIOCC.240G</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>24.359,00</t>
+          <t>1.373,00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2468,14 +3548,14 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>8 GELATINI RICOPERTI CIOCC.240G</t>
+          <t>8 RICOPERTI LOVING 400G</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>35.560,00</t>
+          <t>24.401,00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2490,14 +3570,14 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4 STECCHI CARAM.SALATO E CIOCC 260G</t>
+          <t>4 COPPE AMARENA 350G LOVING</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>11.189,00</t>
+          <t>13.554,00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2512,19 +3592,19 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>6 STECCHI RICOPERTI CIOCC.300G</t>
+          <t>6 GRANCONO MIX LOVING 450G</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>30.344,00</t>
+          <t>24.402,00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -2534,29 +3614,29 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>GHIACCIO ALIMENTARE TRITATO 2K</t>
+          <t>6 CONI PANNA VAR.AMARENA 450G LOVIN</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>9.053,00</t>
+          <t>11.487,00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>6 MINIBISCOTTI LOVING 325G</t>
+          <t>TARTUFO AL CIOCCOLATO LOVING 2X80G</t>
         </is>
       </c>
     </row>
@@ -2595,7 +3675,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -2612,39 +3692,39 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>2,00</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>DESSERT VANIGLIA CACAO LOVING 320G</t>
+          <t>DESSERT CREMA CAFFE' LOVING 320G</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>18.269,00</t>
+          <t>602,00</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>VASCHETTA ZUPPA INGLESE 1KG</t>
+          <t>VASCHETTA CACAO STRACC.CAFFE' 1KG</t>
         </is>
       </c>
     </row>
@@ -2656,51 +3736,51 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>VASCHETTA NOCCIOLATO 1KG</t>
+          <t>VASCHETTA ZUPPA INGLESE 1KG</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>602,00</t>
+          <t>18.268,00</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>VASCHETTA CACAO STRACC.CAFFE' 1KG</t>
+          <t>VASCHETTA AFFOG. CAFFE' 500G</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>602,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -2710,14 +3790,14 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>VASCHETTA VANIGLIA CACAO NOCC.1KG</t>
+          <t>VASCHETTA CAFFE'ARABICA LOVING 200G</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>602,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2732,29 +3812,29 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>VASCHETTA FRAGOLA LIMONE PESCA 1KG</t>
+          <t>VASCHETTA STRACCIATELLA LOVING 200G</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1.375,00</t>
+          <t>12.167,00</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>VASCH.PANNA LOVING 500G</t>
+          <t>VASCHETTA LIMONE SICILIA ADS 200G</t>
         </is>
       </c>
     </row>
@@ -2766,7 +3846,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>9,00</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2776,7 +3856,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>VASCHETTA CASSATA LOVING 200G</t>
+          <t>VASCHETTA PANNA COTTA ADS 200G</t>
         </is>
       </c>
     </row>
@@ -2788,7 +3868,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>11,00</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2798,19 +3878,19 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>VASCHETTA CAFFE'ARABICA LOVING 200G</t>
+          <t>VASCHETTA CARAMELLO SALATO ADS 200G</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>4.550,00</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2820,19 +3900,19 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>VASCHETTA STRACCIATELLA LOVING 200G</t>
+          <t>PISELLI FINISSIMI BUSTA 450G</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>27.610,00</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -2842,36 +3922,36 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>VASCHETTA TRIPLO CIOCC.ADS 200G</t>
+          <t>PISELLI FINISSIMI 1KG</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>8.399,00</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>11,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>VASCHETTA CARAMELLO SALATO ADS 200G</t>
+          <t>ERBETTE DI CAMPO CUBETTI 450G</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>605,00</t>
+          <t>607,00</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2886,14 +3966,14 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>MINESTRONE 15 VERDURE 1KG</t>
+          <t>FUNGHI CHAMPIGNON A FETTE 450G</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>33.046,00</t>
+          <t>26.074,00</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2908,14 +3988,14 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>ZUPPA PRONTA CEREALI/LEG.BIO 600G</t>
+          <t>MISTO FUNGHI TRIFOLATI 300G</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>10.562,00</t>
+          <t>18.424,00</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2930,14 +4010,14 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>ZUCCHINE A CUBETTI 450G</t>
+          <t>PATATE STICK DA FORNO 1KG</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>33.966,00</t>
+          <t>24.166,00</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2952,14 +4032,14 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>FRIARIELLI IN CUBETTI 450G BONT.</t>
+          <t>MIX 5 VERDURE PASTELLATE 300G</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>11.536,00</t>
+          <t>23.988,00</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2974,19 +4054,19 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>VERZA A CUBETTONI 450G</t>
+          <t>MIX DI MINI ARANCINI 300G</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>4.550,00</t>
+          <t>36.863,00</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2996,14 +4076,14 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>PISELLI FINISSIMI BUSTA 450G</t>
+          <t>MEDAGLIONI FILETTO  MERLUZZO 500G</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>31.628,00</t>
+          <t>591,00</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3018,14 +4098,14 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>ROSETTE DI BROCCOLO ROMANESCO 600G</t>
+          <t>MERLUZZO DECAPITATO P.V. PESCARE'</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2.627,00</t>
+          <t>35.203,00</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3040,14 +4120,14 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>PREZZEMOLO TRITATO  50G</t>
+          <t>TRANCE DI PESCE SPADA 450G</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>27.609,00</t>
+          <t>26.390,00</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3062,14 +4142,14 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>VERDURE PER SOFFRITTO 450G</t>
+          <t>LASAGNA ALLA BOLOGNESE GR 600</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>8.399,00</t>
+          <t>36.090,00</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3084,14 +4164,14 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>ERBETTE DI CAMPO CUBETTI 450G</t>
+          <t>CORDON BLEU DI POLLO 360G</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>31.404,00</t>
+          <t>37.307,00</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3106,535 +4186,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>BIETOLINE COLORATE IN FOGLIA 450G</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>1.515,00</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>BIETA IN FOGLIA PORZIONATA 1KG</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>25.765,00</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>CARCIOFI CON GAMBO 450G</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>1.287,00</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>FUNGHI PORCINI CUBETTATI 300G</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>35.774,00</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>PATATE A BARCHETTA 600G</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>18.424,00</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>PATATE STICK DA FORNO 1KG</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>25.437,00</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>PIZZA MARGHERITA 300G</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>18.047,00</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>PIZZA 4 FORMAGGI CUCINO IO 350G</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>29.386,00</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>PIZZA MARGHERITA 26X38 485G</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>26.186,00</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>PIZZA MARGHERITA S/GLUTINE 300G</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>18.380,00</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>4,00</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>PIZZA MARGHERITA AL TAGLIERE 220G</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>32.528,00</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>MOZZARELLA IN CARROZZA 4X50G</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>28.897,00</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>5,00</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>PANCIOTTELLI FORMAGGIO MOZZAR.250G</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>28.897,00</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>3,00</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>PANCIOTTELLI AI FUNGHI 250G</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>24.442,00</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>MEDAGLIONI DI MERLUZZO 2X80G</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>27.552,00</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>FILETTO DI PLATESSA IMPANATA 300G</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>32.770,00</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>2,00</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>CUORI DI FILETTO DI NASELLO 330G</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>591,00</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>MERLUZZO DECAPITATO P.V. PESCARE'</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>32.045,00</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>VONGOLE DEL PACIFICO C/GUSCIO 1K</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>36.474,00</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>CODE GAMBERI ARGENTINI SGUS.240G</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>592,00</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>MISTO DEL PESCATORE PESCARE' 300G</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>37.582,00</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>GHIOZA DI GAMBERI 300G</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>36.090,00</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>CORDON BLEU DI POLLO 360G</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>34.018,00</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>COTOLETTE DI POLLO 2X90 G</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>37.769,00</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>1,00</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>NUGGETS DI POLLO 300G</t>
+          <t>COTOLETTE DI POLLO 2X110 CUCINO IO</t>
         </is>
       </c>
     </row>
@@ -3704,12 +4256,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>36.839,00</t>
+          <t>29.360,00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -3719,14 +4271,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>VELLUTATA DI VERDURE  600G</t>
+          <t>MIX DI CAVOLI E BROCCOLI 450G</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>29.360,00</t>
+          <t>593,00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3741,14 +4293,14 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>MIX DI CAVOLI E BROCCOLI 450G</t>
+          <t>MISTO FUNGHI 300G</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>17.518,00</t>
+          <t>765,00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3763,7 +4315,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>MISTO BOSCO C/PORCINI GR 1000</t>
+          <t>FAGIOLINI INTERI FINISSIMI 1KG</t>
         </is>
       </c>
     </row>
@@ -3792,7 +4344,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>18.261,00</t>
+          <t>2.630,00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3807,14 +4359,14 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CONTORNO CAVOLO NERO TOSCANA 450G</t>
+          <t>BASILICO TRITATO  50G</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1.505,00</t>
+          <t>18.261,00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -3829,14 +4381,14 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>PESCE X SPAGHETTATA PESCARE'300G</t>
+          <t>CONTORNO CAVOLO NERO TOSCANA 450G</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>26.091,00</t>
+          <t>1.084,00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -3851,14 +4403,14 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>FILETTO DI BRANZINO PESCARE' 400G</t>
+          <t>SEPPIE PULITE 400G</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>26.620,00</t>
+          <t>14.306,00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -3873,14 +4425,14 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>TRANCI DI VERDESCA S/P 500G</t>
+          <t>GAMBERI ZUCCHINE C/POM.PESCARE'300G</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>27.383,00</t>
+          <t>17.205,00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -3895,14 +4447,14 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>POLPO PULITO 500G</t>
+          <t>FILETTI DI BACCALA' GR 400</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>30.865,00</t>
+          <t>26.091,00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -3917,14 +4469,14 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>FILETTO MERLUZZO ALLA GRIGLIA 250G</t>
+          <t>FILETTO DI BRANZINO PESCARE' 400G</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>31.077,00</t>
+          <t>26.620,00</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -3939,19 +4491,19 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>FIL.MERLUZZO GRATINATO LIM/PREZ.40</t>
+          <t>TRANCI DI VERDESCA S/P 500G</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>31.077,00</t>
+          <t>27.383,00</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -3961,14 +4513,14 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>FIL.MERLUZZO GRATINATO POM/BAS.400</t>
+          <t>POLPO PULITO 500G</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>33.120,00</t>
+          <t>1.044,00</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -3983,14 +4535,14 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>NUGGETS DI MERLUZZO GRATINATI 225G</t>
+          <t>COZZE SGUSCIATE PESCARE'250G</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20.429,00</t>
+          <t>25.872,00</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -4005,14 +4557,14 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>FIORI DI ZUCCA IN PASTELLA 300G</t>
+          <t>GRANFRITTO DI MARE 300G</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>35.598,00</t>
+          <t>27.552,00</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -4027,14 +4579,14 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>6 BASTONCINI DI SALMONE 150G</t>
+          <t>FILETTO DI PLATESSA IMPANATA 300G</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>31.079,00</t>
+          <t>31.077,00</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -4049,14 +4601,14 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>18 BASTONCINI FILETTO MERLUZZO 450G</t>
+          <t>FIL.MERLUZZO GRATINATO LIM/PREZ.40</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>15.758,00</t>
+          <t>35.598,00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -4071,14 +4623,14 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>BOCCONCINI MOZZARELLA PANATI 300G</t>
+          <t>6 BASTONCINI DI SALMONE 150G</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>22.076,00</t>
+          <t>609,00</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -4093,14 +4645,14 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>MISTO FRUTTI DI BOSCO 300G</t>
+          <t>BASTONCINI DI MERLUZZO 900G</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>18.380,00</t>
+          <t>9.376,00</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -4115,14 +4667,14 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>PIZZA FUNGHI BOSCO AL TAGLIERE 215G</t>
+          <t>CROCCHETTE PATATE ALLA ROMANA 500G</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>25.438,00</t>
+          <t>13.597,00</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -4137,14 +4689,14 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>TRANCIO MARGHERITA 3PZ X 400G</t>
+          <t>MISTO OLIVE/CROCC/SUPPLI/ARANC 500G</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2.181,00</t>
+          <t>26.859,00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -4159,14 +4711,14 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>HAMBURGER BOVINO  320G CUCINO IO</t>
+          <t>MINI TOAST PROSCIUT/MOZZAR. 180G</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>22.200,00</t>
+          <t>26.860,00</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -4181,14 +4733,14 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>BUCATINI ALL'AMATRICIANA 500G</t>
+          <t>MINI HOTDOGS IN PASTA PIZZA 220G</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>18.380,00</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -4203,19 +4755,19 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI ALLA PIZZAIOLA 250G</t>
+          <t>PIZZA FUNGHI BOSCO AL TAGLIERE 215G</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>28.897,00</t>
+          <t>25.438,00</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -4225,14 +4777,14 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>PANCIOTTELLI PROSC.FORMAGGIO 250G</t>
+          <t>TRANCIO MARGHERITA 3PZ X 400G</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>9.338,00</t>
+          <t>26.868,00</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -4247,19 +4799,19 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>SPAGHETTI ALLE VONGOLE 550G</t>
+          <t>PIZZETTE MARGHERITA 4X80G</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>12.654,00</t>
+          <t>2.181,00</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -4269,14 +4821,14 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>GRAN SUGO AI FRUTTI DI MARE  300G</t>
+          <t>HAMBURGER BOVINO  320G CUCINO IO</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1.443,00</t>
+          <t>22.200,00</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -4291,14 +4843,14 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>STRUDEL DI MELE  500G</t>
+          <t>BUCATINI ALL'AMATRICIANA 500G</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>26.900,00</t>
+          <t>35.854,00</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -4313,14 +4865,14 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>6 BISCOTTI PANNA C/GOCCE CIOC.288G</t>
+          <t>NUTELLA CROISSANT 4X85G</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>27.627,00</t>
+          <t>32.265,00</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -4335,19 +4887,19 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>GELATO GRAN RIPIENO MIX 6PZ 360G</t>
+          <t>POLLO E PATATE ALLA DIAVOLA 400G</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>32.200,00</t>
+          <t>12.654,00</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -4357,19 +4909,19 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>GHIACCIOLI THE AL LIMONE 6X70G</t>
+          <t>GRAN SUGO AI FRUTTI DI MARE  300G</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>12.167,00</t>
+          <t>12.654,00</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -4379,19 +4931,19 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>VASCHETTA PISTAC/GIANDUIA ADS 200G</t>
+          <t>GRAN SUGO ALLE VONGOLE CUCINO  350G</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>27.488,00</t>
+          <t>12.654,00</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>5,00</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -4401,19 +4953,19 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>GELATO ALLO YOGURT GRECO B.CO 320G</t>
+          <t>GRAN SUGO AI GAMBERI 250G</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>27.488,00</t>
+          <t>1.443,00</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -4423,41 +4975,41 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO C/AMAREMA 320G</t>
+          <t>STRUDEL DI MELE  500G</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>27.488,00</t>
+          <t>37.582,00</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO AL MIELE 320G</t>
+          <t>GHIOZA DI GAMBERI 300G</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>27.488,00</t>
+          <t>11.190,00</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>5,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -4467,14 +5019,14 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>GELATO YOGURT GRECO C/NOCCIOLA 320G</t>
+          <t>6 COPPETTE PANNA/CIOCCOLATO 300G</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>18.268,00</t>
+          <t>22.645,00</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4489,19 +5041,19 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>VASCHETTA TIRAMISU' 500G</t>
+          <t>12 MINI BON BON PANNA/CIOCC. 110G</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>18.268,00</t>
+          <t>30.728,00</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -4511,14 +5063,14 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>VASCHETTA SPAGNOLA 500G</t>
+          <t>4 STECCHI MIX YOGURT GRECO 280G</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>18.295,00</t>
+          <t>32.200,00</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4528,46 +5080,46 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>TRANCIO GRAN FRUTTA 8/10 PORZ. 700G</t>
+          <t>GHIACCIOLI THE AL LIMONE 6X70G</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>18.295,00</t>
+          <t>33.309,00</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>3,00</t>
+          <t>1,00</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>TRANCIO VAR AMARENA 8/10 PORZ. 700G</t>
+          <t>CONI GRANITA LIMONE/ARANCIA 6X105G</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>32.300,00</t>
+          <t>1.375,00</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>7,00</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -4577,19 +5129,19 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>GELATO PROTEIN GO FIT ARAGHIDI 300</t>
+          <t>VASCH.CREMA LOVING 500G</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>35.624,00</t>
+          <t>32.300,00</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,00</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -4599,14 +5151,14 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>MINIBURGER ALLE VERDURE GRIGL.160G</t>
+          <t>GELATO PROTEIN GO FIT VANIGLIA 300</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>4.668,00</t>
+          <t>18.049,00</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -4621,14 +5173,14 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>BAST.SAPORE GRANCHIO S/GLUTINE 250G</t>
+          <t>PIZZA VEGETALE/VEGAN CUCINO IO 325G</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>35.947,00</t>
+          <t>4.668,00</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -4643,7 +5195,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>CONI PANNA S/GLUTINE 4X75G</t>
+          <t>BAST.SAPORE GRANCHIO S/GLUTINE 250G</t>
         </is>
       </c>
     </row>

</xml_diff>